<commit_message>
Expand test set data and address some conditions with NULL data
The added sample data has some NULLs in the input that the tool should handle.  Some fixes address these, but not all yet.

Major fixups include preserving dtypes for columns as we winsorize data, and setting numeric_only to False in the quantile function so that we can deal with Pint quantities without triggering an error message for NA values.  (Both in base_providers.py)

Added some try wrappers in template.py to make it easier to debug when errors are thrown.

Correct some uncaught errors in how null values are processed in interfaces.py

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9EE4DB-B4EB-8245-B8C3-41D4F4393279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E1DDAA-2491-1347-908A-657C8C561B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46560" yWindow="10080" windowWidth="50500" windowHeight="38360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19540" yWindow="29460" windowWidth="81680" windowHeight="20280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -35,8 +35,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Michael Tiemann</author>
+  </authors>
+  <commentList>
+    <comment ref="L13" authorId="0" shapeId="0" xr:uid="{448510DF-B4CA-A74B-8DA4-8A66766A6D07}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>90% sourced from nuclear so 10% ambition imagines 100% carbon-neutral power sourcing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{CA21DE94-42A9-2242-B39E-4A74054C3A31}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yes: S1+S3</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="323">
   <si>
     <t>Data field</t>
   </si>
@@ -1105,6 +1181,33 @@
   <si>
     <t>S1+S2</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Gt CO2</t>
+  </si>
+  <si>
+    <t>tons CO2/MWh</t>
+  </si>
+  <si>
+    <t>GWh</t>
+  </si>
+  <si>
+    <t>S1+S2+S3</t>
+  </si>
+  <si>
+    <t>t CO2/Fe_ton</t>
+  </si>
+  <si>
+    <t>S1+S3</t>
+  </si>
+  <si>
+    <t>t CO2/MWh</t>
+  </si>
+  <si>
+    <t>TWh</t>
+  </si>
+  <si>
+    <t>M Fe_ton</t>
+  </si>
 </sst>
 </file>
 
@@ -1113,7 +1216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1261,8 +1364,26 @@
       <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1335,6 +1456,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1385,7 +1512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1532,6 +1659,13 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2441,6 +2575,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2770,9 +2908,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AE2" sqref="AE2:AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -2784,11 +2924,13 @@
     <col min="14" max="14" width="25.83203125" customWidth="1"/>
     <col min="15" max="15" width="25.83203125" style="61" customWidth="1"/>
     <col min="16" max="16" width="22.1640625" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="2"/>
-    <col min="23" max="23" width="16.5" style="36"/>
-    <col min="24" max="29" width="16.5" style="2"/>
-    <col min="30" max="30" width="16.5" style="36"/>
-    <col min="31" max="44" width="16.5" style="2"/>
+    <col min="17" max="21" width="16.5" customWidth="1"/>
+    <col min="22" max="22" width="16.5" style="2" customWidth="1"/>
+    <col min="23" max="23" width="16.5" style="36" customWidth="1"/>
+    <col min="24" max="29" width="16.5" style="2" customWidth="1"/>
+    <col min="30" max="30" width="16.5" style="36" customWidth="1"/>
+    <col min="31" max="37" width="16.5" style="2" customWidth="1"/>
+    <col min="38" max="44" width="16.5" style="2"/>
     <col min="45" max="49" width="16.83203125" style="2" customWidth="1"/>
     <col min="50" max="16384" width="16.5" style="2"/>
   </cols>
@@ -2995,80 +3137,105 @@
         <v>143</v>
       </c>
       <c r="P2" s="61" t="s">
-        <v>144</v>
+        <v>316</v>
       </c>
       <c r="Q2" s="53">
-        <v>20.8302862</v>
+        <v>70457000</v>
       </c>
       <c r="R2" s="53">
-        <v>10.483392151</v>
+        <v>59804000</v>
       </c>
       <c r="S2" s="53">
-        <v>11.235889897</v>
+        <v>50291000</v>
       </c>
       <c r="T2" s="53">
-        <v>11.994886356</v>
+        <v>45611000</v>
       </c>
       <c r="U2" s="53">
-        <v>11.423701292000001</v>
+        <v>42961000</v>
       </c>
       <c r="V2" s="53"/>
       <c r="W2" s="53"/>
       <c r="X2" s="53">
-        <v>20.8302862</v>
+        <v>306000</v>
       </c>
       <c r="Y2" s="53">
-        <v>10.483392151</v>
+        <v>220000</v>
       </c>
       <c r="Z2" s="53">
-        <v>11.235889897</v>
+        <v>314000</v>
       </c>
       <c r="AA2" s="53">
-        <v>11.994886356</v>
+        <v>324000</v>
       </c>
       <c r="AB2" s="53">
-        <v>11.423701292000001</v>
+        <v>254000</v>
       </c>
       <c r="AC2" s="53"/>
       <c r="AD2" s="53"/>
       <c r="AE2" s="69">
-        <v>20.8302862</v>
+        <f t="shared" ref="AE2:AE4" si="0">IF(ISBLANK(Q2),IF(ISBLANK(X2),"",X2),Q2+X2)</f>
+        <v>70763000</v>
       </c>
       <c r="AF2" s="69">
-        <v>10.483392151</v>
+        <f t="shared" ref="AF2:AF4" si="1">IF(ISBLANK(R2),IF(ISBLANK(Y2),"",Y2),R2+Y2)</f>
+        <v>60024000</v>
       </c>
       <c r="AG2" s="69">
-        <v>11.235889897</v>
+        <f t="shared" ref="AG2:AG4" si="2">IF(ISBLANK(S2),IF(ISBLANK(Z2),"",Z2),S2+Z2)</f>
+        <v>50605000</v>
       </c>
       <c r="AH2" s="69">
-        <v>11.994886356</v>
+        <f t="shared" ref="AH2:AH4" si="3">IF(ISBLANK(T2),IF(ISBLANK(AA2),"",AA2),T2+AA2)</f>
+        <v>45935000</v>
       </c>
       <c r="AI2" s="69">
-        <v>11.423701292000001</v>
-      </c>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="53"/>
+        <f t="shared" ref="AI2:AI4" si="4">IF(ISBLANK(U2),IF(ISBLANK(AB2),"",AB2),U2+AB2)</f>
+        <v>43215000</v>
+      </c>
+      <c r="AJ2" s="69" t="str">
+        <f t="shared" ref="AJ2:AJ4" si="5">IF(ISBLANK(V2),IF(ISBLANK(AC2),"",AC2),V2+AC2)</f>
+        <v/>
+      </c>
+      <c r="AK2" s="69" t="str">
+        <f t="shared" ref="AK2:AK4" si="6">IF(ISBLANK(W2),IF(ISBLANK(AD2),"",AD2),W2+AD2)</f>
+        <v/>
+      </c>
+      <c r="AL2" s="53">
+        <v>5864000</v>
+      </c>
+      <c r="AM2" s="53">
+        <f>13871000+800</f>
+        <v>13871800</v>
+      </c>
+      <c r="AN2" s="53">
+        <f>10070000+1100</f>
+        <v>10071100</v>
+      </c>
+      <c r="AO2" s="53">
+        <f>9972000+1200</f>
+        <v>9973200</v>
+      </c>
+      <c r="AP2" s="53">
+        <f>7269000+200</f>
+        <v>7269200</v>
+      </c>
       <c r="AQ2" s="53"/>
       <c r="AR2" s="53"/>
       <c r="AS2" s="61">
-        <v>23.95571305</v>
+        <v>104312</v>
       </c>
       <c r="AT2" s="61">
-        <v>12.966211038000001</v>
+        <v>31536</v>
       </c>
       <c r="AU2" s="61">
-        <v>15.107020127</v>
+        <v>83985.94</v>
       </c>
       <c r="AV2" s="61">
-        <v>16.936182994999999</v>
+        <v>759043.55</v>
       </c>
       <c r="AW2" s="61">
-        <v>17.024825235582298</v>
+        <v>75271.521999999997</v>
       </c>
       <c r="AX2" s="53"/>
       <c r="AY2" s="53"/>
@@ -3126,37 +3293,72 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="AE3" s="69">
-        <v>8.0287915250000008</v>
-      </c>
-      <c r="AF3" s="69">
-        <v>6.5660701670000003</v>
-      </c>
-      <c r="AG3" s="69">
-        <v>6.511972042</v>
+      <c r="T3" s="2">
+        <v>1210847</v>
+      </c>
+      <c r="U3" s="2">
+        <v>297479</v>
+      </c>
+      <c r="V3" s="2">
+        <v>2782868</v>
+      </c>
+      <c r="W3" s="36">
+        <v>2720482</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>5249805</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>3221290</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>2027896</v>
+      </c>
+      <c r="AD3" s="36">
+        <v>1370397</v>
+      </c>
+      <c r="AE3" s="69" t="str">
+        <f>IF(ISBLANK(Q3),IF(ISBLANK(X3),"",X3),Q3+X3)</f>
+        <v/>
+      </c>
+      <c r="AF3" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="AG3" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="AH3" s="69">
-        <v>4.3830481260000003</v>
+        <f t="shared" si="3"/>
+        <v>6460652</v>
       </c>
       <c r="AI3" s="69">
-        <v>4.2416594769999998</v>
-      </c>
-      <c r="AS3" s="61">
-        <v>12.04283116</v>
-      </c>
-      <c r="AT3" s="61">
-        <v>10.83695122</v>
-      </c>
-      <c r="AU3" s="61">
-        <v>10.50623193</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>3518769</v>
+      </c>
+      <c r="AJ3" s="69">
+        <f t="shared" si="5"/>
+        <v>4810764</v>
+      </c>
+      <c r="AK3" s="69">
+        <f t="shared" si="6"/>
+        <v>4090879</v>
+      </c>
+      <c r="AS3" s="61"/>
+      <c r="AT3" s="61"/>
+      <c r="AU3" s="61"/>
       <c r="AV3" s="61">
-        <v>8.4213020440000008</v>
+        <v>3441242</v>
       </c>
       <c r="AW3" s="61">
-        <v>8.4483908050000007</v>
+        <v>2540911</v>
+      </c>
+      <c r="AX3" s="2">
+        <v>5081479</v>
+      </c>
+      <c r="AY3" s="2">
+        <v>4870600</v>
       </c>
     </row>
     <row r="4" spans="1:52">
@@ -3210,38 +3412,65 @@
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="AE4" s="69">
-        <v>12.265532917</v>
-      </c>
-      <c r="AF4" s="69">
-        <v>13.800613625</v>
+      <c r="S4" s="2">
+        <v>17598424</v>
+      </c>
+      <c r="T4" s="2">
+        <v>14280935</v>
+      </c>
+      <c r="U4" s="2">
+        <v>12624301</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>5234</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>5236</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>4187</v>
+      </c>
+      <c r="AE4" s="69" t="str">
+        <f t="shared" ref="AE4" si="7">IF(ISBLANK(Q4),IF(ISBLANK(X4),"",X4),Q4+X4)</f>
+        <v/>
+      </c>
+      <c r="AF4" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
       <c r="AG4" s="69">
-        <v>14.989750726</v>
+        <f t="shared" si="2"/>
+        <v>17603658</v>
       </c>
       <c r="AH4" s="69">
-        <v>11.081667744000001</v>
+        <f t="shared" si="3"/>
+        <v>14286171</v>
       </c>
       <c r="AI4" s="69">
-        <v>10.577955574000001</v>
-      </c>
-      <c r="AS4" s="61">
-        <v>20.588826059999999</v>
-      </c>
-      <c r="AT4" s="61">
-        <v>22.836069439999999</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>12628488</v>
+      </c>
+      <c r="AJ4" s="69" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AK4" s="69" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AS4" s="61"/>
+      <c r="AT4" s="61"/>
       <c r="AU4" s="61">
-        <v>26.539897759999999</v>
+        <f>12112825+9730905+35784+200052+3905+1602768</f>
+        <v>23686239</v>
       </c>
       <c r="AV4" s="61">
-        <v>25.164691730000001</v>
+        <f>8643022+11070790+4958+227622+6349+2895846</f>
+        <v>22848587</v>
       </c>
       <c r="AW4" s="61">
-        <v>23.25695385017389</v>
+        <f>7020084+10451667+743+242130+10786+4871874</f>
+        <v>22597284</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -3288,16 +3517,16 @@
         <v>28933000000</v>
       </c>
       <c r="O5" s="61" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="P5" s="61" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="78"/>
       <c r="AE5" s="69">
         <v>29.875229310000002</v>
       </c>
@@ -3378,40 +3607,70 @@
       <c r="P6" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="Q6" s="76">
+        <v>90989994</v>
+      </c>
+      <c r="R6" s="78">
+        <v>72813962</v>
+      </c>
+      <c r="S6" s="78">
+        <v>69614180</v>
+      </c>
+      <c r="T6" s="78">
+        <v>59439006</v>
+      </c>
+      <c r="U6" s="78">
+        <v>44902836</v>
+      </c>
+      <c r="X6" s="76">
+        <v>3006186</v>
+      </c>
+      <c r="Y6" s="78">
+        <v>251231</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="78">
+        <v>8608544</v>
+      </c>
+      <c r="AB6" s="78">
+        <v>6440084</v>
+      </c>
       <c r="AE6" s="69">
-        <v>87.723312172000007</v>
+        <f t="shared" ref="AE6:AE8" si="8">IF(ISBLANK(Q6),IF(ISBLANK(X6),"",X6),Q6+X6)</f>
+        <v>93996180</v>
       </c>
       <c r="AF6" s="69">
-        <v>66.96612196400001</v>
+        <f t="shared" ref="AF6:AF8" si="9">IF(ISBLANK(R6),IF(ISBLANK(Y6),"",Y6),R6+Y6)</f>
+        <v>73065193</v>
       </c>
       <c r="AG6" s="69">
-        <v>66.137236960999999</v>
+        <f t="shared" ref="AG6:AG8" si="10">IF(ISBLANK(S6),IF(ISBLANK(Z6),"",Z6),S6+Z6)</f>
+        <v>69614180</v>
       </c>
       <c r="AH6" s="69">
-        <v>60.045813868000003</v>
+        <f t="shared" ref="AH6:AH8" si="11">IF(ISBLANK(T6),IF(ISBLANK(AA6),"",AA6),T6+AA6)</f>
+        <v>68047550</v>
       </c>
       <c r="AI6" s="69">
-        <v>56.905072285999999</v>
-      </c>
-      <c r="AS6" s="61">
-        <v>133.581626382</v>
-      </c>
-      <c r="AT6" s="61">
-        <v>104.24559965500001</v>
-      </c>
-      <c r="AU6" s="61">
-        <v>103.529138004</v>
-      </c>
-      <c r="AV6" s="61">
-        <v>94.462945003999991</v>
-      </c>
-      <c r="AW6" s="61">
-        <v>90.005723929977037</v>
+        <f t="shared" ref="AI6:AI8" si="12">IF(ISBLANK(U6),IF(ISBLANK(AB6),"",AB6),U6+AB6)</f>
+        <v>51342920</v>
+      </c>
+      <c r="AS6" s="76">
+        <v>137346204</v>
+      </c>
+      <c r="AT6" s="76">
+        <v>108631253</v>
+      </c>
+      <c r="AU6" s="76">
+        <v>104375491</v>
+      </c>
+      <c r="AV6" s="76">
+        <v>106382813</v>
+      </c>
+      <c r="AW6" s="76">
+        <v>94529102</v>
       </c>
     </row>
     <row r="7" spans="1:52">
@@ -3461,42 +3720,67 @@
         <v>143</v>
       </c>
       <c r="P7" s="61" t="s">
-        <v>144</v>
+        <v>316</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="AE7" s="69">
-        <v>2.0475329E-2</v>
-      </c>
-      <c r="AF7" s="69">
-        <v>4.6049666000000003E-2</v>
+      <c r="S7" s="2">
+        <v>1363231</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1934393</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1416448</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>381533</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>231192</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>297283</v>
+      </c>
+      <c r="AE7" s="69" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AF7" s="69" t="str">
+        <f t="shared" si="9"/>
+        <v/>
       </c>
       <c r="AG7" s="69">
-        <v>2.6386597000000001E-2</v>
+        <f t="shared" si="10"/>
+        <v>1744764</v>
       </c>
       <c r="AH7" s="69">
-        <v>2.5963092E-2</v>
+        <f t="shared" si="11"/>
+        <v>2165585</v>
       </c>
       <c r="AI7" s="69">
-        <v>2.306012E-2</v>
-      </c>
-      <c r="AS7" s="61">
-        <v>1.210734</v>
-      </c>
-      <c r="AT7" s="61">
-        <v>1.314970829</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>1713731</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>21590220</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>19892852</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>24528246</v>
+      </c>
+      <c r="AS7" s="61"/>
+      <c r="AT7" s="61"/>
       <c r="AU7" s="61">
-        <v>1.190620357</v>
+        <v>20057</v>
       </c>
       <c r="AV7" s="61">
-        <v>1.212120114</v>
+        <v>20960</v>
       </c>
       <c r="AW7" s="61">
-        <v>1.120229162933025</v>
+        <v>22142</v>
       </c>
     </row>
     <row r="8" spans="1:52">
@@ -3543,345 +3827,955 @@
         <v>7558457000</v>
       </c>
       <c r="O8" s="61" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="P8" s="61" t="s">
         <v>144</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="AE8" s="69">
-        <v>2.7086220929999998</v>
-      </c>
-      <c r="AF8" s="69">
-        <v>3.5576825919999999</v>
+      <c r="S8" s="78">
+        <v>4063143</v>
+      </c>
+      <c r="T8" s="78">
+        <v>3963128</v>
+      </c>
+      <c r="U8" s="78">
+        <v>4036591</v>
+      </c>
+      <c r="Z8" s="78">
+        <v>1300042</v>
+      </c>
+      <c r="AA8" s="78">
+        <v>1219954</v>
+      </c>
+      <c r="AB8" s="78">
+        <v>1001588</v>
+      </c>
+      <c r="AE8" s="69" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="AF8" s="69" t="str">
+        <f t="shared" si="9"/>
+        <v/>
       </c>
       <c r="AG8" s="69">
-        <v>3.6777294390000002</v>
+        <f t="shared" si="10"/>
+        <v>5363185</v>
       </c>
       <c r="AH8" s="69">
-        <v>2.8609599440000002</v>
+        <f t="shared" si="11"/>
+        <v>5183082</v>
       </c>
       <c r="AI8" s="69">
-        <v>2.7420756740000001</v>
-      </c>
-      <c r="AS8" s="61">
-        <v>5.5958280800000004</v>
-      </c>
-      <c r="AT8" s="61">
-        <v>6.4723439799999998</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>5038179</v>
+      </c>
+      <c r="AS8" s="61"/>
+      <c r="AT8" s="61"/>
       <c r="AU8" s="61">
-        <v>6.6480604999999997</v>
+        <v>7067031.0930000003</v>
       </c>
       <c r="AV8" s="61">
-        <v>6.0098643799999998</v>
-      </c>
-      <c r="AW8" s="61">
-        <v>6.0371996609999998</v>
+        <v>7195251.4899999993</v>
+      </c>
+      <c r="AW8" s="76">
+        <v>7324609</v>
       </c>
     </row>
     <row r="9" spans="1:52">
-      <c r="A9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="61"/>
-      <c r="P9" s="61"/>
+      <c r="A9" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J9" s="61">
+        <v>1687208892</v>
+      </c>
+      <c r="K9" s="61">
+        <v>2380200000</v>
+      </c>
+      <c r="L9" s="61">
+        <v>2210808892</v>
+      </c>
+      <c r="M9" s="61">
+        <v>2237808892</v>
+      </c>
+      <c r="N9" s="61">
+        <v>3187800000</v>
+      </c>
+      <c r="O9" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P9" s="61" t="s">
+        <v>322</v>
+      </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="AE9" s="69"/>
-      <c r="AF9" s="69"/>
-      <c r="AG9" s="69"/>
-      <c r="AH9" s="69"/>
-      <c r="AI9" s="69"/>
-      <c r="AS9" s="61"/>
-      <c r="AT9" s="61"/>
-      <c r="AU9" s="61"/>
-      <c r="AV9" s="61"/>
-      <c r="AW9" s="61"/>
+      <c r="AE9" s="69">
+        <v>0.29805500000000001</v>
+      </c>
+      <c r="AF9" s="69">
+        <v>0.29805500000000001</v>
+      </c>
+      <c r="AG9" s="69">
+        <v>0.29805500000000001</v>
+      </c>
+      <c r="AH9" s="69">
+        <v>0.29805500000000001</v>
+      </c>
+      <c r="AI9" s="69">
+        <v>0.29283215098729842</v>
+      </c>
+      <c r="AS9" s="61">
+        <v>0.13883100000000001</v>
+      </c>
+      <c r="AT9" s="61">
+        <v>0.13883100000000001</v>
+      </c>
+      <c r="AU9" s="61">
+        <v>0.13883100000000001</v>
+      </c>
+      <c r="AV9" s="61">
+        <v>0.13883100000000001</v>
+      </c>
+      <c r="AW9" s="61">
+        <v>0.14094485815987501</v>
+      </c>
     </row>
     <row r="10" spans="1:52">
-      <c r="A10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="61"/>
-      <c r="P10" s="61"/>
+      <c r="A10" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J10" s="61">
+        <v>16647000000</v>
+      </c>
+      <c r="K10" s="61">
+        <v>6845000000</v>
+      </c>
+      <c r="L10" s="61">
+        <v>28458000000</v>
+      </c>
+      <c r="M10" s="61">
+        <v>28598000000</v>
+      </c>
+      <c r="N10" s="61">
+        <v>26837000000</v>
+      </c>
+      <c r="O10" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P10" s="61" t="s">
+        <v>321</v>
+      </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
-      <c r="AH10" s="69"/>
-      <c r="AI10" s="69"/>
-      <c r="AS10" s="61"/>
-      <c r="AT10" s="61"/>
-      <c r="AU10" s="61"/>
-      <c r="AV10" s="61"/>
-      <c r="AW10" s="61"/>
+      <c r="AE10" s="69">
+        <v>11.183374199999999</v>
+      </c>
+      <c r="AF10" s="69">
+        <v>12.381008120000001</v>
+      </c>
+      <c r="AG10" s="69">
+        <v>12.27761477</v>
+      </c>
+      <c r="AH10" s="69">
+        <v>12.512963060000001</v>
+      </c>
+      <c r="AI10" s="69">
+        <v>11.91710767</v>
+      </c>
+      <c r="AS10" s="61">
+        <v>18.979711429999998</v>
+      </c>
+      <c r="AT10" s="61">
+        <v>20.31118927</v>
+      </c>
+      <c r="AU10" s="61">
+        <v>20.50728269</v>
+      </c>
+      <c r="AV10" s="61">
+        <v>22.28763412</v>
+      </c>
+      <c r="AW10" s="61">
+        <v>22.324507709999999</v>
+      </c>
+      <c r="AX10" s="79"/>
     </row>
     <row r="11" spans="1:52">
-      <c r="A11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
+      <c r="A11" s="61" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J11" s="61">
+        <v>2200000000</v>
+      </c>
+      <c r="K11" s="61">
+        <v>5829002000</v>
+      </c>
       <c r="L11" s="61"/>
       <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="68"/>
+      <c r="N11" s="61">
+        <v>3758771000</v>
+      </c>
+      <c r="O11" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="P11" s="68" t="s">
+        <v>183</v>
+      </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="AE11" s="69"/>
-      <c r="AF11" s="69"/>
-      <c r="AG11" s="69"/>
-      <c r="AH11" s="69"/>
-      <c r="AI11" s="69"/>
-      <c r="AS11" s="61"/>
-      <c r="AT11" s="61"/>
-      <c r="AU11" s="61"/>
-      <c r="AV11" s="61"/>
-      <c r="AW11" s="61"/>
+      <c r="T11" s="78">
+        <v>1048006</v>
+      </c>
+      <c r="U11" s="78">
+        <v>1106156</v>
+      </c>
+      <c r="V11" s="80">
+        <v>1117753</v>
+      </c>
+      <c r="AA11" s="80">
+        <v>1500431</v>
+      </c>
+      <c r="AB11" s="80">
+        <v>1466830</v>
+      </c>
+      <c r="AC11" s="80">
+        <v>1436765</v>
+      </c>
+      <c r="AE11" s="69" t="str">
+        <f t="shared" ref="AE11:AK11" si="13">IF(ISBLANK(Q11),IF(ISBLANK(X11),"",X11),Q11+X11)</f>
+        <v/>
+      </c>
+      <c r="AF11" s="69" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AG11" s="69" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AH11" s="69">
+        <f t="shared" si="13"/>
+        <v>2548437</v>
+      </c>
+      <c r="AI11" s="69">
+        <f t="shared" si="13"/>
+        <v>2572986</v>
+      </c>
+      <c r="AJ11" s="69">
+        <f t="shared" si="13"/>
+        <v>2554518</v>
+      </c>
+      <c r="AK11" s="69" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AS11" s="61">
+        <v>5301216</v>
+      </c>
+      <c r="AT11" s="61">
+        <v>5301216</v>
+      </c>
+      <c r="AU11" s="61">
+        <v>5301216</v>
+      </c>
+      <c r="AV11" s="61">
+        <f>2548437/0.481</f>
+        <v>5298205.8212058218</v>
+      </c>
+      <c r="AW11" s="61">
+        <f>2572986/0.464</f>
+        <v>5545228.4482758613</v>
+      </c>
+      <c r="AX11" s="79">
+        <f>2554518/0.451</f>
+        <v>5664119.7339246115</v>
+      </c>
     </row>
     <row r="12" spans="1:52">
-      <c r="A12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="H12" s="61"/>
+      <c r="A12" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="5">
+        <v>44561</v>
+      </c>
       <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
+      <c r="K12" s="61">
+        <v>1639605000</v>
+      </c>
       <c r="L12" s="61"/>
       <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="P12" s="61"/>
+      <c r="N12" s="61">
+        <v>7476298000</v>
+      </c>
+      <c r="O12" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="P12" s="61" t="s">
+        <v>321</v>
+      </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
-      <c r="AE12" s="69"/>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="69"/>
-      <c r="AH12" s="69"/>
-      <c r="AI12" s="69"/>
-      <c r="AS12" s="61"/>
-      <c r="AT12" s="61"/>
-      <c r="AU12" s="61"/>
-      <c r="AV12" s="61"/>
-      <c r="AW12" s="61"/>
+      <c r="AE12" s="69">
+        <v>9.9820912380000006</v>
+      </c>
+      <c r="AF12" s="69">
+        <v>8.7791840319999999</v>
+      </c>
+      <c r="AG12" s="69">
+        <v>9.3084717799999996</v>
+      </c>
+      <c r="AH12" s="69">
+        <v>8.448013328</v>
+      </c>
+      <c r="AS12" s="61">
+        <v>14.52558153</v>
+      </c>
+      <c r="AT12" s="61">
+        <v>12.52148775</v>
+      </c>
+      <c r="AU12" s="61">
+        <v>13.19964667</v>
+      </c>
+      <c r="AV12" s="61">
+        <v>13.86123875</v>
+      </c>
+      <c r="AW12" s="61">
+        <v>12.81041680835213</v>
+      </c>
+      <c r="AX12" s="79"/>
     </row>
     <row r="13" spans="1:52">
-      <c r="A13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
+      <c r="A13" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J13" s="61">
+        <v>24000000000</v>
+      </c>
+      <c r="K13" s="61">
+        <v>12574000000</v>
+      </c>
+      <c r="L13" s="61">
+        <v>42992000000</v>
+      </c>
+      <c r="M13" s="61">
+        <v>43973000000</v>
+      </c>
+      <c r="N13" s="61">
+        <v>58079000000</v>
+      </c>
+      <c r="O13" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="P13" s="68" t="s">
+        <v>321</v>
+      </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-      <c r="AE13" s="69"/>
-      <c r="AF13" s="69"/>
-      <c r="AG13" s="69"/>
-      <c r="AH13" s="69"/>
-      <c r="AI13" s="69"/>
-      <c r="AS13" s="61"/>
-      <c r="AT13" s="61"/>
-      <c r="AU13" s="61"/>
-      <c r="AV13" s="61"/>
-      <c r="AW13" s="61"/>
+      <c r="AE13" s="69">
+        <v>1.325786621</v>
+      </c>
+      <c r="AF13" s="69">
+        <v>1.323738978</v>
+      </c>
+      <c r="AG13" s="69">
+        <v>1.2685339369999999</v>
+      </c>
+      <c r="AH13" s="69">
+        <v>1.202690405</v>
+      </c>
+      <c r="AI13" s="69">
+        <v>1.145419433</v>
+      </c>
+      <c r="AS13" s="61">
+        <v>5.3109194439999996</v>
+      </c>
+      <c r="AT13" s="61">
+        <v>5.7325927349999999</v>
+      </c>
+      <c r="AU13" s="61">
+        <v>6.0319896030000004</v>
+      </c>
+      <c r="AV13" s="61">
+        <v>6.5057034040000001</v>
+      </c>
+      <c r="AW13" s="61">
+        <v>6.0125053568358231</v>
+      </c>
+      <c r="AX13" s="79"/>
     </row>
     <row r="14" spans="1:52">
-      <c r="A14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="68"/>
-      <c r="P14" s="68"/>
+      <c r="A14" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J14" s="61">
+        <v>20500000000</v>
+      </c>
+      <c r="K14" s="61">
+        <v>12669000000</v>
+      </c>
+      <c r="L14" s="61">
+        <v>36342000000</v>
+      </c>
+      <c r="M14" s="61">
+        <v>36435000000</v>
+      </c>
+      <c r="N14" s="61">
+        <v>42268000000</v>
+      </c>
+      <c r="O14" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="P14" s="68" t="s">
+        <v>321</v>
+      </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="AE14" s="69"/>
-      <c r="AF14" s="69"/>
-      <c r="AG14" s="69"/>
-      <c r="AH14" s="69"/>
-      <c r="AI14" s="69"/>
-      <c r="AS14" s="61"/>
-      <c r="AT14" s="61"/>
-      <c r="AU14" s="61"/>
-      <c r="AV14" s="61"/>
-      <c r="AW14" s="61"/>
+      <c r="AE14" s="69">
+        <v>26.796145450000001</v>
+      </c>
+      <c r="AF14" s="69">
+        <v>27.947696990000001</v>
+      </c>
+      <c r="AG14" s="69">
+        <v>29.95633261</v>
+      </c>
+      <c r="AH14" s="69">
+        <v>27.00027425</v>
+      </c>
+      <c r="AI14" s="69">
+        <v>26.48364437</v>
+      </c>
+      <c r="AS14" s="61">
+        <v>39.339109710000002</v>
+      </c>
+      <c r="AT14" s="61">
+        <v>39.490179230000003</v>
+      </c>
+      <c r="AU14" s="61">
+        <v>40.7944417</v>
+      </c>
+      <c r="AV14" s="61">
+        <v>40.197309990000001</v>
+      </c>
+      <c r="AW14" s="61">
+        <v>37.14994776685721</v>
+      </c>
+      <c r="AX14" s="79"/>
     </row>
     <row r="15" spans="1:52">
-      <c r="A15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="61"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="68"/>
-      <c r="P15" s="68"/>
+      <c r="A15" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J15" s="61">
+        <v>68000000000</v>
+      </c>
+      <c r="K15" s="61">
+        <v>14401000000</v>
+      </c>
+      <c r="L15" s="61">
+        <v>96863000000</v>
+      </c>
+      <c r="M15" s="61">
+        <v>96998000000</v>
+      </c>
+      <c r="N15" s="61">
+        <v>103823000000</v>
+      </c>
+      <c r="O15" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="P15" s="68" t="s">
+        <v>321</v>
+      </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="AE15" s="69"/>
-      <c r="AF15" s="69"/>
-      <c r="AG15" s="69"/>
-      <c r="AH15" s="69"/>
-      <c r="AI15" s="69"/>
-      <c r="AS15" s="61"/>
-      <c r="AT15" s="61"/>
-      <c r="AU15" s="61"/>
-      <c r="AV15" s="61"/>
-      <c r="AW15" s="61"/>
+      <c r="T15" s="2">
+        <v>31.75</v>
+      </c>
+      <c r="U15" s="2">
+        <v>32.957000000000001</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>8.26</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>4.5759999999999996</v>
+      </c>
+      <c r="AE15" s="69">
+        <v>43.346773548000002</v>
+      </c>
+      <c r="AF15" s="69">
+        <v>36.869361507000001</v>
+      </c>
+      <c r="AG15" s="69">
+        <v>35.455656216999998</v>
+      </c>
+      <c r="AH15" s="69">
+        <v>31.432803556</v>
+      </c>
+      <c r="AI15" s="69">
+        <v>30.418842145999999</v>
+      </c>
+      <c r="AO15" s="2">
+        <f>(0.31+0.142+0.011)*26.6</f>
+        <v>12.315799999999999</v>
+      </c>
+      <c r="AS15" s="61">
+        <v>106.43053159</v>
+      </c>
+      <c r="AT15" s="61">
+        <v>99.522718589999997</v>
+      </c>
+      <c r="AU15" s="61">
+        <v>99.984302179999986</v>
+      </c>
+      <c r="AV15" s="61">
+        <v>102.19514168000001</v>
+      </c>
+      <c r="AW15" s="61">
+        <v>103.314188346027</v>
+      </c>
+      <c r="AX15" s="79"/>
     </row>
     <row r="16" spans="1:52">
-      <c r="A16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="68"/>
-      <c r="P16" s="68"/>
+      <c r="A16" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J16" s="61">
+        <v>58688204289</v>
+      </c>
+      <c r="K16" s="61">
+        <v>25079000000</v>
+      </c>
+      <c r="L16" s="61">
+        <v>121439204289</v>
+      </c>
+      <c r="M16" s="61">
+        <v>121750204289</v>
+      </c>
+      <c r="N16" s="61">
+        <v>158838000000</v>
+      </c>
+      <c r="O16" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="P16" s="68" t="s">
+        <v>321</v>
+      </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
-      <c r="AE16" s="69"/>
-      <c r="AF16" s="69"/>
-      <c r="AG16" s="69"/>
-      <c r="AH16" s="69"/>
-      <c r="AI16" s="69"/>
-      <c r="AS16" s="61"/>
-      <c r="AT16" s="61"/>
-      <c r="AU16" s="61"/>
-      <c r="AV16" s="61"/>
-      <c r="AW16" s="61"/>
-    </row>
-    <row r="17" spans="1:49">
-      <c r="A17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="68"/>
-      <c r="P17" s="68"/>
+      <c r="AE16" s="69">
+        <v>94.923459879999996</v>
+      </c>
+      <c r="AF16" s="69">
+        <v>93.530450478000006</v>
+      </c>
+      <c r="AG16" s="69">
+        <v>95.012237693000003</v>
+      </c>
+      <c r="AH16" s="69">
+        <v>83.595723118999999</v>
+      </c>
+      <c r="AI16" s="69">
+        <v>82.018839239000002</v>
+      </c>
+      <c r="AS16" s="61">
+        <v>221.77898501999999</v>
+      </c>
+      <c r="AT16" s="61">
+        <v>222.41056646000001</v>
+      </c>
+      <c r="AU16" s="61">
+        <v>225.51497273000001</v>
+      </c>
+      <c r="AV16" s="61">
+        <v>216.60189564999999</v>
+      </c>
+      <c r="AW16" s="61">
+        <v>217.79186281500009</v>
+      </c>
+      <c r="AX16" s="79"/>
+    </row>
+    <row r="17" spans="1:50">
+      <c r="A17" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J17" s="61">
+        <v>18800000000</v>
+      </c>
+      <c r="K17" s="61">
+        <v>10878673000</v>
+      </c>
+      <c r="L17" s="61">
+        <v>37434228000</v>
+      </c>
+      <c r="M17" s="61">
+        <v>37859950000</v>
+      </c>
+      <c r="N17" s="61">
+        <v>51723912000</v>
+      </c>
+      <c r="O17" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="P17" s="68" t="s">
+        <v>321</v>
+      </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-      <c r="AE17" s="69"/>
-      <c r="AF17" s="69"/>
-      <c r="AG17" s="69"/>
-      <c r="AH17" s="69"/>
-      <c r="AI17" s="69"/>
-      <c r="AS17" s="61"/>
-      <c r="AT17" s="61"/>
-      <c r="AU17" s="61"/>
-      <c r="AV17" s="61"/>
-      <c r="AW17" s="61"/>
-    </row>
-    <row r="18" spans="1:49">
-      <c r="A18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="68"/>
-      <c r="P18" s="68"/>
+      <c r="AE17" s="69">
+        <v>32.516193991999998</v>
+      </c>
+      <c r="AF17" s="69">
+        <v>31.450986952000001</v>
+      </c>
+      <c r="AG17" s="69">
+        <v>34.631975513</v>
+      </c>
+      <c r="AH17" s="69">
+        <v>33.246229124999999</v>
+      </c>
+      <c r="AS17" s="61">
+        <v>102.999524264</v>
+      </c>
+      <c r="AT17" s="61">
+        <v>98.242043473999999</v>
+      </c>
+      <c r="AU17" s="61">
+        <v>105.741655513</v>
+      </c>
+      <c r="AV17" s="61">
+        <v>109.743440224</v>
+      </c>
+      <c r="AW17" s="61">
+        <v>107.355350022618</v>
+      </c>
+      <c r="AX17" s="79"/>
+    </row>
+    <row r="18" spans="1:50">
+      <c r="A18" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J18" s="61">
+        <v>13410149293</v>
+      </c>
+      <c r="K18" s="61">
+        <v>5147800000</v>
+      </c>
+      <c r="L18" s="61">
+        <v>22133649293</v>
+      </c>
+      <c r="M18" s="61">
+        <v>22156849293</v>
+      </c>
+      <c r="N18" s="61">
+        <v>25975900000</v>
+      </c>
+      <c r="O18" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="P18" s="68" t="s">
+        <v>321</v>
+      </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
-      <c r="AE18" s="69"/>
-      <c r="AF18" s="69"/>
-      <c r="AG18" s="69"/>
-      <c r="AH18" s="69"/>
-      <c r="AI18" s="69"/>
-      <c r="AS18" s="61"/>
-      <c r="AT18" s="61"/>
-      <c r="AU18" s="61"/>
-      <c r="AV18" s="61"/>
-      <c r="AW18" s="61"/>
-    </row>
-    <row r="19" spans="1:49">
+      <c r="AE18" s="69">
+        <v>35.122915438000007</v>
+      </c>
+      <c r="AF18" s="69">
+        <v>32.270565695999998</v>
+      </c>
+      <c r="AG18" s="69">
+        <v>28.483757178000001</v>
+      </c>
+      <c r="AH18" s="69">
+        <v>26.74941115</v>
+      </c>
+      <c r="AI18" s="69">
+        <v>35.013482494000002</v>
+      </c>
+      <c r="AS18" s="61">
+        <v>47.465894990000002</v>
+      </c>
+      <c r="AT18" s="61">
+        <v>47.22838256</v>
+      </c>
+      <c r="AU18" s="61">
+        <v>42.360400810000002</v>
+      </c>
+      <c r="AV18" s="61">
+        <v>41.417892389999999</v>
+      </c>
+      <c r="AW18" s="61">
+        <v>52.209390303404128</v>
+      </c>
+      <c r="AX18" s="79"/>
+    </row>
+    <row r="19" spans="1:50">
       <c r="A19" s="61"/>
       <c r="C19" s="61"/>
       <c r="D19" s="61"/>
@@ -3900,18 +4794,14 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="AE19" s="69"/>
-      <c r="AF19" s="69"/>
-      <c r="AG19" s="69"/>
-      <c r="AH19" s="69"/>
-      <c r="AI19" s="69"/>
       <c r="AS19" s="61"/>
       <c r="AT19" s="61"/>
       <c r="AU19" s="61"/>
       <c r="AV19" s="61"/>
       <c r="AW19" s="61"/>
-    </row>
-    <row r="20" spans="1:49">
+      <c r="AX19" s="79"/>
+    </row>
+    <row r="20" spans="1:50">
       <c r="A20" s="61"/>
       <c r="C20" s="61"/>
       <c r="D20" s="61"/>
@@ -3930,18 +4820,14 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
-      <c r="AE20" s="69"/>
-      <c r="AF20" s="69"/>
-      <c r="AG20" s="69"/>
-      <c r="AH20" s="69"/>
-      <c r="AI20" s="69"/>
       <c r="AS20" s="61"/>
       <c r="AT20" s="61"/>
       <c r="AU20" s="61"/>
       <c r="AV20" s="61"/>
       <c r="AW20" s="61"/>
-    </row>
-    <row r="21" spans="1:49">
+      <c r="AX20" s="79"/>
+    </row>
+    <row r="21" spans="1:50">
       <c r="A21" s="61"/>
       <c r="C21" s="61"/>
       <c r="D21" s="61"/>
@@ -3960,18 +4846,14 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
-      <c r="AE21" s="69"/>
-      <c r="AF21" s="69"/>
-      <c r="AG21" s="69"/>
-      <c r="AH21" s="69"/>
-      <c r="AI21" s="69"/>
       <c r="AS21" s="61"/>
       <c r="AT21" s="61"/>
       <c r="AU21" s="61"/>
       <c r="AV21" s="61"/>
       <c r="AW21" s="61"/>
-    </row>
-    <row r="22" spans="1:49">
+      <c r="AX21" s="79"/>
+    </row>
+    <row r="22" spans="1:50">
       <c r="A22" s="61"/>
       <c r="C22" s="61"/>
       <c r="D22" s="61"/>
@@ -3990,18 +4872,14 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
-      <c r="AE22" s="69"/>
-      <c r="AF22" s="69"/>
-      <c r="AG22" s="69"/>
-      <c r="AH22" s="69"/>
-      <c r="AI22" s="69"/>
       <c r="AS22" s="61"/>
       <c r="AT22" s="61"/>
       <c r="AU22" s="61"/>
       <c r="AV22" s="61"/>
       <c r="AW22" s="61"/>
-    </row>
-    <row r="23" spans="1:49">
+      <c r="AX22" s="76"/>
+    </row>
+    <row r="23" spans="1:50">
       <c r="A23" s="61"/>
       <c r="C23" s="61"/>
       <c r="D23" s="61"/>
@@ -4020,18 +4898,13 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="AE23" s="69"/>
-      <c r="AF23" s="69"/>
-      <c r="AG23" s="69"/>
-      <c r="AH23" s="69"/>
-      <c r="AI23" s="69"/>
       <c r="AS23" s="61"/>
       <c r="AT23" s="61"/>
       <c r="AU23" s="61"/>
       <c r="AV23" s="61"/>
       <c r="AW23" s="61"/>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" spans="1:50">
       <c r="A24" s="61"/>
       <c r="C24" s="61"/>
       <c r="D24" s="61"/>
@@ -4049,18 +4922,13 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="AE24" s="69"/>
-      <c r="AF24" s="69"/>
-      <c r="AG24" s="69"/>
-      <c r="AH24" s="69"/>
-      <c r="AI24" s="69"/>
       <c r="AS24" s="61"/>
       <c r="AT24" s="61"/>
       <c r="AU24" s="61"/>
       <c r="AV24" s="61"/>
       <c r="AW24" s="61"/>
     </row>
-    <row r="25" spans="1:49">
+    <row r="25" spans="1:50">
       <c r="A25" s="61"/>
       <c r="C25" s="61"/>
       <c r="D25" s="61"/>
@@ -4079,18 +4947,13 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-      <c r="AE25" s="69"/>
-      <c r="AF25" s="69"/>
-      <c r="AG25" s="69"/>
-      <c r="AH25" s="69"/>
-      <c r="AI25" s="69"/>
       <c r="AS25" s="61"/>
       <c r="AT25" s="61"/>
       <c r="AU25" s="61"/>
       <c r="AV25" s="61"/>
       <c r="AW25" s="61"/>
     </row>
-    <row r="26" spans="1:49">
+    <row r="26" spans="1:50">
       <c r="A26" s="61"/>
       <c r="C26" s="61"/>
       <c r="D26" s="61"/>
@@ -4109,18 +4972,13 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="AE26" s="69"/>
-      <c r="AF26" s="69"/>
-      <c r="AG26" s="69"/>
-      <c r="AH26" s="69"/>
-      <c r="AI26" s="69"/>
       <c r="AS26" s="61"/>
       <c r="AT26" s="61"/>
       <c r="AU26" s="61"/>
       <c r="AV26" s="61"/>
       <c r="AW26" s="61"/>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" spans="1:50">
       <c r="A27" s="61"/>
       <c r="C27" s="61"/>
       <c r="D27" s="61"/>
@@ -4138,18 +4996,13 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-      <c r="AE27" s="69"/>
-      <c r="AF27" s="69"/>
-      <c r="AG27" s="69"/>
-      <c r="AH27" s="69"/>
-      <c r="AI27" s="69"/>
       <c r="AS27" s="61"/>
       <c r="AT27" s="61"/>
       <c r="AU27" s="61"/>
       <c r="AV27" s="61"/>
       <c r="AW27" s="61"/>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" spans="1:50">
       <c r="A28" s="61"/>
       <c r="C28" s="61"/>
       <c r="D28" s="61"/>
@@ -4168,18 +5021,13 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
-      <c r="AE28" s="69"/>
-      <c r="AF28" s="69"/>
-      <c r="AG28" s="69"/>
-      <c r="AH28" s="69"/>
-      <c r="AI28" s="69"/>
       <c r="AS28" s="61"/>
       <c r="AT28" s="61"/>
       <c r="AU28" s="61"/>
       <c r="AV28" s="61"/>
       <c r="AW28" s="61"/>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" spans="1:50">
       <c r="A29" s="61"/>
       <c r="C29" s="61"/>
       <c r="D29" s="61"/>
@@ -4198,18 +5046,13 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-      <c r="AE29" s="69"/>
-      <c r="AF29" s="69"/>
-      <c r="AG29" s="69"/>
-      <c r="AH29" s="69"/>
-      <c r="AI29" s="69"/>
       <c r="AS29" s="61"/>
       <c r="AT29" s="61"/>
       <c r="AU29" s="61"/>
       <c r="AV29" s="61"/>
       <c r="AW29" s="61"/>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" spans="1:50">
       <c r="A30" s="61"/>
       <c r="C30" s="61"/>
       <c r="D30" s="61"/>
@@ -4228,18 +5071,13 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-      <c r="AE30" s="69"/>
-      <c r="AF30" s="69"/>
-      <c r="AG30" s="69"/>
-      <c r="AH30" s="69"/>
-      <c r="AI30" s="69"/>
       <c r="AS30" s="61"/>
       <c r="AT30" s="61"/>
       <c r="AU30" s="61"/>
       <c r="AV30" s="61"/>
       <c r="AW30" s="61"/>
     </row>
-    <row r="31" spans="1:49">
+    <row r="31" spans="1:50">
       <c r="A31" s="61"/>
       <c r="C31" s="61"/>
       <c r="D31" s="61"/>
@@ -4258,18 +5096,13 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
-      <c r="AE31" s="69"/>
-      <c r="AF31" s="69"/>
-      <c r="AG31" s="69"/>
-      <c r="AH31" s="69"/>
-      <c r="AI31" s="69"/>
       <c r="AS31" s="61"/>
       <c r="AT31" s="61"/>
       <c r="AU31" s="61"/>
       <c r="AV31" s="61"/>
       <c r="AW31" s="61"/>
     </row>
-    <row r="32" spans="1:49">
+    <row r="32" spans="1:50">
       <c r="A32" s="61"/>
       <c r="C32" s="61"/>
       <c r="D32" s="61"/>
@@ -4288,11 +5121,6 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-      <c r="AE32" s="69"/>
-      <c r="AF32" s="69"/>
-      <c r="AG32" s="69"/>
-      <c r="AH32" s="69"/>
-      <c r="AI32" s="69"/>
       <c r="AS32" s="61"/>
       <c r="AT32" s="61"/>
       <c r="AU32" s="61"/>
@@ -4318,11 +5146,6 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
-      <c r="AE33" s="69"/>
-      <c r="AF33" s="69"/>
-      <c r="AG33" s="69"/>
-      <c r="AH33" s="69"/>
-      <c r="AI33" s="69"/>
       <c r="AS33" s="61"/>
       <c r="AT33" s="61"/>
       <c r="AU33" s="61"/>
@@ -4347,11 +5170,6 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
-      <c r="AE34" s="69"/>
-      <c r="AF34" s="69"/>
-      <c r="AG34" s="69"/>
-      <c r="AH34" s="69"/>
-      <c r="AI34" s="69"/>
       <c r="AS34" s="61"/>
       <c r="AT34" s="61"/>
       <c r="AU34" s="61"/>
@@ -4377,11 +5195,6 @@
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
-      <c r="AE35" s="69"/>
-      <c r="AF35" s="69"/>
-      <c r="AG35" s="69"/>
-      <c r="AH35" s="69"/>
-      <c r="AI35" s="69"/>
       <c r="AS35" s="61"/>
       <c r="AT35" s="61"/>
       <c r="AU35" s="61"/>
@@ -4407,11 +5220,6 @@
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
-      <c r="AE36" s="69"/>
-      <c r="AF36" s="69"/>
-      <c r="AG36" s="69"/>
-      <c r="AH36" s="69"/>
-      <c r="AI36" s="69"/>
       <c r="AS36" s="61"/>
       <c r="AT36" s="61"/>
       <c r="AU36" s="61"/>
@@ -4437,11 +5245,6 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
-      <c r="AE37" s="69"/>
-      <c r="AF37" s="69"/>
-      <c r="AG37" s="69"/>
-      <c r="AH37" s="69"/>
-      <c r="AI37" s="69"/>
       <c r="AS37" s="61"/>
       <c r="AT37" s="61"/>
       <c r="AU37" s="61"/>
@@ -4467,11 +5270,6 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
-      <c r="AE38" s="69"/>
-      <c r="AF38" s="69"/>
-      <c r="AG38" s="69"/>
-      <c r="AH38" s="69"/>
-      <c r="AI38" s="69"/>
       <c r="AS38" s="61"/>
       <c r="AT38" s="61"/>
       <c r="AU38" s="61"/>
@@ -4496,11 +5294,6 @@
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
-      <c r="AE39" s="69"/>
-      <c r="AF39" s="69"/>
-      <c r="AG39" s="69"/>
-      <c r="AH39" s="69"/>
-      <c r="AI39" s="69"/>
       <c r="AS39" s="61"/>
       <c r="AT39" s="61"/>
       <c r="AU39" s="61"/>
@@ -4526,11 +5319,6 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
-      <c r="AE40" s="69"/>
-      <c r="AF40" s="69"/>
-      <c r="AG40" s="69"/>
-      <c r="AH40" s="69"/>
-      <c r="AI40" s="69"/>
       <c r="AS40" s="61"/>
       <c r="AT40" s="61"/>
       <c r="AU40" s="61"/>
@@ -4556,11 +5344,6 @@
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
-      <c r="AE41" s="69"/>
-      <c r="AF41" s="69"/>
-      <c r="AG41" s="69"/>
-      <c r="AH41" s="69"/>
-      <c r="AI41" s="69"/>
       <c r="AS41" s="61"/>
       <c r="AT41" s="61"/>
       <c r="AU41" s="61"/>
@@ -4586,11 +5369,6 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
-      <c r="AE42" s="69"/>
-      <c r="AF42" s="69"/>
-      <c r="AG42" s="69"/>
-      <c r="AH42" s="69"/>
-      <c r="AI42" s="69"/>
       <c r="AS42" s="61"/>
       <c r="AT42" s="61"/>
       <c r="AU42" s="61"/>
@@ -4615,11 +5393,6 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
-      <c r="AE43" s="69"/>
-      <c r="AF43" s="69"/>
-      <c r="AG43" s="69"/>
-      <c r="AH43" s="69"/>
-      <c r="AI43" s="69"/>
       <c r="AS43" s="61"/>
       <c r="AT43" s="61"/>
       <c r="AU43" s="61"/>
@@ -4644,11 +5417,6 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-      <c r="AE44" s="69"/>
-      <c r="AF44" s="69"/>
-      <c r="AG44" s="69"/>
-      <c r="AH44" s="69"/>
-      <c r="AI44" s="69"/>
       <c r="AS44" s="61"/>
       <c r="AT44" s="61"/>
       <c r="AU44" s="61"/>
@@ -4673,11 +5441,6 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
-      <c r="AE45" s="69"/>
-      <c r="AF45" s="69"/>
-      <c r="AG45" s="69"/>
-      <c r="AH45" s="69"/>
-      <c r="AI45" s="69"/>
       <c r="AS45" s="61"/>
       <c r="AT45" s="61"/>
       <c r="AU45" s="61"/>
@@ -4703,11 +5466,6 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-      <c r="AE46" s="69"/>
-      <c r="AF46" s="69"/>
-      <c r="AG46" s="69"/>
-      <c r="AH46" s="69"/>
-      <c r="AI46" s="69"/>
       <c r="AS46" s="61"/>
       <c r="AT46" s="61"/>
       <c r="AU46" s="61"/>
@@ -4733,11 +5491,6 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-      <c r="AE47" s="69"/>
-      <c r="AF47" s="69"/>
-      <c r="AG47" s="69"/>
-      <c r="AH47" s="69"/>
-      <c r="AI47" s="69"/>
       <c r="AS47" s="61"/>
       <c r="AT47" s="61"/>
       <c r="AU47" s="61"/>
@@ -4763,11 +5516,6 @@
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
-      <c r="AE48" s="69"/>
-      <c r="AF48" s="69"/>
-      <c r="AG48" s="69"/>
-      <c r="AH48" s="69"/>
-      <c r="AI48" s="69"/>
       <c r="AS48" s="61"/>
       <c r="AT48" s="61"/>
       <c r="AU48" s="61"/>
@@ -4792,11 +5540,6 @@
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
-      <c r="AE49" s="69"/>
-      <c r="AF49" s="69"/>
-      <c r="AG49" s="69"/>
-      <c r="AH49" s="69"/>
-      <c r="AI49" s="69"/>
       <c r="AS49" s="61"/>
       <c r="AT49" s="61"/>
       <c r="AU49" s="61"/>
@@ -4822,11 +5565,6 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
-      <c r="AE50" s="69"/>
-      <c r="AF50" s="69"/>
-      <c r="AG50" s="69"/>
-      <c r="AH50" s="69"/>
-      <c r="AI50" s="69"/>
       <c r="AS50" s="61"/>
       <c r="AT50" s="61"/>
       <c r="AU50" s="61"/>
@@ -4844,11 +5582,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4926,11 +5667,11 @@
       <c r="G2" s="71">
         <v>2019</v>
       </c>
-      <c r="H2" s="71">
-        <v>2019</v>
+      <c r="H2" s="61">
+        <v>2016</v>
       </c>
       <c r="I2" s="73">
-        <v>0.67875875500000005</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="J2" s="71" t="s">
         <v>130</v>
@@ -4942,230 +5683,236 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" s="61" customFormat="1">
       <c r="A3" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="71">
+        <v>2040</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="G3" s="71">
+        <v>2019</v>
+      </c>
+      <c r="H3" s="61">
+        <v>2016</v>
+      </c>
+      <c r="I3" s="76">
+        <v>70457</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>314</v>
+      </c>
+      <c r="K3" s="61">
+        <v>2050</v>
+      </c>
+      <c r="L3" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="61" customFormat="1">
+      <c r="A4" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="71">
+        <v>2040</v>
+      </c>
+      <c r="E4" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G4" s="71">
+        <v>2019</v>
+      </c>
+      <c r="H4" s="61">
+        <v>2016</v>
+      </c>
+      <c r="I4" s="61">
+        <v>0.67</v>
+      </c>
+      <c r="J4" s="61" t="s">
+        <v>315</v>
+      </c>
+      <c r="K4" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L4" s="75">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C5" s="61" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="54">
+      <c r="D5" s="54">
         <v>2050</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E5" s="71" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" s="71" t="s">
+        <v>313</v>
+      </c>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54">
+        <v>2005</v>
+      </c>
+      <c r="I5" s="70">
+        <v>10178945</v>
+      </c>
+      <c r="J5" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="K5" s="54">
+        <v>2050</v>
+      </c>
+      <c r="L5" s="63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E6" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F6" s="61" t="s">
         <v>313</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54">
-        <v>2019</v>
-      </c>
-      <c r="I3" s="70">
-        <v>0.52047155000000001</v>
-      </c>
-      <c r="J3" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" s="54">
-        <v>2050</v>
-      </c>
-      <c r="L3" s="63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="61" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="26">
-        <v>2050</v>
-      </c>
-      <c r="E4" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="61" t="s">
-        <v>310</v>
-      </c>
-      <c r="H4" s="20">
-        <v>2019</v>
-      </c>
-      <c r="I4" s="61">
+      <c r="H6" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I6" s="61">
         <f>(16*0.4+9*0.5)/(16+9)</f>
         <v>0.436</v>
       </c>
-      <c r="J4" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="K4" s="61">
-        <v>2030</v>
-      </c>
-      <c r="L4" s="75">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="61" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="26">
-        <v>2050</v>
-      </c>
-      <c r="E5" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="61" t="s">
-        <v>310</v>
-      </c>
-      <c r="H5" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I5" s="70">
-        <v>0.80188104599999999</v>
-      </c>
-      <c r="J5" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="K5" s="61">
-        <v>2030</v>
-      </c>
-      <c r="L5" s="61">
-        <f>1-0.545504813/0.801881046</f>
-        <v>0.3197185346615613</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="61" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="26">
-        <v>2050</v>
-      </c>
-      <c r="E6" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="61" t="s">
-        <v>310</v>
-      </c>
-      <c r="H6" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I6" s="70">
-        <v>0.80188104599999999</v>
-      </c>
       <c r="J6" s="71" t="s">
         <v>130</v>
       </c>
       <c r="K6" s="61">
-        <v>2040</v>
-      </c>
-      <c r="L6" s="61">
-        <f>1-0.151874771/0.801881046</f>
-        <v>0.810601869494743</v>
+        <v>2030</v>
+      </c>
+      <c r="L6" s="75">
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="61" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D7" s="26">
         <v>2050</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>66</v>
+      <c r="E7" s="71" t="s">
+        <v>311</v>
       </c>
       <c r="F7" s="61" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="H7" s="20">
-        <v>2020</v>
-      </c>
-      <c r="I7" s="61">
-        <f>49271373/76459982</f>
-        <v>0.64440733192953148</v>
+        <v>2005</v>
+      </c>
+      <c r="I7" s="76">
+        <v>38113792</v>
       </c>
       <c r="J7" s="71" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="K7" s="61">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L7" s="75">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="61" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D8" s="26">
-        <v>2035</v>
-      </c>
-      <c r="E8" s="26" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E8" s="71" t="s">
         <v>311</v>
       </c>
       <c r="F8" s="61" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="H8" s="20">
-        <v>2015</v>
-      </c>
-      <c r="I8" s="70">
-        <v>1.3146552000000001E-2</v>
+        <v>2005</v>
+      </c>
+      <c r="I8" s="76">
+        <v>38113792</v>
       </c>
       <c r="J8" s="71" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="K8" s="61">
-        <v>2025</v>
+        <v>2040</v>
       </c>
       <c r="L8" s="75">
-        <v>0.35</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="61" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>175</v>
+        <v>163</v>
+      </c>
+      <c r="D9" s="26">
+        <v>2050</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>66</v>
@@ -5174,51 +5921,513 @@
         <v>310</v>
       </c>
       <c r="H9" s="20">
-        <v>2005</v>
+        <v>2000</v>
       </c>
       <c r="I9" s="61">
-        <v>1</v>
+        <v>167000000</v>
       </c>
       <c r="J9" s="71" t="s">
-        <v>312</v>
+        <v>143</v>
       </c>
       <c r="K9" s="61">
         <v>2030</v>
       </c>
       <c r="L9" s="75">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="61" customFormat="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="61" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" s="26"/>
+        <v>169</v>
+      </c>
+      <c r="D10" s="26">
+        <v>2035</v>
+      </c>
       <c r="E10" s="26" t="s">
-        <v>66</v>
+        <v>311</v>
       </c>
       <c r="F10" s="61" t="s">
         <v>310</v>
       </c>
       <c r="H10" s="20">
+        <v>2015</v>
+      </c>
+      <c r="I10" s="70">
+        <v>1.3146552000000001E-2</v>
+      </c>
+      <c r="J10" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" s="61">
+        <v>2025</v>
+      </c>
+      <c r="L10" s="75">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="H11" s="20">
         <v>2005</v>
       </c>
-      <c r="I10" s="61">
+      <c r="I11" s="61">
         <v>1</v>
       </c>
-      <c r="J10" s="71" t="s">
+      <c r="J11" s="71" t="s">
         <v>312</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K11" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L11" s="75">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="61" customFormat="1">
+      <c r="A12" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="H12" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I12" s="61">
+        <v>1</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>312</v>
+      </c>
+      <c r="K12" s="61">
         <v>2040</v>
       </c>
-      <c r="L10" s="75">
+      <c r="L12" s="75">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="H13" s="20">
+        <v>2020</v>
+      </c>
+      <c r="I13" s="61">
+        <f>0.292832151/0.141</f>
+        <v>2.0768237659574469</v>
+      </c>
+      <c r="J13" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="K13" s="61">
+        <v>2050</v>
+      </c>
+      <c r="L13" s="75">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>311</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="G14" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H14" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I14" s="61">
+        <v>25218000</v>
+      </c>
+      <c r="J14" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="61">
+        <v>2040</v>
+      </c>
+      <c r="L14" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="61" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G15" s="61">
+        <v>2021</v>
+      </c>
+      <c r="H15" s="20">
+        <v>2019</v>
+      </c>
+      <c r="I15" s="61">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="J15" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="K15" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L15" s="75">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="H16" s="20">
+        <v>2011</v>
+      </c>
+      <c r="I16" s="61">
+        <v>24000000</v>
+      </c>
+      <c r="J16" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="K16" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L16" s="75">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G17" s="61">
+        <v>2017</v>
+      </c>
+      <c r="H17" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I17" s="61">
+        <v>37700000</v>
+      </c>
+      <c r="J17" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="K17" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L17" s="75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G18" s="61">
+        <v>2017</v>
+      </c>
+      <c r="H18" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I18" s="61">
+        <v>37700000</v>
+      </c>
+      <c r="J18" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="K18" s="61">
+        <v>2040</v>
+      </c>
+      <c r="L18" s="75">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F19" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="H19" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I19" s="61">
+        <v>59.347999999999999</v>
+      </c>
+      <c r="J19" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="K19" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L19" s="75">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F20" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="H20" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I20" s="61">
+        <v>153000000</v>
+      </c>
+      <c r="J20" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="K20" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L20" s="75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="G21" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H21" s="20">
+        <v>2000</v>
+      </c>
+      <c r="I21" s="61">
+        <v>49960899</v>
+      </c>
+      <c r="J21" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="K21" s="61">
+        <v>2050</v>
+      </c>
+      <c r="L21" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G22" s="61">
+        <v>2030</v>
+      </c>
+      <c r="H22" s="20">
+        <v>2000</v>
+      </c>
+      <c r="I22" s="61">
+        <v>0.4826223</v>
+      </c>
+      <c r="J22" s="71" t="s">
+        <v>320</v>
+      </c>
+      <c r="K22" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L22" s="75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="26">
+        <v>2045</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="H23" s="20">
+        <v>2005</v>
+      </c>
+      <c r="I23" s="76">
+        <v>48455198</v>
+      </c>
+      <c r="J23" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L23" s="75">
         <v>0.7</v>
       </c>
     </row>
@@ -5228,6 +6437,7 @@
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000Confidential&amp;1#</oddHeader>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11609,6 +12819,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -11825,22 +13050,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11857,29 +13092,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update 20220215 ITR Tool Sample Data.xlsx
RMI data more consistent due to ALLETE corp hierarchy.  Difficult to see comparable Y-on-Y data from EEI.
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Dropbox/My Mac (MacBook-Pro.local)/Documents/GitHub/os-climate/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E1DDAA-2491-1347-908A-657C8C561B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AE9538-6439-BC4B-9311-FD47549B0D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19540" yWindow="29460" windowWidth="81680" windowHeight="20280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -2575,10 +2575,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2908,11 +2904,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE2" sqref="AE2:AK4"/>
+      <selection pane="bottomRight" activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -3174,7 +3170,7 @@
       <c r="AC2" s="53"/>
       <c r="AD2" s="53"/>
       <c r="AE2" s="69">
-        <f t="shared" ref="AE2:AE4" si="0">IF(ISBLANK(Q2),IF(ISBLANK(X2),"",X2),Q2+X2)</f>
+        <f t="shared" ref="AE2" si="0">IF(ISBLANK(Q2),IF(ISBLANK(X2),"",X2),Q2+X2)</f>
         <v>70763000</v>
       </c>
       <c r="AF2" s="69">
@@ -3285,80 +3281,46 @@
         <v>5482800000</v>
       </c>
       <c r="O3" s="61" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="P3" s="61" t="s">
-        <v>144</v>
+        <v>321</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2">
-        <v>1210847</v>
-      </c>
-      <c r="U3" s="2">
-        <v>297479</v>
-      </c>
-      <c r="V3" s="2">
-        <v>2782868</v>
-      </c>
-      <c r="W3" s="36">
-        <v>2720482</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>5249805</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>3221290</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>2027896</v>
-      </c>
-      <c r="AD3" s="36">
-        <v>1370397</v>
-      </c>
-      <c r="AE3" s="69" t="str">
-        <f>IF(ISBLANK(Q3),IF(ISBLANK(X3),"",X3),Q3+X3)</f>
-        <v/>
-      </c>
-      <c r="AF3" s="69" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AG3" s="69" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="Z3" s="78"/>
+      <c r="AE3" s="69">
+        <v>8.0287915250000008</v>
+      </c>
+      <c r="AF3" s="69">
+        <v>6.5660701670000003</v>
+      </c>
+      <c r="AG3" s="69">
+        <v>6.511972042</v>
       </c>
       <c r="AH3" s="69">
-        <f t="shared" si="3"/>
-        <v>6460652</v>
+        <v>4.3830481260000003</v>
       </c>
       <c r="AI3" s="69">
-        <f t="shared" si="4"/>
-        <v>3518769</v>
-      </c>
-      <c r="AJ3" s="69">
-        <f t="shared" si="5"/>
-        <v>4810764</v>
-      </c>
-      <c r="AK3" s="69">
-        <f t="shared" si="6"/>
-        <v>4090879</v>
-      </c>
-      <c r="AS3" s="61"/>
-      <c r="AT3" s="61"/>
-      <c r="AU3" s="61"/>
+        <v>4.2416594769999998</v>
+      </c>
+      <c r="AS3" s="61">
+        <v>12.04283116</v>
+      </c>
+      <c r="AT3" s="61">
+        <v>10.83695122</v>
+      </c>
+      <c r="AU3" s="61">
+        <v>10.50623193</v>
+      </c>
       <c r="AV3" s="61">
-        <v>3441242</v>
+        <v>8.4213020440000008</v>
       </c>
       <c r="AW3" s="61">
-        <v>2540911</v>
-      </c>
-      <c r="AX3" s="2">
-        <v>5081479</v>
-      </c>
-      <c r="AY3" s="2">
-        <v>4870600</v>
+        <v>8.4483908050000007</v>
       </c>
     </row>
     <row r="4" spans="1:52">
@@ -3657,6 +3619,14 @@
         <f t="shared" ref="AI6:AI8" si="12">IF(ISBLANK(U6),IF(ISBLANK(AB6),"",AB6),U6+AB6)</f>
         <v>51342920</v>
       </c>
+      <c r="AJ6" s="69" t="str">
+        <f t="shared" ref="AJ6:AK8" si="13">IF(ISBLANK(V6),IF(ISBLANK(AC6),"",AC6),V6+AC6)</f>
+        <v/>
+      </c>
+      <c r="AK6" s="69" t="str">
+        <f t="shared" ref="AK6:AK8" si="14">IF(ISBLANK(W6),IF(ISBLANK(AD6),"",AD6),W6+AD6)</f>
+        <v/>
+      </c>
       <c r="AS6" s="76">
         <v>137346204</v>
       </c>
@@ -3762,6 +3732,14 @@
         <f t="shared" si="12"/>
         <v>1713731</v>
       </c>
+      <c r="AJ7" s="69" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AK7" s="69" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
       <c r="AN7" s="2">
         <v>21590220</v>
       </c>
@@ -3871,6 +3849,14 @@
       <c r="AI8" s="69">
         <f t="shared" si="12"/>
         <v>5038179</v>
+      </c>
+      <c r="AJ8" s="69" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="AK8" s="69" t="str">
+        <f t="shared" si="14"/>
+        <v/>
       </c>
       <c r="AS8" s="61"/>
       <c r="AT8" s="61"/>
@@ -4122,31 +4108,31 @@
         <v>1436765</v>
       </c>
       <c r="AE11" s="69" t="str">
-        <f t="shared" ref="AE11:AK11" si="13">IF(ISBLANK(Q11),IF(ISBLANK(X11),"",X11),Q11+X11)</f>
+        <f t="shared" ref="AE11:AK11" si="15">IF(ISBLANK(Q11),IF(ISBLANK(X11),"",X11),Q11+X11)</f>
         <v/>
       </c>
       <c r="AF11" s="69" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AG11" s="69" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH11" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2548437</v>
       </c>
       <c r="AI11" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2572986</v>
       </c>
       <c r="AJ11" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2554518</v>
       </c>
       <c r="AK11" s="69" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AS11" s="61">
@@ -5589,7 +5575,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="A24:D24"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7655,8 +7641,10 @@
   <dimension ref="A1:AZ54"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AE3" sqref="AE3:AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -12825,15 +12813,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -13050,6 +13029,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
   <ds:schemaRefs>
@@ -13068,14 +13056,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13092,4 +13072,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
This WIP checkin fixes a number of observed problems and target projections now seem to be coming back correctly.
WIP check-in fixes initialization code that was using default, rather than user-provided emissions_units.  Also changed interface of project_targets to work with pd>Series rather than 1-dimensional pd.DataFrames.  Pint is so much happier working with either unitized pd.Series or unitized pd.DataFrame columns.  It can work across columns, but to make element-by-element computations work, one must do un-Pandas-ish things.

Also fixed a data entry error revealed when chasing unit initialization error.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED085D43-E994-804D-B202-8C3FBB4EDCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4D5988-6EB7-F746-BE77-FD95750C480D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46640" yWindow="4720" windowWidth="44300" windowHeight="39960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59720" yWindow="2620" windowWidth="44300" windowHeight="39960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="323">
   <si>
     <t>Data field</t>
   </si>
@@ -1292,9 +1292,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Gt CO2</t>
-  </si>
-  <si>
-    <t>tons CO2/MWh</t>
   </si>
   <si>
     <t>GWh</t>
@@ -3050,10 +3047,10 @@
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AH4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS23" sqref="AS23"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -3278,7 +3275,7 @@
         <v>143</v>
       </c>
       <c r="P2" s="61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q2" s="53">
         <v>70457000</v>
@@ -3429,7 +3426,7 @@
         <v>129</v>
       </c>
       <c r="P3" s="61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -3634,7 +3631,7 @@
         <v>129</v>
       </c>
       <c r="P5" s="61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q5" s="78"/>
       <c r="R5" s="78"/>
@@ -3842,7 +3839,7 @@
         <v>143</v>
       </c>
       <c r="P7" s="61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q7" s="78">
         <v>1040335</v>
@@ -4083,7 +4080,7 @@
         <v>129</v>
       </c>
       <c r="P9" s="61" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -4168,7 +4165,7 @@
         <v>129</v>
       </c>
       <c r="P10" s="61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -4364,7 +4361,7 @@
         <v>129</v>
       </c>
       <c r="P12" s="61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -4447,7 +4444,7 @@
         <v>129</v>
       </c>
       <c r="P13" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -4533,7 +4530,7 @@
         <v>129</v>
       </c>
       <c r="P14" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -4619,7 +4616,7 @@
         <v>129</v>
       </c>
       <c r="P15" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -4719,7 +4716,7 @@
         <v>129</v>
       </c>
       <c r="P16" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -4805,7 +4802,7 @@
         <v>129</v>
       </c>
       <c r="P17" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -4888,7 +4885,7 @@
         <v>129</v>
       </c>
       <c r="P18" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -4974,7 +4971,7 @@
         <v>129</v>
       </c>
       <c r="P19" s="68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q19" s="82"/>
       <c r="R19" s="2"/>
@@ -6134,10 +6131,10 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6248,7 +6245,7 @@
         <v>66</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G3" s="71">
         <v>2019</v>
@@ -6298,7 +6295,7 @@
         <v>0.67</v>
       </c>
       <c r="J4" s="61" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="K4" s="61">
         <v>2030</v>
@@ -6542,7 +6539,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="71" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="K11" s="61">
         <v>2030</v>
@@ -6575,7 +6572,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="71" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="K12" s="61">
         <v>2040</v>
@@ -6608,7 +6605,7 @@
         <v>2.0768237659574469</v>
       </c>
       <c r="J13" s="71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K13" s="61">
         <v>2050</v>
@@ -6631,7 +6628,7 @@
         <v>311</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G14" s="61">
         <v>2020</v>
@@ -6678,7 +6675,7 @@
         <v>0.48099999999999998</v>
       </c>
       <c r="J15" s="71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K15" s="61">
         <v>2030</v>
@@ -6885,7 +6882,7 @@
         <v>311</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G21" s="61">
         <v>2020</v>
@@ -6935,7 +6932,7 @@
         <v>0.4826223</v>
       </c>
       <c r="J22" s="71" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K22" s="61">
         <v>2030</v>
@@ -7040,7 +7037,7 @@
         <v>1050</v>
       </c>
       <c r="J25" s="71" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K25" s="61">
         <v>2022</v>
@@ -7148,7 +7145,7 @@
         <v>0.93</v>
       </c>
       <c r="J28" s="71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K28" s="61">
         <v>2031</v>

</xml_diff>

<commit_message>
Handle columns that start with 1990s, not only 2000s data
Also, update spreadsheet with new targets up through National Grid (which contains a 1990 baseline target).  And update list of company ids to match.

Please look carefully at _add_projections_to_companies, which was wrong and likely is wrong still.  That needs to be fixed!

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4D5988-6EB7-F746-BE77-FD95750C480D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ABD72C-2027-7240-A66D-8EF27E967A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="59720" yWindow="2620" windowWidth="44300" windowHeight="39960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="323">
   <si>
     <t>Data field</t>
   </si>
@@ -3050,7 +3050,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -5449,102 +5449,335 @@
       </c>
     </row>
     <row r="24" spans="1:50">
-      <c r="A24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="AS24" s="61"/>
-      <c r="AT24" s="61"/>
-      <c r="AU24" s="61"/>
-      <c r="AV24" s="61"/>
-      <c r="AW24" s="61"/>
+      <c r="A24" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>230</v>
+      </c>
+      <c r="D24" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J24" s="61">
+        <v>3937071331</v>
+      </c>
+      <c r="K24" s="61">
+        <v>2873948000</v>
+      </c>
+      <c r="L24" s="61">
+        <v>5704623331</v>
+      </c>
+      <c r="M24" s="61">
+        <v>5901436331</v>
+      </c>
+      <c r="N24" s="61">
+        <v>13745251000</v>
+      </c>
+      <c r="O24" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="P24" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>3.8868941879999999</v>
+      </c>
+      <c r="R24" s="2">
+        <v>3.8663196809999998</v>
+      </c>
+      <c r="S24" s="2">
+        <v>3.937301664</v>
+      </c>
+      <c r="T24" s="2">
+        <v>3.9790181429999998</v>
+      </c>
+      <c r="U24" s="2">
+        <v>3.8259789839999998</v>
+      </c>
+      <c r="AS24" s="61">
+        <v>7.9426489999999994</v>
+      </c>
+      <c r="AT24" s="61">
+        <v>7.8881049999999986</v>
+      </c>
+      <c r="AU24" s="61">
+        <v>7.9569290000000006</v>
+      </c>
+      <c r="AV24" s="61">
+        <v>7.9702040000000007</v>
+      </c>
+      <c r="AW24" s="61">
+        <v>8.0778513040000011</v>
+      </c>
     </row>
     <row r="25" spans="1:50">
-      <c r="A25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="68"/>
-      <c r="P25" s="68"/>
+      <c r="A25" s="61" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="61" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J25" s="61">
+        <v>4447584104</v>
+      </c>
+      <c r="K25" s="61">
+        <v>5336776000</v>
+      </c>
+      <c r="L25" s="61">
+        <v>6624232104</v>
+      </c>
+      <c r="M25" s="61">
+        <v>6690691104</v>
+      </c>
+      <c r="N25" s="61">
+        <v>7683059000</v>
+      </c>
+      <c r="O25" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="P25" s="68" t="s">
+        <v>144</v>
+      </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-      <c r="AS25" s="61"/>
-      <c r="AT25" s="61"/>
-      <c r="AU25" s="61"/>
-      <c r="AV25" s="61"/>
-      <c r="AW25" s="61"/>
+      <c r="AE25" s="69">
+        <v>1.8746218750000001</v>
+      </c>
+      <c r="AF25" s="69">
+        <v>1.844359927</v>
+      </c>
+      <c r="AG25" s="69">
+        <v>2.051568649</v>
+      </c>
+      <c r="AH25" s="69">
+        <v>1.710493431</v>
+      </c>
+      <c r="AI25" s="69">
+        <v>0</v>
+      </c>
+      <c r="AS25" s="61">
+        <v>3.1870937499999998</v>
+      </c>
+      <c r="AT25" s="61">
+        <v>3.1660149999999998</v>
+      </c>
+      <c r="AU25" s="61">
+        <v>3.3211175000000002</v>
+      </c>
+      <c r="AV25" s="61">
+        <v>3.1475861959999998</v>
+      </c>
+      <c r="AW25" s="61">
+        <v>3.1903747390000001</v>
+      </c>
     </row>
     <row r="26" spans="1:50">
-      <c r="A26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="68"/>
-      <c r="P26" s="68"/>
+      <c r="A26" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J26" s="61">
+        <v>12430000000</v>
+      </c>
+      <c r="K26" s="61">
+        <v>22588858000</v>
+      </c>
+      <c r="L26" s="61">
+        <v>15186696000</v>
+      </c>
+      <c r="M26" s="61">
+        <v>16721301000</v>
+      </c>
+      <c r="N26" s="61">
+        <v>18344666000</v>
+      </c>
+      <c r="O26" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="P26" s="61" t="s">
+        <v>183</v>
+      </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="AS26" s="61"/>
-      <c r="AT26" s="61"/>
-      <c r="AU26" s="61"/>
-      <c r="AV26" s="61"/>
-      <c r="AW26" s="61"/>
+      <c r="AE26" s="69">
+        <v>12.356382978723399</v>
+      </c>
+      <c r="AF26" s="69">
+        <v>11.819148936170221</v>
+      </c>
+      <c r="AG26" s="69">
+        <v>11.281914893617021</v>
+      </c>
+      <c r="AH26" s="69">
+        <v>10.1</v>
+      </c>
+      <c r="AI26" s="69">
+        <v>10.1</v>
+      </c>
+      <c r="AS26" s="61">
+        <v>21.48936170212766</v>
+      </c>
+      <c r="AT26" s="61">
+        <v>21.48936170212766</v>
+      </c>
+      <c r="AU26" s="61">
+        <v>21.48936170212766</v>
+      </c>
+      <c r="AV26" s="61">
+        <v>21.48936170212766</v>
+      </c>
+      <c r="AW26" s="61">
+        <v>21.48936170212766</v>
+      </c>
     </row>
     <row r="27" spans="1:50">
-      <c r="A27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
+      <c r="A27" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>239</v>
+      </c>
+      <c r="D27" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>241</v>
+      </c>
+      <c r="F27" s="61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="5">
+        <v>44561</v>
+      </c>
+      <c r="J27" s="61">
+        <v>44164533765.359467</v>
+      </c>
+      <c r="K27" s="61">
+        <v>19393506493.506489</v>
+      </c>
       <c r="L27" s="61"/>
       <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="P27" s="61"/>
+      <c r="N27" s="61">
+        <v>81770129870.129868</v>
+      </c>
+      <c r="O27" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="P27" s="68" t="s">
+        <v>144</v>
+      </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-      <c r="AS27" s="61"/>
-      <c r="AT27" s="61"/>
-      <c r="AU27" s="61"/>
-      <c r="AV27" s="61"/>
-      <c r="AW27" s="61"/>
+      <c r="AE27" s="69">
+        <v>3.004725724</v>
+      </c>
+      <c r="AF27" s="69">
+        <v>2.1325357700000001</v>
+      </c>
+      <c r="AG27" s="69">
+        <v>3.0720788620000001</v>
+      </c>
+      <c r="AH27" s="69">
+        <v>2.4277569909999999</v>
+      </c>
+      <c r="AI27" s="69">
+        <v>1.335266345</v>
+      </c>
+      <c r="AS27" s="61">
+        <v>4.836665</v>
+      </c>
+      <c r="AT27" s="61">
+        <v>3.3607879999999999</v>
+      </c>
+      <c r="AU27" s="61">
+        <v>4.6763309999999993</v>
+      </c>
+      <c r="AV27" s="61">
+        <v>3.8903590000000001</v>
+      </c>
+      <c r="AW27" s="61">
+        <v>3.5954304822953862</v>
+      </c>
     </row>
     <row r="28" spans="1:50">
       <c r="A28" s="61"/>
@@ -6128,13 +6361,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7152,6 +7385,187 @@
       </c>
       <c r="L28" s="75">
         <v>0.10800000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G29" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H29" s="20">
+        <v>2010</v>
+      </c>
+      <c r="I29" s="61">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="J29" s="71" t="s">
+        <v>319</v>
+      </c>
+      <c r="K29" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L29" s="75">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="61" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C30" s="61" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="H30" s="20">
+        <v>2000</v>
+      </c>
+      <c r="I30" s="61">
+        <f>2650/2000</f>
+        <v>1.325</v>
+      </c>
+      <c r="J30" s="71" t="s">
+        <v>319</v>
+      </c>
+      <c r="K30" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L30" s="75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="E31" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="G31" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H31" s="61">
+        <v>2015</v>
+      </c>
+      <c r="I31" s="61">
+        <v>0.82</v>
+      </c>
+      <c r="J31" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="K31" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L31" s="75">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="61" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E32" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G32" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H32" s="61">
+        <v>1990</v>
+      </c>
+      <c r="I32" s="61">
+        <f>7000000/(1-0.68)</f>
+        <v>21875000.000000004</v>
+      </c>
+      <c r="J32" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="K32" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L32" s="75">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="61" customFormat="1">
+      <c r="A33" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E33" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="G33" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H33" s="61">
+        <v>1990</v>
+      </c>
+      <c r="I33" s="61">
+        <f>7000000/(1-0.68)</f>
+        <v>21875000.000000004</v>
+      </c>
+      <c r="J33" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="K33" s="61">
+        <v>2040</v>
+      </c>
+      <c r="L33" s="75">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -8378,10 +8792,10 @@
   <dimension ref="A1:AZ54"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28:XFD28"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Regularize emissions_intensity/EI naming and target/trajectory naming
Confusing around target and trajectory naming has been identified as a problem, and now seems like as good a time as any to address.

Changed all emission_XYZ to emissions_XYZ, kept all variables/constants named emissions_intensities, but changed all ABC_emissions_intensities_UVW to ABC_EI_UVW.

Enhanced _add_projections_to_companies to work for multiple scopes.

Enhanced _extrapolate to work with data that doesn't quite reach the end of historic data timeframe in all rows.  Some of our data includes 2021, some does not.  _extrapolate cleans up the ragged edge and then projects from a clean edge.

Fixed some typos in Sample data spreadsheet.

Next thing to fix is GHG_S1S2 variables, which are no longer filled in by the template.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547F21BC-66BA-BD41-AA8F-D45859F09E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02929632-636A-2F48-AD30-CC8BA73B5033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59720" yWindow="2620" windowWidth="44300" windowHeight="39960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55380" yWindow="2620" windowWidth="48640" windowHeight="39960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="322">
   <si>
     <t>Data field</t>
   </si>
@@ -1303,19 +1303,16 @@
     <t>t CO2/Fe_ton</t>
   </si>
   <si>
-    <t>S1+S3</t>
-  </si>
-  <si>
     <t>t CO2/MWh</t>
   </si>
   <si>
     <t>TWh</t>
   </si>
   <si>
-    <t>M Fe_ton</t>
-  </si>
-  <si>
     <t>kt CO2</t>
+  </si>
+  <si>
+    <t>megaFe_ton</t>
   </si>
 </sst>
 </file>
@@ -3049,11 +3046,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32:C32"/>
+      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -3429,7 +3426,7 @@
         <v>129</v>
       </c>
       <c r="P3" s="61" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -3634,7 +3631,7 @@
         <v>129</v>
       </c>
       <c r="P5" s="61" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q5" s="78"/>
       <c r="R5" s="78"/>
@@ -4168,7 +4165,7 @@
         <v>129</v>
       </c>
       <c r="P10" s="61" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -4364,7 +4361,7 @@
         <v>129</v>
       </c>
       <c r="P12" s="61" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -4447,7 +4444,7 @@
         <v>129</v>
       </c>
       <c r="P13" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -4533,7 +4530,7 @@
         <v>129</v>
       </c>
       <c r="P14" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -4619,7 +4616,7 @@
         <v>129</v>
       </c>
       <c r="P15" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -4719,7 +4716,7 @@
         <v>129</v>
       </c>
       <c r="P16" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -4805,7 +4802,7 @@
         <v>129</v>
       </c>
       <c r="P17" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -4888,7 +4885,7 @@
         <v>129</v>
       </c>
       <c r="P18" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -4974,7 +4971,7 @@
         <v>129</v>
       </c>
       <c r="P19" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q19" s="82"/>
       <c r="R19" s="2"/>
@@ -4994,7 +4991,8 @@
         <v>2.2128600000000001E-4</v>
       </c>
       <c r="AI19" s="69">
-        <v>0</v>
+        <f>AH19</f>
+        <v>2.2128600000000001E-4</v>
       </c>
       <c r="AS19" s="61">
         <v>1.080058642</v>
@@ -5598,7 +5596,8 @@
         <v>1.710493431</v>
       </c>
       <c r="AI25" s="69">
-        <v>0</v>
+        <f>AH25*2.26/2.35</f>
+        <v>1.6449851719404254</v>
       </c>
       <c r="AS25" s="61">
         <v>3.1870937499999998</v>
@@ -6113,7 +6112,7 @@
         <v>129</v>
       </c>
       <c r="P31" s="68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -6189,10 +6188,10 @@
         <v>68553124892.036621</v>
       </c>
       <c r="O32" s="61" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="P32" s="61" t="s">
-        <v>183</v>
+        <v>321</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -6685,11 +6684,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6850,7 +6849,7 @@
         <v>0.67</v>
       </c>
       <c r="J4" s="61" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K4" s="61">
         <v>2030</v>
@@ -7094,7 +7093,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K11" s="61">
         <v>2030</v>
@@ -7127,7 +7126,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K12" s="61">
         <v>2040</v>
@@ -7183,7 +7182,7 @@
         <v>311</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G14" s="61">
         <v>2020</v>
@@ -7276,16 +7275,16 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="61" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C17" s="61" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D17" s="26">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="E17" s="26" t="s">
         <v>311</v>
@@ -7294,22 +7293,22 @@
         <v>310</v>
       </c>
       <c r="G17" s="61">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="H17" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I17" s="61">
-        <v>37700000</v>
-      </c>
-      <c r="J17" s="71" t="s">
-        <v>143</v>
+        <v>2020</v>
+      </c>
+      <c r="I17" s="69">
+        <v>1.145419433</v>
+      </c>
+      <c r="J17" s="61" t="s">
+        <v>129</v>
       </c>
       <c r="K17" s="61">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="L17" s="75">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -7344,21 +7343,21 @@
         <v>143</v>
       </c>
       <c r="K18" s="61">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="L18" s="75">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="61" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D19" s="26">
         <v>2050</v>
@@ -7369,31 +7368,34 @@
       <c r="F19" s="61" t="s">
         <v>310</v>
       </c>
+      <c r="G19" s="61">
+        <v>2017</v>
+      </c>
       <c r="H19" s="20">
         <v>2005</v>
       </c>
       <c r="I19" s="61">
-        <v>59.347999999999999</v>
+        <v>37700000</v>
       </c>
       <c r="J19" s="71" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="K19" s="61">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="L19" s="75">
-        <v>0.55000000000000004</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="61" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D20" s="26">
         <v>2050</v>
@@ -7408,27 +7410,27 @@
         <v>2005</v>
       </c>
       <c r="I20" s="61">
-        <v>153000000</v>
+        <v>59.347999999999999</v>
       </c>
       <c r="J20" s="71" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="K20" s="61">
         <v>2030</v>
       </c>
       <c r="L20" s="75">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="61" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D21" s="26">
         <v>2050</v>
@@ -7437,25 +7439,22 @@
         <v>311</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>316</v>
-      </c>
-      <c r="G21" s="61">
-        <v>2020</v>
+        <v>310</v>
       </c>
       <c r="H21" s="20">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="I21" s="61">
-        <v>49960899</v>
+        <v>153000000</v>
       </c>
       <c r="J21" s="71" t="s">
         <v>143</v>
       </c>
       <c r="K21" s="61">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L21" s="75">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -7472,92 +7471,92 @@
         <v>2050</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>66</v>
+        <v>311</v>
       </c>
       <c r="F22" s="61" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="G22" s="61">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="H22" s="20">
         <v>2000</v>
       </c>
       <c r="I22" s="61">
-        <v>0.4826223</v>
+        <v>49960899</v>
       </c>
       <c r="J22" s="71" t="s">
-        <v>319</v>
+        <v>143</v>
       </c>
       <c r="K22" s="61">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L22" s="75">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="61" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D23" s="26">
-        <v>2045</v>
+        <v>2050</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>311</v>
+        <v>66</v>
       </c>
       <c r="F23" s="61" t="s">
         <v>310</v>
       </c>
+      <c r="G23" s="61">
+        <v>2030</v>
+      </c>
       <c r="H23" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I23" s="76">
-        <v>48455198</v>
+        <v>2000</v>
+      </c>
+      <c r="I23" s="61">
+        <v>0.4826223</v>
       </c>
       <c r="J23" s="71" t="s">
-        <v>143</v>
+        <v>318</v>
       </c>
       <c r="K23" s="61">
         <v>2030</v>
       </c>
       <c r="L23" s="75">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="61" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D24" s="26">
-        <v>2030</v>
+        <v>2045</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F24" s="61" t="s">
-        <v>313</v>
-      </c>
-      <c r="G24" s="61">
-        <v>2019</v>
+        <v>310</v>
       </c>
       <c r="H24" s="20">
-        <v>2018</v>
-      </c>
-      <c r="I24" s="61">
-        <v>828107</v>
+        <v>2005</v>
+      </c>
+      <c r="I24" s="76">
+        <v>48455198</v>
       </c>
       <c r="J24" s="71" t="s">
         <v>143</v>
@@ -7566,18 +7565,21 @@
         <v>2030</v>
       </c>
       <c r="L24" s="75">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="61" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>216</v>
+        <v>213</v>
+      </c>
+      <c r="D25" s="26">
+        <v>2030</v>
       </c>
       <c r="E25" s="26" t="s">
         <v>311</v>
@@ -7585,66 +7587,66 @@
       <c r="F25" s="61" t="s">
         <v>313</v>
       </c>
+      <c r="G25" s="61">
+        <v>2019</v>
+      </c>
       <c r="H25" s="20">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="I25" s="61">
-        <v>1050</v>
+        <v>828107</v>
       </c>
       <c r="J25" s="71" t="s">
-        <v>322</v>
+        <v>143</v>
       </c>
       <c r="K25" s="61">
-        <v>2022</v>
+        <v>2030</v>
       </c>
       <c r="L25" s="75">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="61" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C26" s="61" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F26" s="61" t="s">
-        <v>310</v>
-      </c>
-      <c r="G26" s="61">
+        <v>313</v>
+      </c>
+      <c r="H26" s="20">
         <v>2015</v>
       </c>
-      <c r="H26" s="20">
-        <v>2005</v>
-      </c>
       <c r="I26" s="61">
-        <v>86403130</v>
+        <v>1050</v>
       </c>
       <c r="J26" s="71" t="s">
-        <v>143</v>
+        <v>320</v>
       </c>
       <c r="K26" s="61">
-        <v>2045</v>
+        <v>2022</v>
       </c>
       <c r="L26" s="75">
-        <v>0.62</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="61" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>311</v>
@@ -7653,202 +7655,198 @@
         <v>310</v>
       </c>
       <c r="G27" s="61">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="H27" s="20">
-        <v>2019</v>
-      </c>
-      <c r="I27" s="78">
-        <v>11925000</v>
+        <v>2005</v>
+      </c>
+      <c r="I27" s="61">
+        <v>86403130</v>
       </c>
       <c r="J27" s="71" t="s">
         <v>143</v>
       </c>
       <c r="K27" s="61">
-        <v>2035</v>
+        <v>2045</v>
       </c>
       <c r="L27" s="75">
-        <v>0.75</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="61" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C28" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="D28" s="26">
-        <v>2050</v>
+        <v>222</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>66</v>
+        <v>311</v>
       </c>
       <c r="F28" s="61" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G28" s="61">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="H28" s="20">
-        <v>2020</v>
-      </c>
-      <c r="I28" s="61">
-        <v>0.93</v>
+        <v>2019</v>
+      </c>
+      <c r="I28" s="78">
+        <v>11925000</v>
       </c>
       <c r="J28" s="71" t="s">
-        <v>317</v>
+        <v>143</v>
       </c>
       <c r="K28" s="61">
-        <v>2031</v>
+        <v>2035</v>
       </c>
       <c r="L28" s="75">
-        <v>0.10800000000000001</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="61" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C29" s="61" t="s">
-        <v>230</v>
+        <v>225</v>
+      </c>
+      <c r="D29" s="26">
+        <v>2050</v>
       </c>
       <c r="E29" s="26" t="s">
         <v>66</v>
       </c>
       <c r="F29" s="61" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G29" s="61">
+        <v>2022</v>
+      </c>
+      <c r="H29" s="20">
         <v>2020</v>
       </c>
-      <c r="H29" s="20">
-        <v>2010</v>
-      </c>
       <c r="I29" s="61">
-        <v>0.76300000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="J29" s="71" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K29" s="61">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="L29" s="75">
-        <v>0.1</v>
+        <v>0.10800000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="61" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C30" s="61" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>66</v>
       </c>
       <c r="F30" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="G30" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H30" s="20">
+        <v>2010</v>
+      </c>
+      <c r="I30" s="61">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="J30" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="K30" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L30" s="75">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="61" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>233</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="61" t="s">
         <v>313</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H31" s="20">
         <v>2000</v>
       </c>
-      <c r="I30" s="61">
+      <c r="I31" s="61">
         <f>2650/2000</f>
         <v>1.325</v>
       </c>
-      <c r="J30" s="71" t="s">
-        <v>319</v>
-      </c>
-      <c r="K30" s="61">
-        <v>2030</v>
-      </c>
-      <c r="L30" s="75">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="61" t="s">
-        <v>234</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="C31" s="61" t="s">
-        <v>236</v>
-      </c>
-      <c r="E31" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="61" t="s">
-        <v>316</v>
-      </c>
-      <c r="G31" s="61">
-        <v>2020</v>
-      </c>
-      <c r="H31" s="61">
-        <v>2015</v>
-      </c>
-      <c r="I31" s="61">
-        <v>0.82</v>
-      </c>
-      <c r="J31" s="61" t="s">
-        <v>317</v>
+      <c r="J31" s="71" t="s">
+        <v>318</v>
       </c>
       <c r="K31" s="61">
         <v>2030</v>
       </c>
       <c r="L31" s="75">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="61" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C32" s="61" t="s">
-        <v>239</v>
-      </c>
-      <c r="D32" s="26">
-        <v>2050</v>
+        <v>236</v>
       </c>
       <c r="E32" s="61" t="s">
         <v>66</v>
       </c>
       <c r="F32" s="61" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G32" s="61">
         <v>2020</v>
       </c>
       <c r="H32" s="61">
-        <v>1990</v>
+        <v>2015</v>
       </c>
       <c r="I32" s="61">
-        <f>7000000/(1-0.68)</f>
-        <v>21875000.000000004</v>
+        <v>0.82</v>
       </c>
       <c r="J32" s="61" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K32" s="61">
         <v>2030</v>
       </c>
       <c r="L32" s="75">
-        <v>0.8</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="61" customFormat="1">
@@ -7881,48 +7879,49 @@
         <v>21875000.000000004</v>
       </c>
       <c r="J33" s="61" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K33" s="61">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="L33" s="75">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="61" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C34" s="61" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D34" s="26">
         <v>2050</v>
       </c>
-      <c r="E34" s="26" t="s">
-        <v>311</v>
+      <c r="E34" s="61" t="s">
+        <v>66</v>
       </c>
       <c r="F34" s="61" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G34" s="61">
-        <v>2019</v>
-      </c>
-      <c r="H34" s="20">
-        <v>2010</v>
-      </c>
-      <c r="I34" s="76">
-        <v>3734024</v>
+        <v>2020</v>
+      </c>
+      <c r="H34" s="61">
+        <v>1990</v>
+      </c>
+      <c r="I34" s="61">
+        <f>7000000/(1-0.68)</f>
+        <v>21875000.000000004</v>
       </c>
       <c r="J34" s="61" t="s">
-        <v>143</v>
+        <v>318</v>
       </c>
       <c r="K34" s="61">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="L34" s="75">
         <v>0.9</v>
@@ -7930,13 +7929,16 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="61" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C35" s="61" t="s">
-        <v>247</v>
+        <v>244</v>
+      </c>
+      <c r="D35" s="26">
+        <v>2050</v>
       </c>
       <c r="E35" s="26" t="s">
         <v>311</v>
@@ -7945,22 +7947,22 @@
         <v>310</v>
       </c>
       <c r="G35" s="61">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="H35" s="20">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="I35" s="76">
-        <v>21445571</v>
+        <v>3734024</v>
       </c>
       <c r="J35" s="61" t="s">
         <v>143</v>
       </c>
       <c r="K35" s="61">
-        <v>2030</v>
+        <v>2045</v>
       </c>
       <c r="L35" s="75">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -7992,83 +7994,80 @@
         <v>143</v>
       </c>
       <c r="K36" s="61">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="L36" s="75">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="61" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C37" s="61" t="s">
-        <v>253</v>
-      </c>
-      <c r="D37" s="26">
-        <v>2045</v>
+        <v>247</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F37" s="61" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G37" s="61">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="H37" s="20">
-        <v>2016</v>
-      </c>
-      <c r="I37" s="2">
-        <v>2.2165439930000002</v>
+        <v>2005</v>
+      </c>
+      <c r="I37" s="76">
+        <v>21445571</v>
       </c>
       <c r="J37" s="61" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="K37" s="61">
-        <v>2045</v>
+        <v>2050</v>
       </c>
       <c r="L37" s="75">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="61" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C38" s="61" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D38" s="26">
-        <v>2040</v>
+        <v>2045</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>311</v>
       </c>
       <c r="F38" s="61" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="G38" s="61">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="H38" s="20">
-        <v>2005</v>
-      </c>
-      <c r="I38" s="86">
-        <v>6976930.1319702603</v>
+        <v>2016</v>
+      </c>
+      <c r="I38" s="2">
+        <v>2.2165439930000002</v>
       </c>
       <c r="J38" s="61" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="K38" s="61">
-        <v>2040</v>
+        <v>2045</v>
       </c>
       <c r="L38" s="75">
         <v>1</v>
@@ -8076,40 +8075,40 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="61" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C39" s="61" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D39" s="26">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>66</v>
+        <v>311</v>
       </c>
       <c r="F39" s="61" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G39" s="61">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="H39" s="20">
-        <v>2017</v>
-      </c>
-      <c r="I39" s="61">
-        <v>2.06</v>
+        <v>2005</v>
+      </c>
+      <c r="I39" s="86">
+        <v>6976930.1319702603</v>
       </c>
       <c r="J39" s="61" t="s">
-        <v>317</v>
+        <v>143</v>
       </c>
       <c r="K39" s="61">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="L39" s="75">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -8144,14 +8143,49 @@
         <v>317</v>
       </c>
       <c r="K40" s="61">
+        <v>2030</v>
+      </c>
+      <c r="L40" s="75">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C41" s="61" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" s="26">
+        <v>2050</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="G41" s="61">
+        <v>2020</v>
+      </c>
+      <c r="H41" s="20">
+        <v>2017</v>
+      </c>
+      <c r="I41" s="61">
+        <v>2.06</v>
+      </c>
+      <c r="J41" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="K41" s="61">
         <v>2040</v>
       </c>
-      <c r="L40" s="75">
+      <c r="L41" s="75">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="I41" s="76"/>
     </row>
     <row r="42" spans="1:12">
       <c r="I42" s="76"/>

</xml_diff>

<commit_message>
Added handlers for S1 and S2 targets
Many companies report S1-only targets.  We should handle that, and translate to S1S2 according to methodology.
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B4F718-FE1C-D34E-BE12-B870CDD66632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E629529-ED6D-C042-A24F-B5BEF973FD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35920" yWindow="2620" windowWidth="68100" windowHeight="39960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64520" yWindow="2620" windowWidth="39500" windowHeight="39960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -3050,10 +3050,10 @@
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X30" sqref="X30:AK30"/>
+      <selection pane="bottomRight" activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -6827,7 +6827,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Generate target projections for S1 and S2 scopes individually
Provide target projections based on S1 and S2 scopes, not only S1S2.  Also fix base year data exclusion bug (we don't have to abandon projection if base year == last_year).

Also, simplify input data as we have not yet implemented  everything described in https://github.com/os-climate/ITR/issues/32

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E629529-ED6D-C042-A24F-B5BEF973FD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED996875-A1FE-4F45-9E9F-1A83EA7FEC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64520" yWindow="2620" windowWidth="39500" windowHeight="39960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55420" yWindow="2620" windowWidth="48600" windowHeight="39960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -1322,7 +1322,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1501,11 +1501,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="ArialMT"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1640,7 +1635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1795,8 +1790,7 @@
     </xf>
     <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3050,10 +3044,10 @@
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB19" sqref="AB19"/>
+      <selection pane="bottomRight" activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -4449,24 +4443,19 @@
       <c r="P13" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="AE13" s="69">
+      <c r="Q13" s="2">
         <v>1.325786621</v>
       </c>
-      <c r="AF13" s="69">
+      <c r="R13" s="2">
         <v>1.323738978</v>
       </c>
-      <c r="AG13" s="69">
+      <c r="S13" s="2">
         <v>1.2685339369999999</v>
       </c>
-      <c r="AH13" s="69">
+      <c r="T13" s="2">
         <v>1.202690405</v>
       </c>
-      <c r="AI13" s="69">
+      <c r="U13" s="2">
         <v>1.145419433</v>
       </c>
       <c r="AS13" s="61">
@@ -4535,24 +4524,19 @@
       <c r="P14" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="AE14" s="69">
+      <c r="Q14" s="2">
         <v>26.796145450000001</v>
       </c>
-      <c r="AF14" s="69">
+      <c r="R14" s="2">
         <v>27.947696990000001</v>
       </c>
-      <c r="AG14" s="69">
+      <c r="S14" s="2">
         <v>29.95633261</v>
       </c>
-      <c r="AH14" s="69">
+      <c r="T14" s="2">
         <v>27.00027425</v>
       </c>
-      <c r="AI14" s="69">
+      <c r="U14" s="2">
         <v>26.48364437</v>
       </c>
       <c r="AS14" s="61">
@@ -4721,24 +4705,19 @@
       <c r="P16" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="AE16" s="69">
+      <c r="Q16" s="2">
         <v>94.923459879999996</v>
       </c>
-      <c r="AF16" s="69">
+      <c r="R16" s="2">
         <v>93.530450478000006</v>
       </c>
-      <c r="AG16" s="69">
+      <c r="S16" s="2">
         <v>95.012237693000003</v>
       </c>
-      <c r="AH16" s="69">
+      <c r="T16" s="2">
         <v>83.595723118999999</v>
       </c>
-      <c r="AI16" s="69">
+      <c r="U16" s="2">
         <v>82.018839239000002</v>
       </c>
       <c r="AS16" s="61">
@@ -4807,23 +4786,19 @@
       <c r="P17" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
+      <c r="Q17" s="2">
+        <v>32.516193991999998</v>
+      </c>
+      <c r="R17" s="2">
+        <v>31.450986952000001</v>
+      </c>
+      <c r="S17" s="2">
+        <v>34.631975513</v>
+      </c>
+      <c r="T17" s="2">
+        <v>33.246229124999999</v>
+      </c>
       <c r="U17" s="2"/>
-      <c r="AE17" s="69">
-        <v>32.516193991999998</v>
-      </c>
-      <c r="AF17" s="69">
-        <v>31.450986952000001</v>
-      </c>
-      <c r="AG17" s="69">
-        <v>34.631975513</v>
-      </c>
-      <c r="AH17" s="69">
-        <v>33.246229124999999</v>
-      </c>
       <c r="AS17" s="61">
         <v>102.999524264</v>
       </c>
@@ -4890,25 +4865,63 @@
       <c r="P18" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
+      <c r="Q18" s="2">
+        <v>35.122915438000007</v>
+      </c>
+      <c r="R18" s="2">
+        <v>32.270565695999998</v>
+      </c>
+      <c r="S18" s="2">
+        <v>28.483757178000001</v>
+      </c>
+      <c r="T18" s="2">
+        <v>26.74941115</v>
+      </c>
+      <c r="U18" s="2">
+        <v>35.013482494000002</v>
+      </c>
+      <c r="X18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>0</v>
+      </c>
       <c r="AE18" s="69">
+        <f t="shared" ref="AE18" si="14">IF(OR(ISBLANK(Q18), ISBLANK(X18)),"",Q18+X18)</f>
         <v>35.122915438000007</v>
       </c>
       <c r="AF18" s="69">
+        <f t="shared" ref="AF18" si="15">IF(OR(ISBLANK(R18), ISBLANK(Y18)),"",R18+Y18)</f>
         <v>32.270565695999998</v>
       </c>
       <c r="AG18" s="69">
+        <f t="shared" ref="AG18" si="16">IF(OR(ISBLANK(S18), ISBLANK(Z18)),"",S18+Z18)</f>
         <v>28.483757178000001</v>
       </c>
       <c r="AH18" s="69">
+        <f t="shared" ref="AH18" si="17">IF(OR(ISBLANK(T18), ISBLANK(AA18)),"",T18+AA18)</f>
         <v>26.74941115</v>
       </c>
       <c r="AI18" s="69">
+        <f t="shared" ref="AI18" si="18">IF(OR(ISBLANK(U18), ISBLANK(AB18)),"",U18+AB18)</f>
         <v>35.013482494000002</v>
+      </c>
+      <c r="AJ18" s="69" t="str">
+        <f t="shared" ref="AJ18" si="19">IF(OR(ISBLANK(V18), ISBLANK(AC18)),"",V18+AC18)</f>
+        <v/>
+      </c>
+      <c r="AK18" s="69" t="str">
+        <f t="shared" ref="AK18" si="20">IF(OR(ISBLANK(W18), ISBLANK(AD18)),"",W18+AD18)</f>
+        <v/>
       </c>
       <c r="AS18" s="61">
         <v>47.465894990000002</v>
@@ -4976,25 +4989,20 @@
       <c r="P19" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="AE19" s="69">
+      <c r="Q19" s="2">
         <v>0.54127069000000005</v>
       </c>
-      <c r="AF19" s="69">
+      <c r="R19" s="2">
         <v>0.38852905199999999</v>
       </c>
-      <c r="AG19" s="69">
+      <c r="S19" s="2">
         <v>3.4941450000000002E-3</v>
       </c>
-      <c r="AH19" s="69">
+      <c r="T19" s="2">
         <v>2.2128600000000001E-4</v>
       </c>
-      <c r="AI19" s="69">
-        <f>AH19</f>
+      <c r="U19" s="2">
+        <f>T19</f>
         <v>2.2128600000000001E-4</v>
       </c>
       <c r="AS19" s="61">
@@ -5065,31 +5073,31 @@
       <c r="Q20" s="2">
         <v>9723000</v>
       </c>
-      <c r="R20" s="84">
+      <c r="R20" s="83">
         <v>9532000</v>
       </c>
-      <c r="S20" s="84">
+      <c r="S20" s="83">
         <v>8841000</v>
       </c>
-      <c r="T20" s="84">
+      <c r="T20" s="83">
         <v>8566000</v>
       </c>
-      <c r="U20" s="87">
+      <c r="U20" s="86">
         <v>8493000</v>
       </c>
       <c r="X20" s="2">
         <v>7061000</v>
       </c>
-      <c r="Y20" s="84">
+      <c r="Y20" s="83">
         <v>17693000</v>
       </c>
-      <c r="Z20" s="84">
+      <c r="Z20" s="83">
         <v>21022000</v>
       </c>
-      <c r="AA20" s="84">
+      <c r="AA20" s="83">
         <v>18864000</v>
       </c>
-      <c r="AB20" s="87">
+      <c r="AB20" s="86">
         <v>13720000</v>
       </c>
       <c r="AE20" s="69">
@@ -5097,41 +5105,41 @@
         <v>16784000</v>
       </c>
       <c r="AF20" s="69">
-        <f t="shared" ref="AF20" si="14">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
+        <f t="shared" ref="AF20" si="21">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
         <v>27225000</v>
       </c>
       <c r="AG20" s="69">
-        <f t="shared" ref="AG20" si="15">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
+        <f t="shared" ref="AG20" si="22">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
         <v>29863000</v>
       </c>
       <c r="AH20" s="69">
-        <f t="shared" ref="AH20" si="16">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
+        <f t="shared" ref="AH20" si="23">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
         <v>27430000</v>
       </c>
       <c r="AI20" s="69">
-        <f t="shared" ref="AI20" si="17">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
+        <f t="shared" ref="AI20" si="24">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
         <v>22213000</v>
       </c>
       <c r="AJ20" s="69" t="str">
-        <f t="shared" ref="AJ20" si="18">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
+        <f t="shared" ref="AJ20" si="25">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
         <v/>
       </c>
       <c r="AK20" s="69" t="str">
-        <f t="shared" ref="AK20" si="19">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
+        <f t="shared" ref="AK20" si="26">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
         <v/>
       </c>
       <c r="AS20" s="76">
         <v>186212000</v>
       </c>
-      <c r="AT20" s="83">
+      <c r="AT20" s="82">
         <f>195307000+51595000</f>
         <v>246902000</v>
       </c>
-      <c r="AU20" s="84">
+      <c r="AU20" s="83">
         <f>194224000+59050000</f>
         <v>253274000</v>
       </c>
-      <c r="AV20" s="85">
+      <c r="AV20" s="84">
         <f>189463000+69708000</f>
         <v>259171000</v>
       </c>
@@ -5218,27 +5226,27 @@
         <v/>
       </c>
       <c r="AF21" s="69">
-        <f t="shared" ref="AF21" si="20">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
+        <f t="shared" ref="AF21" si="27">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
         <v>60434671</v>
       </c>
       <c r="AG21" s="69">
-        <f t="shared" ref="AG21" si="21">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
+        <f t="shared" ref="AG21" si="28">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
         <v>52972697</v>
       </c>
       <c r="AH21" s="69">
-        <f t="shared" ref="AH21" si="22">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
+        <f t="shared" ref="AH21" si="29">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
         <v>49863111</v>
       </c>
       <c r="AI21" s="69">
-        <f t="shared" ref="AI21" si="23">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
+        <f t="shared" ref="AI21" si="30">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
         <v>42750225</v>
       </c>
       <c r="AJ21" s="69" t="str">
-        <f t="shared" ref="AJ21" si="24">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
+        <f t="shared" ref="AJ21" si="31">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
         <v/>
       </c>
       <c r="AK21" s="69" t="str">
-        <f t="shared" ref="AK21" si="25">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
+        <f t="shared" ref="AK21" si="32">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
         <v/>
       </c>
       <c r="AS21" s="61"/>
@@ -5332,31 +5340,31 @@
         <v>2487000</v>
       </c>
       <c r="AE22" s="69">
-        <f t="shared" ref="AE22:AK22" si="26">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
+        <f t="shared" ref="AE22:AK22" si="33">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
         <v>14435000</v>
       </c>
       <c r="AF22" s="69">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>13858000</v>
       </c>
       <c r="AG22" s="69">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>13933000</v>
       </c>
       <c r="AH22" s="69">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>14858000</v>
       </c>
       <c r="AI22" s="69">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v>12580000</v>
       </c>
       <c r="AJ22" s="69" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AK22" s="69" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AS22" s="61">
@@ -5423,24 +5431,19 @@
       <c r="P23" s="61" t="s">
         <v>321</v>
       </c>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="AE23" s="69">
+      <c r="Q23" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="AF23" s="69">
+      <c r="R23" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="AG23" s="69">
+      <c r="S23" s="2">
         <v>14.27265885416667</v>
       </c>
-      <c r="AH23" s="69">
+      <c r="T23" s="2">
         <v>11.947505</v>
       </c>
-      <c r="AI23" s="69">
+      <c r="U23" s="2">
         <v>11.738147617323991</v>
       </c>
       <c r="AS23" s="61">
@@ -5539,31 +5542,31 @@
         <v>0</v>
       </c>
       <c r="AE24" s="69">
-        <f t="shared" ref="AE24" si="27">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
+        <f t="shared" ref="AE24" si="34">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
         <v>3.8868941879999999</v>
       </c>
       <c r="AF24" s="69">
-        <f t="shared" ref="AF24" si="28">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
+        <f t="shared" ref="AF24" si="35">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
         <v>3.8663196809999998</v>
       </c>
       <c r="AG24" s="69">
-        <f t="shared" ref="AG24" si="29">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
+        <f t="shared" ref="AG24" si="36">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
         <v>3.937301664</v>
       </c>
       <c r="AH24" s="69">
-        <f t="shared" ref="AH24" si="30">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
+        <f t="shared" ref="AH24" si="37">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
         <v>3.9790181429999998</v>
       </c>
       <c r="AI24" s="69">
-        <f t="shared" ref="AI24" si="31">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
+        <f t="shared" ref="AI24" si="38">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
         <v>3.8259789839999998</v>
       </c>
       <c r="AJ24" s="69" t="str">
-        <f t="shared" ref="AJ24" si="32">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
+        <f t="shared" ref="AJ24" si="39">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
         <v/>
       </c>
       <c r="AK24" s="69" t="str">
-        <f t="shared" ref="AK24" si="33">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
+        <f t="shared" ref="AK24" si="40">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
         <v/>
       </c>
       <c r="AS24" s="61">
@@ -5631,26 +5634,64 @@
       <c r="P25" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
+      <c r="Q25" s="2">
+        <v>1.8746218750000001</v>
+      </c>
+      <c r="R25" s="2">
+        <v>1.844359927</v>
+      </c>
+      <c r="S25" s="2">
+        <v>2.051568649</v>
+      </c>
+      <c r="T25" s="2">
+        <v>1.710493431</v>
+      </c>
+      <c r="U25" s="2">
+        <f>T25*2.26/2.35</f>
+        <v>1.6449851719404254</v>
+      </c>
+      <c r="X25" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>0</v>
+      </c>
       <c r="AE25" s="69">
+        <f t="shared" ref="AE25:AE27" si="41">IF(OR(ISBLANK(Q25), ISBLANK(X25)),"",Q25+X25)</f>
         <v>1.8746218750000001</v>
       </c>
       <c r="AF25" s="69">
+        <f t="shared" ref="AF25:AF27" si="42">IF(OR(ISBLANK(R25), ISBLANK(Y25)),"",R25+Y25)</f>
         <v>1.844359927</v>
       </c>
       <c r="AG25" s="69">
+        <f t="shared" ref="AG25:AG27" si="43">IF(OR(ISBLANK(S25), ISBLANK(Z25)),"",S25+Z25)</f>
         <v>2.051568649</v>
       </c>
       <c r="AH25" s="69">
+        <f t="shared" ref="AH25:AH27" si="44">IF(OR(ISBLANK(T25), ISBLANK(AA25)),"",T25+AA25)</f>
         <v>1.710493431</v>
       </c>
       <c r="AI25" s="69">
-        <f>AH25*2.26/2.35</f>
+        <f t="shared" ref="AI25:AI27" si="45">IF(OR(ISBLANK(U25), ISBLANK(AB25)),"",U25+AB25)</f>
         <v>1.6449851719404254</v>
+      </c>
+      <c r="AJ25" s="69" t="str">
+        <f t="shared" ref="AJ25:AJ27" si="46">IF(OR(ISBLANK(V25), ISBLANK(AC25)),"",V25+AC25)</f>
+        <v/>
+      </c>
+      <c r="AK25" s="69" t="str">
+        <f t="shared" ref="AK25:AK27" si="47">IF(OR(ISBLANK(W25), ISBLANK(AD25)),"",W25+AD25)</f>
+        <v/>
       </c>
       <c r="AS25" s="61">
         <v>3.1870937499999998</v>
@@ -5717,25 +5758,63 @@
       <c r="P26" s="61" t="s">
         <v>321</v>
       </c>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
+      <c r="Q26" s="2">
+        <v>12.356382978723399</v>
+      </c>
+      <c r="R26" s="2">
+        <v>11.819148936170221</v>
+      </c>
+      <c r="S26" s="2">
+        <v>11.281914893617021</v>
+      </c>
+      <c r="T26" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="U26" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="X26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>0</v>
+      </c>
       <c r="AE26" s="69">
+        <f t="shared" si="41"/>
         <v>12.356382978723399</v>
       </c>
       <c r="AF26" s="69">
+        <f t="shared" si="42"/>
         <v>11.819148936170221</v>
       </c>
       <c r="AG26" s="69">
+        <f t="shared" si="43"/>
         <v>11.281914893617021</v>
       </c>
       <c r="AH26" s="69">
+        <f t="shared" si="44"/>
         <v>10.1</v>
       </c>
       <c r="AI26" s="69">
+        <f t="shared" si="45"/>
         <v>10.1</v>
+      </c>
+      <c r="AJ26" s="69" t="str">
+        <f t="shared" si="46"/>
+        <v/>
+      </c>
+      <c r="AK26" s="69" t="str">
+        <f t="shared" si="47"/>
+        <v/>
       </c>
       <c r="AS26" s="61">
         <v>21.48936170212766</v>
@@ -5798,25 +5877,63 @@
       <c r="P27" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
+      <c r="Q27" s="2">
+        <v>3.004725724</v>
+      </c>
+      <c r="R27" s="2">
+        <v>2.1325357700000001</v>
+      </c>
+      <c r="S27" s="2">
+        <v>3.0720788620000001</v>
+      </c>
+      <c r="T27" s="2">
+        <v>2.4277569909999999</v>
+      </c>
+      <c r="U27" s="2">
+        <v>1.335266345</v>
+      </c>
+      <c r="X27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>0</v>
+      </c>
       <c r="AE27" s="69">
+        <f t="shared" si="41"/>
         <v>3.004725724</v>
       </c>
       <c r="AF27" s="69">
+        <f t="shared" si="42"/>
         <v>2.1325357700000001</v>
       </c>
       <c r="AG27" s="69">
+        <f t="shared" si="43"/>
         <v>3.0720788620000001</v>
       </c>
       <c r="AH27" s="69">
+        <f t="shared" si="44"/>
         <v>2.4277569909999999</v>
       </c>
       <c r="AI27" s="69">
+        <f t="shared" si="45"/>
         <v>1.335266345</v>
+      </c>
+      <c r="AJ27" s="69" t="str">
+        <f t="shared" si="46"/>
+        <v/>
+      </c>
+      <c r="AK27" s="69" t="str">
+        <f t="shared" si="47"/>
+        <v/>
       </c>
       <c r="AS27" s="61">
         <v>4.836665</v>
@@ -5914,31 +6031,31 @@
         <v>0</v>
       </c>
       <c r="AE28" s="69">
-        <f t="shared" ref="AE28" si="34">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
+        <f t="shared" ref="AE28" si="48">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
         <v>0.99625009600000003</v>
       </c>
       <c r="AF28" s="69">
-        <f t="shared" ref="AF28" si="35">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
+        <f t="shared" ref="AF28" si="49">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
         <v>0.98354598199999999</v>
       </c>
       <c r="AG28" s="69">
-        <f t="shared" ref="AG28" si="36">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
+        <f t="shared" ref="AG28" si="50">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
         <v>2.6019487300000002</v>
       </c>
       <c r="AH28" s="69">
-        <f t="shared" ref="AH28" si="37">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
+        <f t="shared" ref="AH28" si="51">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
         <v>2.5352979329999998</v>
       </c>
       <c r="AI28" s="69">
-        <f t="shared" ref="AI28" si="38">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
+        <f t="shared" ref="AI28" si="52">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
         <v>1.926808946</v>
       </c>
       <c r="AJ28" s="69" t="str">
-        <f t="shared" ref="AJ28" si="39">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
+        <f t="shared" ref="AJ28" si="53">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
         <v/>
       </c>
       <c r="AK28" s="69" t="str">
-        <f t="shared" ref="AK28" si="40">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
+        <f t="shared" ref="AK28" si="54">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
         <v/>
       </c>
       <c r="AS28" s="61">
@@ -6033,31 +6150,31 @@
         <v>6063090</v>
       </c>
       <c r="AE29" s="69">
-        <f t="shared" ref="AE29:AE30" si="41">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
+        <f t="shared" ref="AE29:AE30" si="55">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
         <v>33167324</v>
       </c>
       <c r="AF29" s="69">
-        <f t="shared" ref="AF29:AF30" si="42">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
+        <f t="shared" ref="AF29:AF30" si="56">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
         <v>36362250</v>
       </c>
       <c r="AG29" s="69">
-        <f t="shared" ref="AG29:AG30" si="43">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
+        <f t="shared" ref="AG29:AG30" si="57">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
         <v>35896971</v>
       </c>
       <c r="AH29" s="69">
-        <f t="shared" ref="AH29:AH30" si="44">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
+        <f t="shared" ref="AH29:AH30" si="58">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
         <v>30327168</v>
       </c>
       <c r="AI29" s="69">
-        <f t="shared" ref="AI29:AI30" si="45">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
+        <f t="shared" ref="AI29:AI30" si="59">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
         <v>31822330</v>
       </c>
       <c r="AJ29" s="69" t="str">
-        <f t="shared" ref="AJ29:AJ30" si="46">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
+        <f t="shared" ref="AJ29:AJ30" si="60">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
         <v/>
       </c>
       <c r="AK29" s="69" t="str">
-        <f t="shared" ref="AK29:AK30" si="47">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
+        <f t="shared" ref="AK29:AK30" si="61">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
         <v/>
       </c>
       <c r="AS29" s="1">
@@ -6161,31 +6278,31 @@
         <v>0</v>
       </c>
       <c r="AE30" s="69">
-        <f t="shared" si="41"/>
+        <f t="shared" si="55"/>
         <v>2.2165439930000002</v>
       </c>
       <c r="AF30" s="69">
-        <f t="shared" si="42"/>
+        <f t="shared" si="56"/>
         <v>2.2511915660000001</v>
       </c>
       <c r="AG30" s="69">
-        <f t="shared" si="43"/>
+        <f t="shared" si="57"/>
         <v>2.4511497719999999</v>
       </c>
       <c r="AH30" s="69">
-        <f t="shared" si="44"/>
+        <f t="shared" si="58"/>
         <v>2.4417731950000001</v>
       </c>
       <c r="AI30" s="69">
-        <f t="shared" si="45"/>
+        <f t="shared" si="59"/>
         <v>2.3478588409999999</v>
       </c>
       <c r="AJ30" s="69" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="60"/>
         <v/>
       </c>
       <c r="AK30" s="69" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="61"/>
         <v/>
       </c>
       <c r="AS30" s="61">
@@ -6253,24 +6370,19 @@
       <c r="P31" s="68" t="s">
         <v>319</v>
       </c>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="AE31" s="69">
+      <c r="Q31" s="2">
         <v>6.3372507860000002</v>
       </c>
-      <c r="AF31" s="69">
+      <c r="R31" s="2">
         <v>6.1180013459999998</v>
       </c>
-      <c r="AG31" s="69">
+      <c r="S31" s="2">
         <v>5.2178957580000001</v>
       </c>
-      <c r="AH31" s="69">
+      <c r="T31" s="2">
         <v>5.3678279890000002</v>
       </c>
-      <c r="AI31" s="69">
+      <c r="U31" s="2">
         <v>5.0787910969999999</v>
       </c>
       <c r="AS31" s="61">
@@ -6333,21 +6445,16 @@
         <v>321</v>
       </c>
       <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="AE32" s="69"/>
-      <c r="AF32" s="69">
+      <c r="R32" s="2">
         <v>78.8</v>
       </c>
-      <c r="AG32" s="69">
+      <c r="S32" s="2">
         <v>78.8</v>
       </c>
-      <c r="AH32" s="69">
+      <c r="T32" s="2">
         <v>78.8</v>
       </c>
-      <c r="AI32" s="69">
+      <c r="U32" s="2">
         <v>68.873999999999995</v>
       </c>
       <c r="AS32" s="61"/>
@@ -6824,10 +6931,10 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7321,7 +7428,7 @@
         <v>311</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G14" s="61">
         <v>2020</v>
@@ -8237,7 +8344,7 @@
       <c r="H39" s="20">
         <v>2005</v>
       </c>
-      <c r="I39" s="86">
+      <c r="I39" s="85">
         <v>6976930.1319702603</v>
       </c>
       <c r="J39" s="61" t="s">

</xml_diff>

<commit_message>
Test cases can now run with Sample data.
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED996875-A1FE-4F45-9E9F-1A83EA7FEC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5CB5E5-D0D1-2245-AC30-C348D7921DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55420" yWindow="2620" windowWidth="48600" windowHeight="39960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55420" yWindow="2620" windowWidth="48600" windowHeight="39960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -216,6 +216,219 @@
         </r>
       </text>
     </comment>
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CBCC6D2D-3589-F54A-A3D8-C85B5415A3A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{E1E20C21-AC41-454F-BD00-E2E3A76147CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{D7FC3687-67D6-B94A-81A4-A3F0B5E62612}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{D6EF40F2-AAE1-0D4C-AB96-6234B272A95B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{3621CB18-1100-1A47-8F98-EC355E02058C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1322,7 +1535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1504,6 +1717,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -3043,11 +3263,11 @@
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X30" sqref="X30"/>
+      <selection pane="bottomRight" activeCell="AX26" sqref="AX26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -5005,6 +5225,49 @@
         <f>T19</f>
         <v>2.2128600000000001E-4</v>
       </c>
+      <c r="X19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="69">
+        <f t="shared" ref="AE19" si="21">IF(OR(ISBLANK(Q19), ISBLANK(X19)),"",Q19+X19)</f>
+        <v>0.54127069000000005</v>
+      </c>
+      <c r="AF19" s="69">
+        <f t="shared" ref="AF19" si="22">IF(OR(ISBLANK(R19), ISBLANK(Y19)),"",R19+Y19)</f>
+        <v>0.38852905199999999</v>
+      </c>
+      <c r="AG19" s="69">
+        <f t="shared" ref="AG19" si="23">IF(OR(ISBLANK(S19), ISBLANK(Z19)),"",S19+Z19)</f>
+        <v>3.4941450000000002E-3</v>
+      </c>
+      <c r="AH19" s="69">
+        <f t="shared" ref="AH19" si="24">IF(OR(ISBLANK(T19), ISBLANK(AA19)),"",T19+AA19)</f>
+        <v>2.2128600000000001E-4</v>
+      </c>
+      <c r="AI19" s="69">
+        <f t="shared" ref="AI19" si="25">IF(OR(ISBLANK(U19), ISBLANK(AB19)),"",U19+AB19)</f>
+        <v>2.2128600000000001E-4</v>
+      </c>
+      <c r="AJ19" s="69" t="str">
+        <f t="shared" ref="AJ19" si="26">IF(OR(ISBLANK(V19), ISBLANK(AC19)),"",V19+AC19)</f>
+        <v/>
+      </c>
+      <c r="AK19" s="69" t="str">
+        <f t="shared" ref="AK19" si="27">IF(OR(ISBLANK(W19), ISBLANK(AD19)),"",W19+AD19)</f>
+        <v/>
+      </c>
       <c r="AS19" s="61">
         <v>1.080058642</v>
       </c>
@@ -5105,27 +5368,27 @@
         <v>16784000</v>
       </c>
       <c r="AF20" s="69">
-        <f t="shared" ref="AF20" si="21">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
+        <f t="shared" ref="AF20" si="28">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
         <v>27225000</v>
       </c>
       <c r="AG20" s="69">
-        <f t="shared" ref="AG20" si="22">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
+        <f t="shared" ref="AG20" si="29">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
         <v>29863000</v>
       </c>
       <c r="AH20" s="69">
-        <f t="shared" ref="AH20" si="23">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
+        <f t="shared" ref="AH20" si="30">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
         <v>27430000</v>
       </c>
       <c r="AI20" s="69">
-        <f t="shared" ref="AI20" si="24">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
+        <f t="shared" ref="AI20" si="31">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
         <v>22213000</v>
       </c>
       <c r="AJ20" s="69" t="str">
-        <f t="shared" ref="AJ20" si="25">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
+        <f t="shared" ref="AJ20" si="32">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
         <v/>
       </c>
       <c r="AK20" s="69" t="str">
-        <f t="shared" ref="AK20" si="26">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
+        <f t="shared" ref="AK20" si="33">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
         <v/>
       </c>
       <c r="AS20" s="76">
@@ -5226,27 +5489,27 @@
         <v/>
       </c>
       <c r="AF21" s="69">
-        <f t="shared" ref="AF21" si="27">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
+        <f t="shared" ref="AF21" si="34">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
         <v>60434671</v>
       </c>
       <c r="AG21" s="69">
-        <f t="shared" ref="AG21" si="28">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
+        <f t="shared" ref="AG21" si="35">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
         <v>52972697</v>
       </c>
       <c r="AH21" s="69">
-        <f t="shared" ref="AH21" si="29">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
+        <f t="shared" ref="AH21" si="36">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
         <v>49863111</v>
       </c>
       <c r="AI21" s="69">
-        <f t="shared" ref="AI21" si="30">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
+        <f t="shared" ref="AI21" si="37">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
         <v>42750225</v>
       </c>
       <c r="AJ21" s="69" t="str">
-        <f t="shared" ref="AJ21" si="31">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
+        <f t="shared" ref="AJ21" si="38">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
         <v/>
       </c>
       <c r="AK21" s="69" t="str">
-        <f t="shared" ref="AK21" si="32">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
+        <f t="shared" ref="AK21" si="39">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
         <v/>
       </c>
       <c r="AS21" s="61"/>
@@ -5340,31 +5603,31 @@
         <v>2487000</v>
       </c>
       <c r="AE22" s="69">
-        <f t="shared" ref="AE22:AK22" si="33">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
+        <f t="shared" ref="AE22:AK23" si="40">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
         <v>14435000</v>
       </c>
       <c r="AF22" s="69">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>13858000</v>
       </c>
       <c r="AG22" s="69">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>13933000</v>
       </c>
       <c r="AH22" s="69">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>14858000</v>
       </c>
       <c r="AI22" s="69">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v>12580000</v>
       </c>
       <c r="AJ22" s="69" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AK22" s="69" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AS22" s="61">
@@ -5446,6 +5709,49 @@
       <c r="U23" s="2">
         <v>11.738147617323991</v>
       </c>
+      <c r="X23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="69">
+        <f t="shared" si="40"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="AF23" s="69">
+        <f t="shared" si="40"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="AG23" s="69">
+        <f t="shared" si="40"/>
+        <v>14.27265885416667</v>
+      </c>
+      <c r="AH23" s="69">
+        <f t="shared" si="40"/>
+        <v>11.947505</v>
+      </c>
+      <c r="AI23" s="69">
+        <f t="shared" si="40"/>
+        <v>11.738147617323991</v>
+      </c>
+      <c r="AJ23" s="69" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AK23" s="69" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
       <c r="AS23" s="61">
         <v>16.100000000000001</v>
       </c>
@@ -5542,31 +5848,31 @@
         <v>0</v>
       </c>
       <c r="AE24" s="69">
-        <f t="shared" ref="AE24" si="34">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
+        <f t="shared" ref="AE24" si="41">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
         <v>3.8868941879999999</v>
       </c>
       <c r="AF24" s="69">
-        <f t="shared" ref="AF24" si="35">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
+        <f t="shared" ref="AF24" si="42">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
         <v>3.8663196809999998</v>
       </c>
       <c r="AG24" s="69">
-        <f t="shared" ref="AG24" si="36">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
+        <f t="shared" ref="AG24" si="43">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
         <v>3.937301664</v>
       </c>
       <c r="AH24" s="69">
-        <f t="shared" ref="AH24" si="37">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
+        <f t="shared" ref="AH24" si="44">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
         <v>3.9790181429999998</v>
       </c>
       <c r="AI24" s="69">
-        <f t="shared" ref="AI24" si="38">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
+        <f t="shared" ref="AI24" si="45">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
         <v>3.8259789839999998</v>
       </c>
       <c r="AJ24" s="69" t="str">
-        <f t="shared" ref="AJ24" si="39">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
+        <f t="shared" ref="AJ24" si="46">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
         <v/>
       </c>
       <c r="AK24" s="69" t="str">
-        <f t="shared" ref="AK24" si="40">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
+        <f t="shared" ref="AK24" si="47">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
         <v/>
       </c>
       <c r="AS24" s="61">
@@ -5666,31 +5972,31 @@
         <v>0</v>
       </c>
       <c r="AE25" s="69">
-        <f t="shared" ref="AE25:AE27" si="41">IF(OR(ISBLANK(Q25), ISBLANK(X25)),"",Q25+X25)</f>
+        <f t="shared" ref="AE25:AE27" si="48">IF(OR(ISBLANK(Q25), ISBLANK(X25)),"",Q25+X25)</f>
         <v>1.8746218750000001</v>
       </c>
       <c r="AF25" s="69">
-        <f t="shared" ref="AF25:AF27" si="42">IF(OR(ISBLANK(R25), ISBLANK(Y25)),"",R25+Y25)</f>
+        <f t="shared" ref="AF25:AF27" si="49">IF(OR(ISBLANK(R25), ISBLANK(Y25)),"",R25+Y25)</f>
         <v>1.844359927</v>
       </c>
       <c r="AG25" s="69">
-        <f t="shared" ref="AG25:AG27" si="43">IF(OR(ISBLANK(S25), ISBLANK(Z25)),"",S25+Z25)</f>
+        <f t="shared" ref="AG25:AG27" si="50">IF(OR(ISBLANK(S25), ISBLANK(Z25)),"",S25+Z25)</f>
         <v>2.051568649</v>
       </c>
       <c r="AH25" s="69">
-        <f t="shared" ref="AH25:AH27" si="44">IF(OR(ISBLANK(T25), ISBLANK(AA25)),"",T25+AA25)</f>
+        <f t="shared" ref="AH25:AH27" si="51">IF(OR(ISBLANK(T25), ISBLANK(AA25)),"",T25+AA25)</f>
         <v>1.710493431</v>
       </c>
       <c r="AI25" s="69">
-        <f t="shared" ref="AI25:AI27" si="45">IF(OR(ISBLANK(U25), ISBLANK(AB25)),"",U25+AB25)</f>
+        <f t="shared" ref="AI25:AI27" si="52">IF(OR(ISBLANK(U25), ISBLANK(AB25)),"",U25+AB25)</f>
         <v>1.6449851719404254</v>
       </c>
       <c r="AJ25" s="69" t="str">
-        <f t="shared" ref="AJ25:AJ27" si="46">IF(OR(ISBLANK(V25), ISBLANK(AC25)),"",V25+AC25)</f>
+        <f t="shared" ref="AJ25:AJ27" si="53">IF(OR(ISBLANK(V25), ISBLANK(AC25)),"",V25+AC25)</f>
         <v/>
       </c>
       <c r="AK25" s="69" t="str">
-        <f t="shared" ref="AK25:AK27" si="47">IF(OR(ISBLANK(W25), ISBLANK(AD25)),"",W25+AD25)</f>
+        <f t="shared" ref="AK25:AK27" si="54">IF(OR(ISBLANK(W25), ISBLANK(AD25)),"",W25+AD25)</f>
         <v/>
       </c>
       <c r="AS25" s="61">
@@ -5789,31 +6095,31 @@
         <v>0</v>
       </c>
       <c r="AE26" s="69">
-        <f t="shared" si="41"/>
+        <f t="shared" si="48"/>
         <v>12.356382978723399</v>
       </c>
       <c r="AF26" s="69">
-        <f t="shared" si="42"/>
+        <f t="shared" si="49"/>
         <v>11.819148936170221</v>
       </c>
       <c r="AG26" s="69">
-        <f t="shared" si="43"/>
+        <f t="shared" si="50"/>
         <v>11.281914893617021</v>
       </c>
       <c r="AH26" s="69">
-        <f t="shared" si="44"/>
+        <f t="shared" si="51"/>
         <v>10.1</v>
       </c>
       <c r="AI26" s="69">
-        <f t="shared" si="45"/>
+        <f t="shared" si="52"/>
         <v>10.1</v>
       </c>
       <c r="AJ26" s="69" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AK26" s="69" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="AS26" s="61">
@@ -5908,31 +6214,31 @@
         <v>0</v>
       </c>
       <c r="AE27" s="69">
-        <f t="shared" si="41"/>
+        <f t="shared" si="48"/>
         <v>3.004725724</v>
       </c>
       <c r="AF27" s="69">
-        <f t="shared" si="42"/>
+        <f t="shared" si="49"/>
         <v>2.1325357700000001</v>
       </c>
       <c r="AG27" s="69">
-        <f t="shared" si="43"/>
+        <f t="shared" si="50"/>
         <v>3.0720788620000001</v>
       </c>
       <c r="AH27" s="69">
-        <f t="shared" si="44"/>
+        <f t="shared" si="51"/>
         <v>2.4277569909999999</v>
       </c>
       <c r="AI27" s="69">
-        <f t="shared" si="45"/>
+        <f t="shared" si="52"/>
         <v>1.335266345</v>
       </c>
       <c r="AJ27" s="69" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AK27" s="69" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="AS27" s="61">
@@ -6031,31 +6337,31 @@
         <v>0</v>
       </c>
       <c r="AE28" s="69">
-        <f t="shared" ref="AE28" si="48">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
+        <f t="shared" ref="AE28" si="55">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
         <v>0.99625009600000003</v>
       </c>
       <c r="AF28" s="69">
-        <f t="shared" ref="AF28" si="49">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
+        <f t="shared" ref="AF28" si="56">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
         <v>0.98354598199999999</v>
       </c>
       <c r="AG28" s="69">
-        <f t="shared" ref="AG28" si="50">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
+        <f t="shared" ref="AG28" si="57">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
         <v>2.6019487300000002</v>
       </c>
       <c r="AH28" s="69">
-        <f t="shared" ref="AH28" si="51">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
+        <f t="shared" ref="AH28" si="58">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
         <v>2.5352979329999998</v>
       </c>
       <c r="AI28" s="69">
-        <f t="shared" ref="AI28" si="52">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
+        <f t="shared" ref="AI28" si="59">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
         <v>1.926808946</v>
       </c>
       <c r="AJ28" s="69" t="str">
-        <f t="shared" ref="AJ28" si="53">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
+        <f t="shared" ref="AJ28" si="60">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
         <v/>
       </c>
       <c r="AK28" s="69" t="str">
-        <f t="shared" ref="AK28" si="54">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
+        <f t="shared" ref="AK28" si="61">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
         <v/>
       </c>
       <c r="AS28" s="61">
@@ -6150,31 +6456,31 @@
         <v>6063090</v>
       </c>
       <c r="AE29" s="69">
-        <f t="shared" ref="AE29:AE30" si="55">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
+        <f t="shared" ref="AE29:AE30" si="62">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
         <v>33167324</v>
       </c>
       <c r="AF29" s="69">
-        <f t="shared" ref="AF29:AF30" si="56">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
+        <f t="shared" ref="AF29:AF30" si="63">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
         <v>36362250</v>
       </c>
       <c r="AG29" s="69">
-        <f t="shared" ref="AG29:AG30" si="57">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
+        <f t="shared" ref="AG29:AG30" si="64">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
         <v>35896971</v>
       </c>
       <c r="AH29" s="69">
-        <f t="shared" ref="AH29:AH30" si="58">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
+        <f t="shared" ref="AH29:AH30" si="65">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
         <v>30327168</v>
       </c>
       <c r="AI29" s="69">
-        <f t="shared" ref="AI29:AI30" si="59">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
+        <f t="shared" ref="AI29:AI30" si="66">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
         <v>31822330</v>
       </c>
       <c r="AJ29" s="69" t="str">
-        <f t="shared" ref="AJ29:AJ30" si="60">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
+        <f t="shared" ref="AJ29:AJ30" si="67">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
         <v/>
       </c>
       <c r="AK29" s="69" t="str">
-        <f t="shared" ref="AK29:AK30" si="61">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
+        <f t="shared" ref="AK29:AK30" si="68">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
         <v/>
       </c>
       <c r="AS29" s="1">
@@ -6278,31 +6584,31 @@
         <v>0</v>
       </c>
       <c r="AE30" s="69">
-        <f t="shared" si="55"/>
+        <f t="shared" si="62"/>
         <v>2.2165439930000002</v>
       </c>
       <c r="AF30" s="69">
-        <f t="shared" si="56"/>
+        <f t="shared" si="63"/>
         <v>2.2511915660000001</v>
       </c>
       <c r="AG30" s="69">
-        <f t="shared" si="57"/>
+        <f t="shared" si="64"/>
         <v>2.4511497719999999</v>
       </c>
       <c r="AH30" s="69">
-        <f t="shared" si="58"/>
+        <f t="shared" si="65"/>
         <v>2.4417731950000001</v>
       </c>
       <c r="AI30" s="69">
-        <f t="shared" si="59"/>
+        <f t="shared" si="66"/>
         <v>2.3478588409999999</v>
       </c>
       <c r="AJ30" s="69" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
       <c r="AK30" s="69" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="68"/>
         <v/>
       </c>
       <c r="AS30" s="61">
@@ -6456,6 +6762,49 @@
       </c>
       <c r="U32" s="2">
         <v>68.873999999999995</v>
+      </c>
+      <c r="X32" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="69" t="str">
+        <f t="shared" ref="AE32" si="69">IF(OR(ISBLANK(Q32), ISBLANK(X32)),"",Q32+X32)</f>
+        <v/>
+      </c>
+      <c r="AF32" s="69">
+        <f t="shared" ref="AF32" si="70">IF(OR(ISBLANK(R32), ISBLANK(Y32)),"",R32+Y32)</f>
+        <v>78.8</v>
+      </c>
+      <c r="AG32" s="69">
+        <f t="shared" ref="AG32" si="71">IF(OR(ISBLANK(S32), ISBLANK(Z32)),"",S32+Z32)</f>
+        <v>78.8</v>
+      </c>
+      <c r="AH32" s="69">
+        <f t="shared" ref="AH32" si="72">IF(OR(ISBLANK(T32), ISBLANK(AA32)),"",T32+AA32)</f>
+        <v>78.8</v>
+      </c>
+      <c r="AI32" s="69">
+        <f t="shared" ref="AI32" si="73">IF(OR(ISBLANK(U32), ISBLANK(AB32)),"",U32+AB32)</f>
+        <v>68.873999999999995</v>
+      </c>
+      <c r="AJ32" s="69" t="str">
+        <f t="shared" ref="AJ32" si="74">IF(OR(ISBLANK(V32), ISBLANK(AC32)),"",V32+AC32)</f>
+        <v/>
+      </c>
+      <c r="AK32" s="69" t="str">
+        <f t="shared" ref="AK32" si="75">IF(OR(ISBLANK(W32), ISBLANK(AD32)),"",W32+AD32)</f>
+        <v/>
       </c>
       <c r="AS32" s="61"/>
       <c r="AT32" s="61">
@@ -6930,11 +7279,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7720,7 +8069,7 @@
         <v>311</v>
       </c>
       <c r="F22" s="61" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G22" s="61">
         <v>2020</v>
@@ -8074,7 +8423,7 @@
         <v>66</v>
       </c>
       <c r="F32" s="61" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G32" s="61">
         <v>2020</v>
@@ -8298,7 +8647,7 @@
         <v>311</v>
       </c>
       <c r="F38" s="61" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G38" s="61">
         <v>2021</v>
@@ -8374,7 +8723,7 @@
         <v>66</v>
       </c>
       <c r="F40" s="61" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G40" s="61">
         <v>2020</v>
@@ -8412,7 +8761,7 @@
         <v>66</v>
       </c>
       <c r="F41" s="61" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G41" s="61">
         <v>2020</v>

</xml_diff>

<commit_message>
Fix test and 2019 AES corp production data
Signed-off-by: David Kroon <david.kroon@ortec-finance.com>
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ITR\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD664DD-4459-BB4D-A540-782F0675653C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51600" yWindow="7880" windowWidth="44560" windowHeight="22440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51600" yWindow="7875" windowWidth="44565" windowHeight="22440" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="ITR input data (2)" sheetId="9" r:id="rId8"/>
     <sheet name="ITR target input data (2)" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,12 +38,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Michael Tiemann</author>
   </authors>
   <commentList>
-    <comment ref="AT2" authorId="0" shapeId="0" xr:uid="{FE07E697-8595-F149-90BA-0F794AF36923}">
+    <comment ref="AT2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{96C7E1CF-0386-CF41-8CC6-D6DC6ABF7CBB}">
+    <comment ref="R4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{809C1E46-BD52-814B-864B-65206C310321}">
+    <comment ref="Y4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF4" authorId="0" shapeId="0" xr:uid="{9CEBEB8E-A75A-A849-8EB4-15FCB953D619}">
+    <comment ref="AF4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{5CE2AC56-DBD4-F44E-8F7A-F2354A542158}">
+    <comment ref="J12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{E690D3D1-6563-964F-9370-62C106346114}">
+    <comment ref="J22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{ACADDAA5-6A0B-2240-80EB-179B5573D605}">
+    <comment ref="J23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -275,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J32" authorId="0" shapeId="0" xr:uid="{BE1A2F56-E041-FF47-8F16-701373C98C67}">
+    <comment ref="J32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -313,12 +312,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Michael Tiemann</author>
   </authors>
   <commentList>
-    <comment ref="L13" authorId="0" shapeId="0" xr:uid="{448510DF-B4CA-A74B-8DA4-8A66766A6D07}">
+    <comment ref="L13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -351,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{CA21DE94-42A9-2242-B39E-4A74054C3A31}">
+    <comment ref="F14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -384,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CBCC6D2D-3589-F54A-A3D8-C85B5415A3A1}">
+    <comment ref="F22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -418,7 +417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{E1E20C21-AC41-454F-BD00-E2E3A76147CB}">
+    <comment ref="F32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -451,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{D7FC3687-67D6-B94A-81A4-A3F0B5E62612}">
+    <comment ref="F38" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -496,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{D6EF40F2-AAE1-0D4C-AB96-6234B272A95B}">
+    <comment ref="F40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -541,7 +540,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{3621CB18-1100-1A47-8F98-EC355E02058C}">
+    <comment ref="F41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1697,7 +1696,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -3426,12 +3425,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275022A1-1FB4-4C34-9A96-60091C6220F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L20:R20"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="20" spans="12:18">
       <c r="L20" s="2"/>
@@ -3453,16 +3452,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CA0A32-C851-E646-9A5B-E6BA11976796}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ4"/>
   <sheetViews>
     <sheetView topLeftCell="AC1" workbookViewId="0">
       <selection activeCell="AN14" sqref="AN13:AN14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
+    <row r="1" spans="1:52" s="3" customFormat="1" ht="30">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -3781,14 +3780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0758D588-98FD-D448-B506-81C13C1B78B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12" s="61" customFormat="1">
       <c r="A1" s="10" t="s">
@@ -3872,40 +3871,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B77C2D-751E-4405-8B8F-EC57999324C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33:C33"/>
+      <selection pane="bottomRight" activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="24"/>
-    <col min="7" max="7" width="16.5" style="4"/>
-    <col min="9" max="9" width="16.5" style="5"/>
-    <col min="14" max="14" width="25.83203125" customWidth="1"/>
-    <col min="15" max="15" width="25.83203125" style="61" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" customWidth="1"/>
-    <col min="17" max="21" width="16.5" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="2" customWidth="1"/>
-    <col min="23" max="23" width="16.5" style="36" customWidth="1"/>
-    <col min="24" max="29" width="16.5" style="2" customWidth="1"/>
-    <col min="30" max="30" width="16.5" style="36" customWidth="1"/>
-    <col min="31" max="37" width="16.5" style="2" customWidth="1"/>
-    <col min="38" max="44" width="16.5" style="2"/>
-    <col min="45" max="49" width="16.83203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.5" style="2"/>
+    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="24"/>
+    <col min="7" max="7" width="16.42578125" style="4"/>
+    <col min="9" max="9" width="16.42578125" style="5"/>
+    <col min="14" max="14" width="25.85546875" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" style="61" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" customWidth="1"/>
+    <col min="17" max="21" width="16.42578125" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" style="36" customWidth="1"/>
+    <col min="24" max="29" width="16.42578125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="36" customWidth="1"/>
+    <col min="31" max="37" width="16.42578125" style="2" customWidth="1"/>
+    <col min="38" max="44" width="16.42578125" style="2"/>
+    <col min="45" max="49" width="16.85546875" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
+    <row r="1" spans="1:52" s="3" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -4203,7 +4202,7 @@
         <v>83985.94</v>
       </c>
       <c r="AV2" s="61">
-        <v>759043.55</v>
+        <v>75904.354999999996</v>
       </c>
       <c r="AW2" s="61">
         <v>75271.521999999997</v>
@@ -5157,7 +5156,7 @@
         <v>5664119.7339246115</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="16">
+    <row r="12" spans="1:52" ht="15.75">
       <c r="A12" s="61" t="s">
         <v>190</v>
       </c>
@@ -7995,29 +7994,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="61" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="61"/>
-    <col min="4" max="4" width="16.5" style="26"/>
-    <col min="5" max="5" width="17.5" style="26" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="61"/>
+    <col min="4" max="4" width="16.42578125" style="26"/>
+    <col min="5" max="5" width="17.42578125" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="61" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="20" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" style="61" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="61" customWidth="1"/>
     <col min="10" max="10" width="24" style="61" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" style="61" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="61" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="61" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -9611,22 +9610,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F5420B-4269-4C0B-A558-3652DBE2EE0B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.6640625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.7109375" style="51" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
-    <col min="8" max="8" width="87.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>12</v>
       </c>
@@ -9646,7 +9645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16">
+    <row r="2" spans="1:6">
       <c r="A2" s="40" t="s">
         <v>13</v>
       </c>
@@ -9666,7 +9665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6">
       <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
@@ -9686,7 +9685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32">
+    <row r="4" spans="1:6" ht="45">
       <c r="A4" s="40" t="s">
         <v>13</v>
       </c>
@@ -9706,7 +9705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="32">
+    <row r="5" spans="1:6" ht="30">
       <c r="A5" s="40" t="s">
         <v>13</v>
       </c>
@@ -9726,7 +9725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48">
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" s="40" t="s">
         <v>13</v>
       </c>
@@ -9746,7 +9745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16">
+    <row r="7" spans="1:6">
       <c r="A7" s="40" t="s">
         <v>13</v>
       </c>
@@ -9766,7 +9765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16">
+    <row r="8" spans="1:6">
       <c r="A8" s="40" t="s">
         <v>13</v>
       </c>
@@ -9786,7 +9785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="32">
+    <row r="9" spans="1:6" ht="45">
       <c r="A9" s="40" t="s">
         <v>13</v>
       </c>
@@ -9806,7 +9805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6">
       <c r="A10" s="40" t="s">
         <v>13</v>
       </c>
@@ -9826,7 +9825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6">
       <c r="A11" s="40" t="s">
         <v>13</v>
       </c>
@@ -9846,7 +9845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16">
+    <row r="12" spans="1:6">
       <c r="A12" s="40" t="s">
         <v>13</v>
       </c>
@@ -9866,7 +9865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16">
+    <row r="13" spans="1:6">
       <c r="A13" s="40" t="s">
         <v>13</v>
       </c>
@@ -9886,7 +9885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="40" t="s">
         <v>13</v>
       </c>
@@ -9906,7 +9905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16">
+    <row r="15" spans="1:6">
       <c r="A15" s="40" t="s">
         <v>13</v>
       </c>
@@ -9966,7 +9965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="31" t="s">
         <v>15</v>
       </c>
@@ -9986,7 +9985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="31" t="s">
         <v>15</v>
       </c>
@@ -10006,7 +10005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="32">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="31" t="s">
         <v>15</v>
       </c>
@@ -10026,7 +10025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="32">
+    <row r="21" spans="1:6" ht="30">
       <c r="A21" s="31" t="s">
         <v>15</v>
       </c>
@@ -10046,7 +10045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="32">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="31" t="s">
         <v>15</v>
       </c>
@@ -10066,7 +10065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="32">
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="31" t="s">
         <v>15</v>
       </c>
@@ -10086,7 +10085,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="48">
+    <row r="24" spans="1:6" ht="45">
       <c r="A24" s="31" t="s">
         <v>15</v>
       </c>
@@ -10106,7 +10105,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32">
+    <row r="25" spans="1:6" ht="30">
       <c r="A25" s="31" t="s">
         <v>15</v>
       </c>
@@ -10126,7 +10125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="32">
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="31" t="s">
         <v>15</v>
       </c>
@@ -10146,7 +10145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="32">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="31" t="s">
         <v>15</v>
       </c>
@@ -10166,7 +10165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32">
+    <row r="28" spans="1:6" ht="30">
       <c r="A28" s="31" t="s">
         <v>15</v>
       </c>
@@ -10186,7 +10185,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="32">
+    <row r="29" spans="1:6" ht="30">
       <c r="A29" s="31" t="s">
         <v>15</v>
       </c>
@@ -10206,7 +10205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="32">
+    <row r="30" spans="1:6" ht="30">
       <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
@@ -10226,7 +10225,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="48">
+    <row r="31" spans="1:6" ht="45">
       <c r="A31" s="31" t="s">
         <v>15</v>
       </c>
@@ -10246,7 +10245,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="32">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="31" t="s">
         <v>15</v>
       </c>
@@ -10266,7 +10265,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="32">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="31" t="s">
         <v>15</v>
       </c>
@@ -10286,7 +10285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="32">
+    <row r="34" spans="1:6" ht="30">
       <c r="A34" s="31" t="s">
         <v>15</v>
       </c>
@@ -10306,7 +10305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="32">
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="31" t="s">
         <v>15</v>
       </c>
@@ -10326,7 +10325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="32">
+    <row r="36" spans="1:6" ht="30">
       <c r="A36" s="31" t="s">
         <v>15</v>
       </c>
@@ -10346,7 +10345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="32">
+    <row r="37" spans="1:6" ht="30">
       <c r="A37" s="31" t="s">
         <v>15</v>
       </c>
@@ -10366,7 +10365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="48">
+    <row r="38" spans="1:6" ht="45">
       <c r="A38" s="31" t="s">
         <v>15</v>
       </c>
@@ -10386,7 +10385,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="32">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="31" t="s">
         <v>15</v>
       </c>
@@ -10406,7 +10405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="32">
+    <row r="40" spans="1:6" ht="30">
       <c r="A40" s="31" t="s">
         <v>15</v>
       </c>
@@ -10426,7 +10425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="32">
+    <row r="41" spans="1:6" ht="30">
       <c r="A41" s="31" t="s">
         <v>15</v>
       </c>
@@ -10446,7 +10445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="32">
+    <row r="42" spans="1:6" ht="30">
       <c r="A42" s="31" t="s">
         <v>15</v>
       </c>
@@ -10466,7 +10465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="32">
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="31" t="s">
         <v>15</v>
       </c>
@@ -10486,7 +10485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="32">
+    <row r="44" spans="1:6" ht="30">
       <c r="A44" s="31" t="s">
         <v>15</v>
       </c>
@@ -10506,7 +10505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="48">
+    <row r="45" spans="1:6" ht="45">
       <c r="A45" s="31" t="s">
         <v>15</v>
       </c>
@@ -10526,7 +10525,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="32">
+    <row r="46" spans="1:6" ht="30">
       <c r="A46" s="50" t="s">
         <v>75</v>
       </c>
@@ -10546,7 +10545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="32">
+    <row r="47" spans="1:6" ht="30">
       <c r="A47" s="50" t="s">
         <v>75</v>
       </c>
@@ -10566,7 +10565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="32">
+    <row r="48" spans="1:6" ht="30">
       <c r="A48" s="50" t="s">
         <v>75</v>
       </c>
@@ -10586,7 +10585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="32">
+    <row r="49" spans="1:6" ht="30">
       <c r="A49" s="50" t="s">
         <v>75</v>
       </c>
@@ -10606,7 +10605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="32">
+    <row r="50" spans="1:6" ht="30">
       <c r="A50" s="50" t="s">
         <v>75</v>
       </c>
@@ -10626,7 +10625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="32">
+    <row r="51" spans="1:6" ht="30">
       <c r="A51" s="44" t="s">
         <v>14</v>
       </c>
@@ -10646,7 +10645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="48">
+    <row r="52" spans="1:6" ht="60">
       <c r="A52" s="44" t="s">
         <v>14</v>
       </c>
@@ -10666,7 +10665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16">
+    <row r="53" spans="1:6">
       <c r="A53" s="44" t="s">
         <v>14</v>
       </c>
@@ -10686,7 +10685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16">
+    <row r="54" spans="1:6">
       <c r="A54" s="44" t="s">
         <v>14</v>
       </c>
@@ -10706,7 +10705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="80">
+    <row r="55" spans="1:6" ht="75">
       <c r="A55" s="44" t="s">
         <v>14</v>
       </c>
@@ -10726,7 +10725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="64">
+    <row r="56" spans="1:6" ht="75">
       <c r="A56" s="44" t="s">
         <v>14</v>
       </c>
@@ -10746,7 +10745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16">
+    <row r="57" spans="1:6">
       <c r="A57" s="44" t="s">
         <v>14</v>
       </c>
@@ -10766,7 +10765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="32">
+    <row r="58" spans="1:6" ht="30">
       <c r="A58" s="44" t="s">
         <v>14</v>
       </c>
@@ -10786,7 +10785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="48">
+    <row r="59" spans="1:6" ht="45">
       <c r="A59" s="45" t="s">
         <v>103</v>
       </c>
@@ -10817,19 +10816,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="61" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10864,7 +10863,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>72202</v>
+        <v>54173</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10881,8 +10880,8 @@
         <v>147</v>
       </c>
       <c r="E3" s="61">
-        <f t="shared" ref="E3:E41" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>73526</v>
+        <f t="shared" ref="E3:E33" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
+        <v>98590</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10900,7 +10899,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>240322</v>
+        <v>159377</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10918,7 +10917,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>107919</v>
+        <v>210445</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10936,7 +10935,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>72844</v>
+        <v>38219</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10954,7 +10953,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>92782</v>
+        <v>123326</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10972,7 +10971,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>92119</v>
+        <v>93004</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10990,7 +10989,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>218353</v>
+        <v>116763</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11008,7 +11007,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>65475</v>
+        <v>128506</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11026,7 +11025,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>223699</v>
+        <v>77402</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11044,7 +11043,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>196417</v>
+        <v>188530</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11062,7 +11061,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>140770</v>
+        <v>36186</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11080,7 +11079,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>121912</v>
+        <v>165727</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -11098,7 +11097,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>196880</v>
+        <v>101690</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11116,7 +11115,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>200429</v>
+        <v>120592</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11134,7 +11133,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>176914</v>
+        <v>127438</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11152,7 +11151,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>95469</v>
+        <v>196333</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11170,7 +11169,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>149405</v>
+        <v>152722</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11188,7 +11187,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>175462</v>
+        <v>125969</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11206,7 +11205,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>218599</v>
+        <v>180101</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11224,7 +11223,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>159201</v>
+        <v>156801</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -11242,7 +11241,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>158753</v>
+        <v>175770</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -11260,7 +11259,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>194641</v>
+        <v>119305</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -11278,7 +11277,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>40914</v>
+        <v>89926</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -11296,7 +11295,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>171655</v>
+        <v>126370</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -11314,7 +11313,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>211491</v>
+        <v>197235</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -11332,7 +11331,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>163760</v>
+        <v>122102</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -11350,7 +11349,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>79169</v>
+        <v>177763</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -11368,7 +11367,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>38383</v>
+        <v>174816</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -11386,7 +11385,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>60079</v>
+        <v>81388</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -11404,7 +11403,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>189840</v>
+        <v>211885</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -11422,7 +11421,7 @@
       </c>
       <c r="E33" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>68380</v>
+        <v>243388</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -11487,49 +11486,49 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364511B7-3F85-F540-BA5C-9DA3347FB2A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AZ54"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="61"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="61"/>
+    <col min="1" max="1" width="16.42578125" style="61"/>
+    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="61"/>
     <col min="4" max="4" width="8" style="61" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="24"/>
-    <col min="6" max="6" width="16.5" style="61"/>
+    <col min="5" max="5" width="16.42578125" style="24"/>
+    <col min="6" max="6" width="16.42578125" style="61"/>
     <col min="7" max="7" width="10" style="4" customWidth="1"/>
     <col min="8" max="8" width="9" style="61" customWidth="1"/>
     <col min="9" max="9" width="11" style="5" customWidth="1"/>
-    <col min="10" max="13" width="16.5" style="61"/>
+    <col min="10" max="13" width="16.42578125" style="61"/>
     <col min="14" max="14" width="17" style="61" customWidth="1"/>
-    <col min="15" max="15" width="15.5" style="61" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" style="61" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" style="61" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="61" customWidth="1"/>
     <col min="17" max="19" width="0" style="61" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="16.5" style="61"/>
+    <col min="20" max="21" width="16.42578125" style="61"/>
     <col min="22" max="22" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="0" style="36" hidden="1" customWidth="1"/>
     <col min="24" max="29" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="0" style="36" hidden="1" customWidth="1"/>
     <col min="31" max="33" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="34" max="36" width="16.5" style="2"/>
+    <col min="34" max="36" width="16.42578125" style="2"/>
     <col min="37" max="44" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="45" max="47" width="16.83203125" style="2" hidden="1" customWidth="1"/>
-    <col min="48" max="49" width="16.83203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.5" style="2"/>
+    <col min="45" max="47" width="16.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="48" max="49" width="16.85546875" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
+    <row r="1" spans="1:52" s="3" customFormat="1" ht="30">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -16114,27 +16113,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B625E0-7A95-AB40-9EC5-2C6C2025FC51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="61" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="61"/>
-    <col min="4" max="4" width="8.83203125" style="26"/>
-    <col min="5" max="5" width="17.5" style="26" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="61"/>
+    <col min="4" max="4" width="8.85546875" style="26"/>
+    <col min="5" max="5" width="17.42578125" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="61" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="20" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" style="61" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="61" customWidth="1"/>
     <col min="10" max="10" width="24" style="61" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" style="61" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="61" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="61"/>
+    <col min="11" max="11" width="19.28515625" style="61" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="61" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="61"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -16675,6 +16674,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -16891,12 +16896,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
   <ds:schemaRefs>
@@ -16906,6 +16905,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16922,21 +16938,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Also update sample data in main test area
Ugh...we have two copies of the same data.  More tests should run with this updated data.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ITR\test\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC2D88E-09D2-7C45-AFBE-48F94FC59B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51600" yWindow="7875" windowWidth="44565" windowHeight="22440" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="44680" yWindow="14200" windowWidth="44560" windowHeight="22440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="ITR input data (2)" sheetId="9" r:id="rId8"/>
     <sheet name="ITR target input data (2)" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,12 +39,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Michael Tiemann</author>
   </authors>
   <commentList>
-    <comment ref="AT2" authorId="0" shapeId="0">
+    <comment ref="AT2" authorId="0" shapeId="0" xr:uid="{FE07E697-8595-F149-90BA-0F794AF36923}">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0" shapeId="0">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{96C7E1CF-0386-CF41-8CC6-D6DC6ABF7CBB}">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y4" authorId="0" shapeId="0">
+    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{809C1E46-BD52-814B-864B-65206C310321}">
       <text>
         <r>
           <rPr>
@@ -142,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF4" authorId="0" shapeId="0">
+    <comment ref="AF4" authorId="0" shapeId="0" xr:uid="{9CEBEB8E-A75A-A849-8EB4-15FCB953D619}">
       <text>
         <r>
           <rPr>
@@ -175,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0" shapeId="0">
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{5CE2AC56-DBD4-F44E-8F7A-F2354A542158}">
       <text>
         <r>
           <rPr>
@@ -208,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{E690D3D1-6563-964F-9370-62C106346114}">
       <text>
         <r>
           <rPr>
@@ -241,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{ACADDAA5-6A0B-2240-80EB-179B5573D605}">
       <text>
         <r>
           <rPr>
@@ -274,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J32" authorId="0" shapeId="0">
+    <comment ref="J32" authorId="0" shapeId="0" xr:uid="{BE1A2F56-E041-FF47-8F16-701373C98C67}">
       <text>
         <r>
           <rPr>
@@ -312,12 +313,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Michael Tiemann</author>
   </authors>
   <commentList>
-    <comment ref="L13" authorId="0" shapeId="0">
+    <comment ref="L13" authorId="0" shapeId="0" xr:uid="{448510DF-B4CA-A74B-8DA4-8A66766A6D07}">
       <text>
         <r>
           <rPr>
@@ -350,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{CA21DE94-42A9-2242-B39E-4A74054C3A31}">
       <text>
         <r>
           <rPr>
@@ -383,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CBCC6D2D-3589-F54A-A3D8-C85B5415A3A1}">
       <text>
         <r>
           <rPr>
@@ -417,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{E1E20C21-AC41-454F-BD00-E2E3A76147CB}">
       <text>
         <r>
           <rPr>
@@ -450,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{D7FC3687-67D6-B94A-81A4-A3F0B5E62612}">
       <text>
         <r>
           <rPr>
@@ -495,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{D6EF40F2-AAE1-0D4C-AB96-6234B272A95B}">
       <text>
         <r>
           <rPr>
@@ -523,24 +524,13 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Really S1+S2+S3 but setting to S1+S2 for now.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{3621CB18-1100-1A47-8F98-EC355E02058C}">
       <text>
         <r>
           <rPr>
@@ -568,19 +558,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>Really S1+S2+S3 but setting to S1+S2 for now.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Really S1+S2+S3 but setting to S1+S2 for now.
 </t>
         </r>
       </text>
@@ -590,7 +569,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="324">
   <si>
     <t>Data field</t>
   </si>
@@ -1687,16 +1666,13 @@
     <t>investment_value</t>
   </si>
   <si>
-    <t>Asia</t>
-  </si>
-  <si>
     <t>netzero_year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -3425,12 +3401,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275022A1-1FB4-4C34-9A96-60091C6220F6}">
   <dimension ref="L20:R20"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="20" spans="12:18">
       <c r="L20" s="2"/>
@@ -3452,16 +3428,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CA0A32-C851-E646-9A5B-E6BA11976796}">
   <dimension ref="A1:AZ4"/>
   <sheetViews>
     <sheetView topLeftCell="AC1" workbookViewId="0">
       <selection activeCell="AN14" sqref="AN13:AN14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="30">
+    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -3780,14 +3756,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0758D588-98FD-D448-B506-81C13C1B78B8}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12" s="61" customFormat="1">
       <c r="A1" s="10" t="s">
@@ -3800,7 +3776,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>123</v>
@@ -3871,40 +3847,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B77C2D-751E-4405-8B8F-EC57999324C2}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV2" sqref="AV2"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="24"/>
-    <col min="7" max="7" width="16.42578125" style="4"/>
-    <col min="9" max="9" width="16.42578125" style="5"/>
-    <col min="14" max="14" width="25.85546875" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" style="61" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" customWidth="1"/>
-    <col min="17" max="21" width="16.42578125" customWidth="1"/>
-    <col min="22" max="22" width="16.42578125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="16.42578125" style="36" customWidth="1"/>
-    <col min="24" max="29" width="16.42578125" style="2" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="36" customWidth="1"/>
-    <col min="31" max="37" width="16.42578125" style="2" customWidth="1"/>
-    <col min="38" max="44" width="16.42578125" style="2"/>
-    <col min="45" max="49" width="16.85546875" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.42578125" style="2"/>
+    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="24"/>
+    <col min="7" max="7" width="16.5" style="4"/>
+    <col min="9" max="9" width="16.5" style="5"/>
+    <col min="14" max="14" width="25.83203125" customWidth="1"/>
+    <col min="15" max="15" width="25.83203125" style="61" customWidth="1"/>
+    <col min="16" max="16" width="22.1640625" customWidth="1"/>
+    <col min="17" max="21" width="16.5" customWidth="1"/>
+    <col min="22" max="22" width="16.5" style="2" customWidth="1"/>
+    <col min="23" max="23" width="16.5" style="36" customWidth="1"/>
+    <col min="24" max="29" width="16.5" style="2" customWidth="1"/>
+    <col min="30" max="30" width="16.5" style="36" customWidth="1"/>
+    <col min="31" max="37" width="16.5" style="2" customWidth="1"/>
+    <col min="38" max="44" width="16.5" style="2"/>
+    <col min="45" max="49" width="16.83203125" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1">
+    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -4072,9 +4048,7 @@
       <c r="D2" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E2" s="61"/>
       <c r="F2" s="61" t="s">
         <v>142</v>
       </c>
@@ -4202,7 +4176,7 @@
         <v>83985.94</v>
       </c>
       <c r="AV2" s="61">
-        <v>75904.354999999996</v>
+        <v>759043.55</v>
       </c>
       <c r="AW2" s="61">
         <v>75271.521999999997</v>
@@ -4224,9 +4198,7 @@
       <c r="D3" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E3" s="61"/>
       <c r="F3" s="61" t="s">
         <v>142</v>
       </c>
@@ -4310,9 +4282,7 @@
       <c r="D4" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E4" s="61"/>
       <c r="F4" s="61" t="s">
         <v>142</v>
       </c>
@@ -4429,9 +4399,7 @@
       <c r="D5" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E5" s="61"/>
       <c r="F5" s="61" t="s">
         <v>142</v>
       </c>
@@ -4514,9 +4482,7 @@
       <c r="D6" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E6" s="61"/>
       <c r="F6" s="61" t="s">
         <v>142</v>
       </c>
@@ -4637,9 +4603,7 @@
       <c r="D7" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E7" s="61"/>
       <c r="F7" s="61" t="s">
         <v>142</v>
       </c>
@@ -4769,9 +4733,7 @@
       <c r="D8" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E8" s="61"/>
       <c r="F8" s="61" t="s">
         <v>142</v>
       </c>
@@ -4878,9 +4840,7 @@
       <c r="D9" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E9" s="61"/>
       <c r="F9" s="61" t="s">
         <v>182</v>
       </c>
@@ -4963,9 +4923,7 @@
       <c r="D10" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E10" s="61"/>
       <c r="F10" s="61" t="s">
         <v>142</v>
       </c>
@@ -5049,9 +5007,7 @@
       <c r="D11" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E11" s="61"/>
       <c r="F11" s="61" t="s">
         <v>182</v>
       </c>
@@ -5156,7 +5112,7 @@
         <v>5664119.7339246115</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="15.75">
+    <row r="12" spans="1:52" ht="16">
       <c r="A12" s="61" t="s">
         <v>190</v>
       </c>
@@ -5169,9 +5125,7 @@
       <c r="D12" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E12" s="61"/>
       <c r="F12" s="61" t="s">
         <v>142</v>
       </c>
@@ -5200,7 +5154,7 @@
         <v>7476298000</v>
       </c>
       <c r="O12" s="61" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="P12" s="61" t="s">
         <v>318</v>
@@ -5255,9 +5209,7 @@
       <c r="D13" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E13" s="61"/>
       <c r="F13" s="61" t="s">
         <v>142</v>
       </c>
@@ -5305,6 +5257,49 @@
       </c>
       <c r="U13" s="2">
         <v>1.145419433</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="69">
+        <f>IF(OR(ISBLANK(Q13), ISBLANK(X13)),"",Q13+X13)</f>
+        <v>1.325786621</v>
+      </c>
+      <c r="AF13" s="69">
+        <f t="shared" ref="AF13" si="14">IF(ISBLANK(R13),IF(ISBLANK(Y13),"",Y13),R13+Y13)</f>
+        <v>1.323738978</v>
+      </c>
+      <c r="AG13" s="69">
+        <f t="shared" ref="AG13" si="15">IF(ISBLANK(S13),IF(ISBLANK(Z13),"",Z13),S13+Z13)</f>
+        <v>1.2685339369999999</v>
+      </c>
+      <c r="AH13" s="69">
+        <f t="shared" ref="AH13" si="16">IF(ISBLANK(T13),IF(ISBLANK(AA13),"",AA13),T13+AA13)</f>
+        <v>1.202690405</v>
+      </c>
+      <c r="AI13" s="69">
+        <f t="shared" ref="AI13" si="17">IF(ISBLANK(U13),IF(ISBLANK(AB13),"",AB13),U13+AB13)</f>
+        <v>1.145419433</v>
+      </c>
+      <c r="AJ13" s="69" t="str">
+        <f t="shared" ref="AJ13" si="18">IF(ISBLANK(V13),IF(ISBLANK(AC13),"",AC13),V13+AC13)</f>
+        <v/>
+      </c>
+      <c r="AK13" s="69" t="str">
+        <f t="shared" ref="AK13" si="19">IF(ISBLANK(W13),IF(ISBLANK(AD13),"",AD13),W13+AD13)</f>
+        <v/>
       </c>
       <c r="AS13" s="61">
         <v>5.3109194439999996</v>
@@ -5336,9 +5331,7 @@
       <c r="D14" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E14" s="61"/>
       <c r="F14" s="61" t="s">
         <v>142</v>
       </c>
@@ -5386,6 +5379,49 @@
       </c>
       <c r="U14" s="2">
         <v>26.48364437</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="69">
+        <f>IF(OR(ISBLANK(Q14), ISBLANK(X14)),"",Q14+X14)</f>
+        <v>26.796145450000001</v>
+      </c>
+      <c r="AF14" s="69">
+        <f t="shared" ref="AF14" si="20">IF(ISBLANK(R14),IF(ISBLANK(Y14),"",Y14),R14+Y14)</f>
+        <v>27.947696990000001</v>
+      </c>
+      <c r="AG14" s="69">
+        <f t="shared" ref="AG14" si="21">IF(ISBLANK(S14),IF(ISBLANK(Z14),"",Z14),S14+Z14)</f>
+        <v>29.95633261</v>
+      </c>
+      <c r="AH14" s="69">
+        <f t="shared" ref="AH14" si="22">IF(ISBLANK(T14),IF(ISBLANK(AA14),"",AA14),T14+AA14)</f>
+        <v>27.00027425</v>
+      </c>
+      <c r="AI14" s="69">
+        <f t="shared" ref="AI14" si="23">IF(ISBLANK(U14),IF(ISBLANK(AB14),"",AB14),U14+AB14)</f>
+        <v>26.48364437</v>
+      </c>
+      <c r="AJ14" s="69" t="str">
+        <f t="shared" ref="AJ14" si="24">IF(ISBLANK(V14),IF(ISBLANK(AC14),"",AC14),V14+AC14)</f>
+        <v/>
+      </c>
+      <c r="AK14" s="69" t="str">
+        <f t="shared" ref="AK14" si="25">IF(ISBLANK(W14),IF(ISBLANK(AD14),"",AD14),W14+AD14)</f>
+        <v/>
       </c>
       <c r="AS14" s="61">
         <v>39.339109710000002</v>
@@ -5417,9 +5453,7 @@
       <c r="D15" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E15" s="61"/>
       <c r="F15" s="61" t="s">
         <v>142</v>
       </c>
@@ -5517,9 +5551,7 @@
       <c r="D16" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E16" s="61"/>
       <c r="F16" s="61" t="s">
         <v>142</v>
       </c>
@@ -5567,6 +5599,49 @@
       </c>
       <c r="U16" s="2">
         <v>82.018839239000002</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="69">
+        <f t="shared" ref="AE16:AE17" si="26">IF(OR(ISBLANK(Q16), ISBLANK(X16)),"",Q16+X16)</f>
+        <v>94.923459879999996</v>
+      </c>
+      <c r="AF16" s="69">
+        <f t="shared" ref="AF16:AF17" si="27">IF(ISBLANK(R16),IF(ISBLANK(Y16),"",Y16),R16+Y16)</f>
+        <v>93.530450478000006</v>
+      </c>
+      <c r="AG16" s="69">
+        <f t="shared" ref="AG16:AG17" si="28">IF(ISBLANK(S16),IF(ISBLANK(Z16),"",Z16),S16+Z16)</f>
+        <v>95.012237693000003</v>
+      </c>
+      <c r="AH16" s="69">
+        <f t="shared" ref="AH16:AH17" si="29">IF(ISBLANK(T16),IF(ISBLANK(AA16),"",AA16),T16+AA16)</f>
+        <v>83.595723118999999</v>
+      </c>
+      <c r="AI16" s="69">
+        <f t="shared" ref="AI16:AI17" si="30">IF(ISBLANK(U16),IF(ISBLANK(AB16),"",AB16),U16+AB16)</f>
+        <v>82.018839239000002</v>
+      </c>
+      <c r="AJ16" s="69" t="str">
+        <f t="shared" ref="AJ16:AJ17" si="31">IF(ISBLANK(V16),IF(ISBLANK(AC16),"",AC16),V16+AC16)</f>
+        <v/>
+      </c>
+      <c r="AK16" s="69" t="str">
+        <f t="shared" ref="AK16:AK17" si="32">IF(ISBLANK(W16),IF(ISBLANK(AD16),"",AD16),W16+AD16)</f>
+        <v/>
       </c>
       <c r="AS16" s="61">
         <v>221.77898501999999</v>
@@ -5598,9 +5673,7 @@
       <c r="D17" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E17" s="61"/>
       <c r="F17" s="61" t="s">
         <v>142</v>
       </c>
@@ -5648,6 +5721,49 @@
       </c>
       <c r="U17" s="90">
         <v>33.246229124999999</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="69">
+        <f t="shared" si="26"/>
+        <v>32.516193991999998</v>
+      </c>
+      <c r="AF17" s="69">
+        <f t="shared" si="27"/>
+        <v>31.450986952000001</v>
+      </c>
+      <c r="AG17" s="69">
+        <f t="shared" si="28"/>
+        <v>34.631975513</v>
+      </c>
+      <c r="AH17" s="69">
+        <f t="shared" si="29"/>
+        <v>33.246229124999999</v>
+      </c>
+      <c r="AI17" s="69">
+        <f t="shared" si="30"/>
+        <v>33.246229124999999</v>
+      </c>
+      <c r="AJ17" s="69" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="AK17" s="69" t="str">
+        <f t="shared" si="32"/>
+        <v/>
       </c>
       <c r="AS17" s="61">
         <v>102.999524264</v>
@@ -5679,9 +5795,7 @@
       <c r="D18" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E18" s="61"/>
       <c r="F18" s="61" t="s">
         <v>142</v>
       </c>
@@ -5746,31 +5860,31 @@
         <v>0</v>
       </c>
       <c r="AE18" s="69">
-        <f t="shared" ref="AE18" si="14">IF(OR(ISBLANK(Q18), ISBLANK(X18)),"",Q18+X18)</f>
+        <f t="shared" ref="AE18" si="33">IF(OR(ISBLANK(Q18), ISBLANK(X18)),"",Q18+X18)</f>
         <v>35.122915438000007</v>
       </c>
       <c r="AF18" s="69">
-        <f t="shared" ref="AF18" si="15">IF(OR(ISBLANK(R18), ISBLANK(Y18)),"",R18+Y18)</f>
+        <f t="shared" ref="AF18" si="34">IF(OR(ISBLANK(R18), ISBLANK(Y18)),"",R18+Y18)</f>
         <v>32.270565695999998</v>
       </c>
       <c r="AG18" s="69">
-        <f t="shared" ref="AG18" si="16">IF(OR(ISBLANK(S18), ISBLANK(Z18)),"",S18+Z18)</f>
+        <f t="shared" ref="AG18" si="35">IF(OR(ISBLANK(S18), ISBLANK(Z18)),"",S18+Z18)</f>
         <v>28.483757178000001</v>
       </c>
       <c r="AH18" s="69">
-        <f t="shared" ref="AH18" si="17">IF(OR(ISBLANK(T18), ISBLANK(AA18)),"",T18+AA18)</f>
+        <f t="shared" ref="AH18" si="36">IF(OR(ISBLANK(T18), ISBLANK(AA18)),"",T18+AA18)</f>
         <v>26.74941115</v>
       </c>
       <c r="AI18" s="69">
-        <f t="shared" ref="AI18" si="18">IF(OR(ISBLANK(U18), ISBLANK(AB18)),"",U18+AB18)</f>
+        <f t="shared" ref="AI18" si="37">IF(OR(ISBLANK(U18), ISBLANK(AB18)),"",U18+AB18)</f>
         <v>35.013482494000002</v>
       </c>
       <c r="AJ18" s="69" t="str">
-        <f t="shared" ref="AJ18" si="19">IF(OR(ISBLANK(V18), ISBLANK(AC18)),"",V18+AC18)</f>
+        <f t="shared" ref="AJ18" si="38">IF(OR(ISBLANK(V18), ISBLANK(AC18)),"",V18+AC18)</f>
         <v/>
       </c>
       <c r="AK18" s="69" t="str">
-        <f t="shared" ref="AK18" si="20">IF(OR(ISBLANK(W18), ISBLANK(AD18)),"",W18+AD18)</f>
+        <f t="shared" ref="AK18" si="39">IF(OR(ISBLANK(W18), ISBLANK(AD18)),"",W18+AD18)</f>
         <v/>
       </c>
       <c r="AS18" s="61">
@@ -5803,9 +5917,7 @@
       <c r="D19" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E19" s="61"/>
       <c r="F19" s="61" t="s">
         <v>142</v>
       </c>
@@ -5871,31 +5983,31 @@
         <v>0</v>
       </c>
       <c r="AE19" s="69">
-        <f t="shared" ref="AE19" si="21">IF(OR(ISBLANK(Q19), ISBLANK(X19)),"",Q19+X19)</f>
+        <f t="shared" ref="AE19" si="40">IF(OR(ISBLANK(Q19), ISBLANK(X19)),"",Q19+X19)</f>
         <v>0.54127069000000005</v>
       </c>
       <c r="AF19" s="69">
-        <f t="shared" ref="AF19" si="22">IF(OR(ISBLANK(R19), ISBLANK(Y19)),"",R19+Y19)</f>
+        <f t="shared" ref="AF19" si="41">IF(OR(ISBLANK(R19), ISBLANK(Y19)),"",R19+Y19)</f>
         <v>0.38852905199999999</v>
       </c>
       <c r="AG19" s="69">
-        <f t="shared" ref="AG19" si="23">IF(OR(ISBLANK(S19), ISBLANK(Z19)),"",S19+Z19)</f>
+        <f t="shared" ref="AG19" si="42">IF(OR(ISBLANK(S19), ISBLANK(Z19)),"",S19+Z19)</f>
         <v>3.4941450000000002E-3</v>
       </c>
       <c r="AH19" s="69">
-        <f t="shared" ref="AH19" si="24">IF(OR(ISBLANK(T19), ISBLANK(AA19)),"",T19+AA19)</f>
+        <f t="shared" ref="AH19" si="43">IF(OR(ISBLANK(T19), ISBLANK(AA19)),"",T19+AA19)</f>
         <v>2.2128600000000001E-4</v>
       </c>
       <c r="AI19" s="69">
-        <f t="shared" ref="AI19" si="25">IF(OR(ISBLANK(U19), ISBLANK(AB19)),"",U19+AB19)</f>
+        <f t="shared" ref="AI19" si="44">IF(OR(ISBLANK(U19), ISBLANK(AB19)),"",U19+AB19)</f>
         <v>2.2128600000000001E-4</v>
       </c>
       <c r="AJ19" s="69" t="str">
-        <f t="shared" ref="AJ19" si="26">IF(OR(ISBLANK(V19), ISBLANK(AC19)),"",V19+AC19)</f>
+        <f t="shared" ref="AJ19" si="45">IF(OR(ISBLANK(V19), ISBLANK(AC19)),"",V19+AC19)</f>
         <v/>
       </c>
       <c r="AK19" s="69" t="str">
-        <f t="shared" ref="AK19" si="27">IF(OR(ISBLANK(W19), ISBLANK(AD19)),"",W19+AD19)</f>
+        <f t="shared" ref="AK19" si="46">IF(OR(ISBLANK(W19), ISBLANK(AD19)),"",W19+AD19)</f>
         <v/>
       </c>
       <c r="AS19" s="61">
@@ -5927,9 +6039,7 @@
       <c r="D20" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E20" s="61"/>
       <c r="F20" s="61" t="s">
         <v>142</v>
       </c>
@@ -5998,27 +6108,27 @@
         <v>16784000</v>
       </c>
       <c r="AF20" s="69">
-        <f t="shared" ref="AF20" si="28">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
+        <f t="shared" ref="AF20" si="47">IF(ISBLANK(R20),IF(ISBLANK(Y20),"",Y20),R20+Y20)</f>
         <v>27225000</v>
       </c>
       <c r="AG20" s="69">
-        <f t="shared" ref="AG20" si="29">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
+        <f t="shared" ref="AG20" si="48">IF(ISBLANK(S20),IF(ISBLANK(Z20),"",Z20),S20+Z20)</f>
         <v>29863000</v>
       </c>
       <c r="AH20" s="69">
-        <f t="shared" ref="AH20" si="30">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
+        <f t="shared" ref="AH20" si="49">IF(ISBLANK(T20),IF(ISBLANK(AA20),"",AA20),T20+AA20)</f>
         <v>27430000</v>
       </c>
       <c r="AI20" s="69">
-        <f t="shared" ref="AI20" si="31">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
+        <f t="shared" ref="AI20" si="50">IF(ISBLANK(U20),IF(ISBLANK(AB20),"",AB20),U20+AB20)</f>
         <v>22213000</v>
       </c>
       <c r="AJ20" s="69" t="str">
-        <f t="shared" ref="AJ20" si="32">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
+        <f t="shared" ref="AJ20" si="51">IF(ISBLANK(V20),IF(ISBLANK(AC20),"",AC20),V20+AC20)</f>
         <v/>
       </c>
       <c r="AK20" s="69" t="str">
-        <f t="shared" ref="AK20" si="33">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
+        <f t="shared" ref="AK20" si="52">IF(ISBLANK(W20),IF(ISBLANK(AD20),"",AD20),W20+AD20)</f>
         <v/>
       </c>
       <c r="AS20" s="76">
@@ -6053,9 +6163,7 @@
       <c r="D21" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E21" s="61"/>
       <c r="F21" s="61" t="s">
         <v>142</v>
       </c>
@@ -6119,27 +6227,27 @@
         <v/>
       </c>
       <c r="AF21" s="69">
-        <f t="shared" ref="AF21" si="34">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
+        <f t="shared" ref="AF21" si="53">IF(ISBLANK(R21),IF(ISBLANK(Y21),"",Y21),R21+Y21)</f>
         <v>60434671</v>
       </c>
       <c r="AG21" s="69">
-        <f t="shared" ref="AG21" si="35">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
+        <f t="shared" ref="AG21" si="54">IF(ISBLANK(S21),IF(ISBLANK(Z21),"",Z21),S21+Z21)</f>
         <v>52972697</v>
       </c>
       <c r="AH21" s="69">
-        <f t="shared" ref="AH21" si="36">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
+        <f t="shared" ref="AH21" si="55">IF(ISBLANK(T21),IF(ISBLANK(AA21),"",AA21),T21+AA21)</f>
         <v>49863111</v>
       </c>
       <c r="AI21" s="69">
-        <f t="shared" ref="AI21" si="37">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
+        <f t="shared" ref="AI21" si="56">IF(ISBLANK(U21),IF(ISBLANK(AB21),"",AB21),U21+AB21)</f>
         <v>42750225</v>
       </c>
       <c r="AJ21" s="69" t="str">
-        <f t="shared" ref="AJ21" si="38">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
+        <f t="shared" ref="AJ21" si="57">IF(ISBLANK(V21),IF(ISBLANK(AC21),"",AC21),V21+AC21)</f>
         <v/>
       </c>
       <c r="AK21" s="69" t="str">
-        <f t="shared" ref="AK21" si="39">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
+        <f t="shared" ref="AK21" si="58">IF(ISBLANK(W21),IF(ISBLANK(AD21),"",AD21),W21+AD21)</f>
         <v/>
       </c>
       <c r="AS21" s="61"/>
@@ -6169,9 +6277,7 @@
       <c r="D22" s="61" t="s">
         <v>154</v>
       </c>
-      <c r="E22" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E22" s="61"/>
       <c r="F22" s="61" t="s">
         <v>142</v>
       </c>
@@ -6240,31 +6346,31 @@
         <v>2487000</v>
       </c>
       <c r="AE22" s="69">
-        <f t="shared" ref="AE22:AK23" si="40">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
+        <f t="shared" ref="AE22:AK23" si="59">IF(OR(ISBLANK(Q22), ISBLANK(X22)),"",Q22+X22)</f>
         <v>14435000</v>
       </c>
       <c r="AF22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>13858000</v>
       </c>
       <c r="AG22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>13933000</v>
       </c>
       <c r="AH22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>14858000</v>
       </c>
       <c r="AI22" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>12580000</v>
       </c>
       <c r="AJ22" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AK22" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AS22" s="61">
@@ -6301,9 +6407,7 @@
       <c r="D23" s="61" t="s">
         <v>226</v>
       </c>
-      <c r="E23" s="61" t="s">
-        <v>227</v>
-      </c>
+      <c r="E23" s="61"/>
       <c r="F23" s="61" t="s">
         <v>182</v>
       </c>
@@ -6369,31 +6473,31 @@
         <v>0</v>
       </c>
       <c r="AE23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>16.100000000000001</v>
       </c>
       <c r="AF23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>16.100000000000001</v>
       </c>
       <c r="AG23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>14.27265885416667</v>
       </c>
       <c r="AH23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>11.947505</v>
       </c>
       <c r="AI23" s="69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>11.738147617323991</v>
       </c>
       <c r="AJ23" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AK23" s="69" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AS23" s="61">
@@ -6425,9 +6529,7 @@
       <c r="D24" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E24" s="61"/>
       <c r="F24" s="61" t="s">
         <v>142</v>
       </c>
@@ -6492,31 +6594,31 @@
         <v>0</v>
       </c>
       <c r="AE24" s="69">
-        <f t="shared" ref="AE24" si="41">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
+        <f t="shared" ref="AE24" si="60">IF(OR(ISBLANK(Q24), ISBLANK(X24)),"",Q24+X24)</f>
         <v>3.8868941879999999</v>
       </c>
       <c r="AF24" s="69">
-        <f t="shared" ref="AF24" si="42">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
+        <f t="shared" ref="AF24" si="61">IF(OR(ISBLANK(R24), ISBLANK(Y24)),"",R24+Y24)</f>
         <v>3.8663196809999998</v>
       </c>
       <c r="AG24" s="69">
-        <f t="shared" ref="AG24" si="43">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
+        <f t="shared" ref="AG24" si="62">IF(OR(ISBLANK(S24), ISBLANK(Z24)),"",S24+Z24)</f>
         <v>3.937301664</v>
       </c>
       <c r="AH24" s="69">
-        <f t="shared" ref="AH24" si="44">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
+        <f t="shared" ref="AH24" si="63">IF(OR(ISBLANK(T24), ISBLANK(AA24)),"",T24+AA24)</f>
         <v>3.9790181429999998</v>
       </c>
       <c r="AI24" s="69">
-        <f t="shared" ref="AI24" si="45">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
+        <f t="shared" ref="AI24" si="64">IF(OR(ISBLANK(U24), ISBLANK(AB24)),"",U24+AB24)</f>
         <v>3.8259789839999998</v>
       </c>
       <c r="AJ24" s="69" t="str">
-        <f t="shared" ref="AJ24" si="46">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
+        <f t="shared" ref="AJ24" si="65">IF(OR(ISBLANK(V24), ISBLANK(AC24)),"",V24+AC24)</f>
         <v/>
       </c>
       <c r="AK24" s="69" t="str">
-        <f t="shared" ref="AK24" si="47">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
+        <f t="shared" ref="AK24" si="66">IF(OR(ISBLANK(W24), ISBLANK(AD24)),"",W24+AD24)</f>
         <v/>
       </c>
       <c r="AS24" s="61">
@@ -6548,9 +6650,7 @@
       <c r="D25" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E25" s="61"/>
       <c r="F25" s="61" t="s">
         <v>142</v>
       </c>
@@ -6616,31 +6716,31 @@
         <v>0</v>
       </c>
       <c r="AE25" s="69">
-        <f t="shared" ref="AE25:AE27" si="48">IF(OR(ISBLANK(Q25), ISBLANK(X25)),"",Q25+X25)</f>
+        <f t="shared" ref="AE25:AE27" si="67">IF(OR(ISBLANK(Q25), ISBLANK(X25)),"",Q25+X25)</f>
         <v>1.8746218750000001</v>
       </c>
       <c r="AF25" s="69">
-        <f t="shared" ref="AF25:AF27" si="49">IF(OR(ISBLANK(R25), ISBLANK(Y25)),"",R25+Y25)</f>
+        <f t="shared" ref="AF25:AF27" si="68">IF(OR(ISBLANK(R25), ISBLANK(Y25)),"",R25+Y25)</f>
         <v>1.844359927</v>
       </c>
       <c r="AG25" s="69">
-        <f t="shared" ref="AG25:AG27" si="50">IF(OR(ISBLANK(S25), ISBLANK(Z25)),"",S25+Z25)</f>
+        <f t="shared" ref="AG25:AG27" si="69">IF(OR(ISBLANK(S25), ISBLANK(Z25)),"",S25+Z25)</f>
         <v>2.051568649</v>
       </c>
       <c r="AH25" s="69">
-        <f t="shared" ref="AH25:AH27" si="51">IF(OR(ISBLANK(T25), ISBLANK(AA25)),"",T25+AA25)</f>
+        <f t="shared" ref="AH25:AH27" si="70">IF(OR(ISBLANK(T25), ISBLANK(AA25)),"",T25+AA25)</f>
         <v>1.710493431</v>
       </c>
       <c r="AI25" s="69">
-        <f t="shared" ref="AI25:AI27" si="52">IF(OR(ISBLANK(U25), ISBLANK(AB25)),"",U25+AB25)</f>
+        <f t="shared" ref="AI25:AI27" si="71">IF(OR(ISBLANK(U25), ISBLANK(AB25)),"",U25+AB25)</f>
         <v>1.6449851719404254</v>
       </c>
       <c r="AJ25" s="69" t="str">
-        <f t="shared" ref="AJ25:AJ27" si="53">IF(OR(ISBLANK(V25), ISBLANK(AC25)),"",V25+AC25)</f>
+        <f t="shared" ref="AJ25:AJ27" si="72">IF(OR(ISBLANK(V25), ISBLANK(AC25)),"",V25+AC25)</f>
         <v/>
       </c>
       <c r="AK25" s="69" t="str">
-        <f t="shared" ref="AK25:AK27" si="54">IF(OR(ISBLANK(W25), ISBLANK(AD25)),"",W25+AD25)</f>
+        <f t="shared" ref="AK25:AK27" si="73">IF(OR(ISBLANK(W25), ISBLANK(AD25)),"",W25+AD25)</f>
         <v/>
       </c>
       <c r="AS25" s="61">
@@ -6672,9 +6772,7 @@
       <c r="D26" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E26" s="61"/>
       <c r="F26" s="61" t="s">
         <v>182</v>
       </c>
@@ -6739,31 +6837,31 @@
         <v>0</v>
       </c>
       <c r="AE26" s="69">
-        <f t="shared" si="48"/>
+        <f t="shared" si="67"/>
         <v>12.356382978723399</v>
       </c>
       <c r="AF26" s="69">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>11.819148936170221</v>
       </c>
       <c r="AG26" s="69">
-        <f t="shared" si="50"/>
+        <f t="shared" si="69"/>
         <v>11.281914893617021</v>
       </c>
       <c r="AH26" s="69">
-        <f t="shared" si="51"/>
+        <f t="shared" si="70"/>
         <v>10.1</v>
       </c>
       <c r="AI26" s="69">
-        <f t="shared" si="52"/>
+        <f t="shared" si="71"/>
         <v>10.1</v>
       </c>
       <c r="AJ26" s="69" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="72"/>
         <v/>
       </c>
       <c r="AK26" s="69" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="AS26" s="61">
@@ -6795,9 +6893,7 @@
       <c r="D27" s="61" t="s">
         <v>240</v>
       </c>
-      <c r="E27" s="61" t="s">
-        <v>241</v>
-      </c>
+      <c r="E27" s="61"/>
       <c r="F27" s="61" t="s">
         <v>142</v>
       </c>
@@ -6862,31 +6958,31 @@
         <v>0</v>
       </c>
       <c r="AE27" s="69">
-        <f t="shared" si="48"/>
+        <f t="shared" si="67"/>
         <v>3.004725724</v>
       </c>
       <c r="AF27" s="69">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>2.1325357700000001</v>
       </c>
       <c r="AG27" s="69">
-        <f t="shared" si="50"/>
+        <f t="shared" si="69"/>
         <v>3.0720788620000001</v>
       </c>
       <c r="AH27" s="69">
-        <f t="shared" si="51"/>
+        <f t="shared" si="70"/>
         <v>2.4277569909999999</v>
       </c>
       <c r="AI27" s="69">
-        <f t="shared" si="52"/>
+        <f t="shared" si="71"/>
         <v>1.335266345</v>
       </c>
       <c r="AJ27" s="69" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="72"/>
         <v/>
       </c>
       <c r="AK27" s="69" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="73"/>
         <v/>
       </c>
       <c r="AS27" s="61">
@@ -6918,9 +7014,7 @@
       <c r="D28" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E28" s="61"/>
       <c r="F28" s="61" t="s">
         <v>142</v>
       </c>
@@ -6985,31 +7079,31 @@
         <v>0</v>
       </c>
       <c r="AE28" s="69">
-        <f t="shared" ref="AE28" si="55">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
+        <f t="shared" ref="AE28" si="74">IF(OR(ISBLANK(Q28), ISBLANK(X28)),"",Q28+X28)</f>
         <v>0.99625009600000003</v>
       </c>
       <c r="AF28" s="69">
-        <f t="shared" ref="AF28" si="56">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
+        <f t="shared" ref="AF28" si="75">IF(OR(ISBLANK(R28), ISBLANK(Y28)),"",R28+Y28)</f>
         <v>0.98354598199999999</v>
       </c>
       <c r="AG28" s="69">
-        <f t="shared" ref="AG28" si="57">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
+        <f t="shared" ref="AG28" si="76">IF(OR(ISBLANK(S28), ISBLANK(Z28)),"",S28+Z28)</f>
         <v>2.6019487300000002</v>
       </c>
       <c r="AH28" s="69">
-        <f t="shared" ref="AH28" si="58">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
+        <f t="shared" ref="AH28" si="77">IF(OR(ISBLANK(T28), ISBLANK(AA28)),"",T28+AA28)</f>
         <v>2.5352979329999998</v>
       </c>
       <c r="AI28" s="69">
-        <f t="shared" ref="AI28" si="59">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
+        <f t="shared" ref="AI28" si="78">IF(OR(ISBLANK(U28), ISBLANK(AB28)),"",U28+AB28)</f>
         <v>1.926808946</v>
       </c>
       <c r="AJ28" s="69" t="str">
-        <f t="shared" ref="AJ28" si="60">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
+        <f t="shared" ref="AJ28" si="79">IF(OR(ISBLANK(V28), ISBLANK(AC28)),"",V28+AC28)</f>
         <v/>
       </c>
       <c r="AK28" s="69" t="str">
-        <f t="shared" ref="AK28" si="61">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
+        <f t="shared" ref="AK28" si="80">IF(OR(ISBLANK(W28), ISBLANK(AD28)),"",W28+AD28)</f>
         <v/>
       </c>
       <c r="AS28" s="61">
@@ -7041,9 +7135,7 @@
       <c r="D29" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E29" s="61"/>
       <c r="F29" s="61" t="s">
         <v>142</v>
       </c>
@@ -7108,31 +7200,31 @@
         <v>6063090</v>
       </c>
       <c r="AE29" s="69">
-        <f t="shared" ref="AE29:AE30" si="62">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
+        <f t="shared" ref="AE29:AE31" si="81">IF(OR(ISBLANK(Q29), ISBLANK(X29)),"",Q29+X29)</f>
         <v>33167324</v>
       </c>
       <c r="AF29" s="69">
-        <f t="shared" ref="AF29:AF30" si="63">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
+        <f t="shared" ref="AF29:AF30" si="82">IF(OR(ISBLANK(R29), ISBLANK(Y29)),"",R29+Y29)</f>
         <v>36362250</v>
       </c>
       <c r="AG29" s="69">
-        <f t="shared" ref="AG29:AG30" si="64">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
+        <f t="shared" ref="AG29:AG30" si="83">IF(OR(ISBLANK(S29), ISBLANK(Z29)),"",S29+Z29)</f>
         <v>35896971</v>
       </c>
       <c r="AH29" s="69">
-        <f t="shared" ref="AH29:AH30" si="65">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
+        <f t="shared" ref="AH29:AH30" si="84">IF(OR(ISBLANK(T29), ISBLANK(AA29)),"",T29+AA29)</f>
         <v>30327168</v>
       </c>
       <c r="AI29" s="69">
-        <f t="shared" ref="AI29:AI30" si="66">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
+        <f t="shared" ref="AI29:AI30" si="85">IF(OR(ISBLANK(U29), ISBLANK(AB29)),"",U29+AB29)</f>
         <v>31822330</v>
       </c>
       <c r="AJ29" s="69" t="str">
-        <f t="shared" ref="AJ29:AJ30" si="67">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
+        <f t="shared" ref="AJ29:AJ30" si="86">IF(OR(ISBLANK(V29), ISBLANK(AC29)),"",V29+AC29)</f>
         <v/>
       </c>
       <c r="AK29" s="69" t="str">
-        <f t="shared" ref="AK29:AK30" si="68">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
+        <f t="shared" ref="AK29:AK30" si="87">IF(OR(ISBLANK(W29), ISBLANK(AD29)),"",W29+AD29)</f>
         <v/>
       </c>
       <c r="AS29" s="1">
@@ -7169,9 +7261,7 @@
       <c r="D30" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E30" s="61"/>
       <c r="F30" s="61" t="s">
         <v>142</v>
       </c>
@@ -7236,31 +7326,31 @@
         <v>0</v>
       </c>
       <c r="AE30" s="69">
-        <f t="shared" si="62"/>
+        <f t="shared" si="81"/>
         <v>2.2165439930000002</v>
       </c>
       <c r="AF30" s="69">
-        <f t="shared" si="63"/>
+        <f t="shared" si="82"/>
         <v>2.2511915660000001</v>
       </c>
       <c r="AG30" s="69">
-        <f t="shared" si="64"/>
+        <f t="shared" si="83"/>
         <v>2.4511497719999999</v>
       </c>
       <c r="AH30" s="69">
-        <f t="shared" si="65"/>
+        <f t="shared" si="84"/>
         <v>2.4417731950000001</v>
       </c>
       <c r="AI30" s="69">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>2.3478588409999999</v>
       </c>
       <c r="AJ30" s="69" t="str">
-        <f t="shared" si="67"/>
+        <f t="shared" si="86"/>
         <v/>
       </c>
       <c r="AK30" s="69" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" si="87"/>
         <v/>
       </c>
       <c r="AS30" s="61">
@@ -7292,9 +7382,7 @@
       <c r="D31" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E31" s="61"/>
       <c r="F31" s="61" t="s">
         <v>142</v>
       </c>
@@ -7342,6 +7430,49 @@
       </c>
       <c r="U31" s="2">
         <v>5.0787910969999999</v>
+      </c>
+      <c r="X31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="69">
+        <f t="shared" si="81"/>
+        <v>6.3372507860000002</v>
+      </c>
+      <c r="AF31" s="69">
+        <f t="shared" ref="AF31" si="88">IF(ISBLANK(R31),IF(ISBLANK(Y31),"",Y31),R31+Y31)</f>
+        <v>6.1180013459999998</v>
+      </c>
+      <c r="AG31" s="69">
+        <f t="shared" ref="AG31" si="89">IF(ISBLANK(S31),IF(ISBLANK(Z31),"",Z31),S31+Z31)</f>
+        <v>5.2178957580000001</v>
+      </c>
+      <c r="AH31" s="69">
+        <f t="shared" ref="AH31" si="90">IF(ISBLANK(T31),IF(ISBLANK(AA31),"",AA31),T31+AA31)</f>
+        <v>5.3678279890000002</v>
+      </c>
+      <c r="AI31" s="69">
+        <f t="shared" ref="AI31" si="91">IF(ISBLANK(U31),IF(ISBLANK(AB31),"",AB31),U31+AB31)</f>
+        <v>5.0787910969999999</v>
+      </c>
+      <c r="AJ31" s="69" t="str">
+        <f t="shared" ref="AJ31" si="92">IF(ISBLANK(V31),IF(ISBLANK(AC31),"",AC31),V31+AC31)</f>
+        <v/>
+      </c>
+      <c r="AK31" s="69" t="str">
+        <f t="shared" ref="AK31" si="93">IF(ISBLANK(W31),IF(ISBLANK(AD31),"",AD31),W31+AD31)</f>
+        <v/>
       </c>
       <c r="AS31" s="61">
         <v>11.83516337</v>
@@ -7372,9 +7503,7 @@
       <c r="D32" s="61" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="61" t="s">
-        <v>323</v>
-      </c>
+      <c r="E32" s="61"/>
       <c r="F32" s="61" t="s">
         <v>182</v>
       </c>
@@ -7437,31 +7566,31 @@
         <v>0</v>
       </c>
       <c r="AE32" s="69" t="str">
-        <f t="shared" ref="AE32" si="69">IF(OR(ISBLANK(Q32), ISBLANK(X32)),"",Q32+X32)</f>
+        <f t="shared" ref="AE32" si="94">IF(OR(ISBLANK(Q32), ISBLANK(X32)),"",Q32+X32)</f>
         <v/>
       </c>
       <c r="AF32" s="69">
-        <f t="shared" ref="AF32" si="70">IF(OR(ISBLANK(R32), ISBLANK(Y32)),"",R32+Y32)</f>
+        <f t="shared" ref="AF32" si="95">IF(OR(ISBLANK(R32), ISBLANK(Y32)),"",R32+Y32)</f>
         <v>78.8</v>
       </c>
       <c r="AG32" s="69">
-        <f t="shared" ref="AG32" si="71">IF(OR(ISBLANK(S32), ISBLANK(Z32)),"",S32+Z32)</f>
+        <f t="shared" ref="AG32" si="96">IF(OR(ISBLANK(S32), ISBLANK(Z32)),"",S32+Z32)</f>
         <v>78.8</v>
       </c>
       <c r="AH32" s="69">
-        <f t="shared" ref="AH32" si="72">IF(OR(ISBLANK(T32), ISBLANK(AA32)),"",T32+AA32)</f>
+        <f t="shared" ref="AH32" si="97">IF(OR(ISBLANK(T32), ISBLANK(AA32)),"",T32+AA32)</f>
         <v>78.8</v>
       </c>
       <c r="AI32" s="69">
-        <f t="shared" ref="AI32" si="73">IF(OR(ISBLANK(U32), ISBLANK(AB32)),"",U32+AB32)</f>
+        <f t="shared" ref="AI32" si="98">IF(OR(ISBLANK(U32), ISBLANK(AB32)),"",U32+AB32)</f>
         <v>68.873999999999995</v>
       </c>
       <c r="AJ32" s="69" t="str">
-        <f t="shared" ref="AJ32" si="74">IF(OR(ISBLANK(V32), ISBLANK(AC32)),"",V32+AC32)</f>
+        <f t="shared" ref="AJ32" si="99">IF(OR(ISBLANK(V32), ISBLANK(AC32)),"",V32+AC32)</f>
         <v/>
       </c>
       <c r="AK32" s="69" t="str">
-        <f t="shared" ref="AK32" si="75">IF(OR(ISBLANK(W32), ISBLANK(AD32)),"",W32+AD32)</f>
+        <f t="shared" ref="AK32" si="100">IF(OR(ISBLANK(W32), ISBLANK(AD32)),"",W32+AD32)</f>
         <v/>
       </c>
       <c r="AS32" s="61"/>
@@ -7491,9 +7620,7 @@
       <c r="D33" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="61" t="s">
-        <v>62</v>
-      </c>
+      <c r="E33" s="61"/>
       <c r="F33" s="61" t="s">
         <v>142</v>
       </c>
@@ -7994,29 +8121,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="61" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="61"/>
-    <col min="4" max="4" width="16.42578125" style="26"/>
-    <col min="5" max="5" width="17.42578125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" style="61" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="61"/>
+    <col min="4" max="4" width="16.5" style="26"/>
+    <col min="5" max="5" width="17.5" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="61" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" style="61" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="20" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" style="61" customWidth="1"/>
     <col min="10" max="10" width="24" style="61" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="61" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" style="61" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="61" customWidth="1"/>
+    <col min="12" max="12" width="21.5" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -8030,7 +8157,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>123</v>
@@ -9610,22 +9737,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F5420B-4269-4C0B-A558-3652DBE2EE0B}">
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.7109375" style="51" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.6640625" style="51" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="8" max="8" width="87.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="87.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="17" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>12</v>
       </c>
@@ -9645,7 +9772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="16">
       <c r="A2" s="40" t="s">
         <v>13</v>
       </c>
@@ -9665,7 +9792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="16">
       <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
@@ -9685,7 +9812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45">
+    <row r="4" spans="1:6" ht="32">
       <c r="A4" s="40" t="s">
         <v>13</v>
       </c>
@@ -9705,7 +9832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
+    <row r="5" spans="1:6" ht="32">
       <c r="A5" s="40" t="s">
         <v>13</v>
       </c>
@@ -9725,7 +9852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60">
+    <row r="6" spans="1:6" ht="48">
       <c r="A6" s="40" t="s">
         <v>13</v>
       </c>
@@ -9745,7 +9872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="40" t="s">
         <v>13</v>
       </c>
@@ -9765,7 +9892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="40" t="s">
         <v>13</v>
       </c>
@@ -9785,7 +9912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45">
+    <row r="9" spans="1:6" ht="32">
       <c r="A9" s="40" t="s">
         <v>13</v>
       </c>
@@ -9805,7 +9932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="40" t="s">
         <v>13</v>
       </c>
@@ -9825,7 +9952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="40" t="s">
         <v>13</v>
       </c>
@@ -9845,7 +9972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="40" t="s">
         <v>13</v>
       </c>
@@ -9865,7 +9992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="40" t="s">
         <v>13</v>
       </c>
@@ -9885,7 +10012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30">
+    <row r="14" spans="1:6" ht="32">
       <c r="A14" s="40" t="s">
         <v>13</v>
       </c>
@@ -9905,7 +10032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="40" t="s">
         <v>13</v>
       </c>
@@ -9965,7 +10092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30">
+    <row r="18" spans="1:6" ht="32">
       <c r="A18" s="31" t="s">
         <v>15</v>
       </c>
@@ -9985,7 +10112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="32">
       <c r="A19" s="31" t="s">
         <v>15</v>
       </c>
@@ -10005,7 +10132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30">
+    <row r="20" spans="1:6" ht="32">
       <c r="A20" s="31" t="s">
         <v>15</v>
       </c>
@@ -10025,7 +10152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30">
+    <row r="21" spans="1:6" ht="32">
       <c r="A21" s="31" t="s">
         <v>15</v>
       </c>
@@ -10045,7 +10172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="32">
       <c r="A22" s="31" t="s">
         <v>15</v>
       </c>
@@ -10065,7 +10192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="32">
       <c r="A23" s="31" t="s">
         <v>15</v>
       </c>
@@ -10085,7 +10212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45">
+    <row r="24" spans="1:6" ht="48">
       <c r="A24" s="31" t="s">
         <v>15</v>
       </c>
@@ -10105,7 +10232,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30">
+    <row r="25" spans="1:6" ht="32">
       <c r="A25" s="31" t="s">
         <v>15</v>
       </c>
@@ -10125,7 +10252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:6" ht="32">
       <c r="A26" s="31" t="s">
         <v>15</v>
       </c>
@@ -10145,7 +10272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30">
+    <row r="27" spans="1:6" ht="32">
       <c r="A27" s="31" t="s">
         <v>15</v>
       </c>
@@ -10165,7 +10292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30">
+    <row r="28" spans="1:6" ht="32">
       <c r="A28" s="31" t="s">
         <v>15</v>
       </c>
@@ -10185,7 +10312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30">
+    <row r="29" spans="1:6" ht="32">
       <c r="A29" s="31" t="s">
         <v>15</v>
       </c>
@@ -10205,7 +10332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30">
+    <row r="30" spans="1:6" ht="32">
       <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
@@ -10225,7 +10352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="45">
+    <row r="31" spans="1:6" ht="48">
       <c r="A31" s="31" t="s">
         <v>15</v>
       </c>
@@ -10245,7 +10372,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="32">
       <c r="A32" s="31" t="s">
         <v>15</v>
       </c>
@@ -10265,7 +10392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30">
+    <row r="33" spans="1:6" ht="32">
       <c r="A33" s="31" t="s">
         <v>15</v>
       </c>
@@ -10285,7 +10412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" ht="32">
       <c r="A34" s="31" t="s">
         <v>15</v>
       </c>
@@ -10305,7 +10432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="32">
       <c r="A35" s="31" t="s">
         <v>15</v>
       </c>
@@ -10325,7 +10452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30">
+    <row r="36" spans="1:6" ht="32">
       <c r="A36" s="31" t="s">
         <v>15</v>
       </c>
@@ -10345,7 +10472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30">
+    <row r="37" spans="1:6" ht="32">
       <c r="A37" s="31" t="s">
         <v>15</v>
       </c>
@@ -10365,7 +10492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="45">
+    <row r="38" spans="1:6" ht="48">
       <c r="A38" s="31" t="s">
         <v>15</v>
       </c>
@@ -10385,7 +10512,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30">
+    <row r="39" spans="1:6" ht="32">
       <c r="A39" s="31" t="s">
         <v>15</v>
       </c>
@@ -10405,7 +10532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30">
+    <row r="40" spans="1:6" ht="32">
       <c r="A40" s="31" t="s">
         <v>15</v>
       </c>
@@ -10425,7 +10552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30">
+    <row r="41" spans="1:6" ht="32">
       <c r="A41" s="31" t="s">
         <v>15</v>
       </c>
@@ -10445,7 +10572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30">
+    <row r="42" spans="1:6" ht="32">
       <c r="A42" s="31" t="s">
         <v>15</v>
       </c>
@@ -10465,7 +10592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30">
+    <row r="43" spans="1:6" ht="32">
       <c r="A43" s="31" t="s">
         <v>15</v>
       </c>
@@ -10485,7 +10612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30">
+    <row r="44" spans="1:6" ht="32">
       <c r="A44" s="31" t="s">
         <v>15</v>
       </c>
@@ -10505,7 +10632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="45">
+    <row r="45" spans="1:6" ht="48">
       <c r="A45" s="31" t="s">
         <v>15</v>
       </c>
@@ -10525,7 +10652,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30">
+    <row r="46" spans="1:6" ht="32">
       <c r="A46" s="50" t="s">
         <v>75</v>
       </c>
@@ -10545,7 +10672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="30">
+    <row r="47" spans="1:6" ht="32">
       <c r="A47" s="50" t="s">
         <v>75</v>
       </c>
@@ -10565,7 +10692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30">
+    <row r="48" spans="1:6" ht="32">
       <c r="A48" s="50" t="s">
         <v>75</v>
       </c>
@@ -10585,7 +10712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="30">
+    <row r="49" spans="1:6" ht="32">
       <c r="A49" s="50" t="s">
         <v>75</v>
       </c>
@@ -10605,7 +10732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="30">
+    <row r="50" spans="1:6" ht="32">
       <c r="A50" s="50" t="s">
         <v>75</v>
       </c>
@@ -10625,7 +10752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="30">
+    <row r="51" spans="1:6" ht="32">
       <c r="A51" s="44" t="s">
         <v>14</v>
       </c>
@@ -10645,7 +10772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="60">
+    <row r="52" spans="1:6" ht="48">
       <c r="A52" s="44" t="s">
         <v>14</v>
       </c>
@@ -10665,7 +10792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="16">
       <c r="A53" s="44" t="s">
         <v>14</v>
       </c>
@@ -10685,7 +10812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" ht="16">
       <c r="A54" s="44" t="s">
         <v>14</v>
       </c>
@@ -10705,7 +10832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="75">
+    <row r="55" spans="1:6" ht="80">
       <c r="A55" s="44" t="s">
         <v>14</v>
       </c>
@@ -10725,7 +10852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="75">
+    <row r="56" spans="1:6" ht="64">
       <c r="A56" s="44" t="s">
         <v>14</v>
       </c>
@@ -10745,7 +10872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" ht="16">
       <c r="A57" s="44" t="s">
         <v>14</v>
       </c>
@@ -10765,7 +10892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="30">
+    <row r="58" spans="1:6" ht="32">
       <c r="A58" s="44" t="s">
         <v>14</v>
       </c>
@@ -10785,7 +10912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="45">
+    <row r="59" spans="1:6" ht="48">
       <c r="A59" s="45" t="s">
         <v>103</v>
       </c>
@@ -10816,19 +10943,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="61" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10863,7 +10990,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>54173</v>
+        <v>99859</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10880,8 +11007,8 @@
         <v>147</v>
       </c>
       <c r="E3" s="61">
-        <f t="shared" ref="E3:E33" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>98590</v>
+        <f t="shared" ref="E3:E41" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
+        <v>57333</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10899,7 +11026,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>159377</v>
+        <v>155750</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10917,7 +11044,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>210445</v>
+        <v>90003</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10935,7 +11062,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>38219</v>
+        <v>100298</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10953,7 +11080,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>123326</v>
+        <v>123657</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10971,7 +11098,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>93004</v>
+        <v>107777</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10989,7 +11116,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>116763</v>
+        <v>248140</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11007,7 +11134,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>128506</v>
+        <v>128904</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11025,7 +11152,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>77402</v>
+        <v>109980</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -11043,7 +11170,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>188530</v>
+        <v>228354</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -11061,7 +11188,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>36186</v>
+        <v>173230</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -11079,7 +11206,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>165727</v>
+        <v>113389</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -11097,7 +11224,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>101690</v>
+        <v>166732</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11115,7 +11242,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>120592</v>
+        <v>52190</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -11133,7 +11260,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>127438</v>
+        <v>127892</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11151,7 +11278,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>196333</v>
+        <v>153275</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11169,7 +11296,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>152722</v>
+        <v>105108</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11187,7 +11314,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>125969</v>
+        <v>35548</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11205,7 +11332,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>180101</v>
+        <v>233771</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11223,7 +11350,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>156801</v>
+        <v>205264</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -11241,7 +11368,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>175770</v>
+        <v>128382</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -11259,7 +11386,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>119305</v>
+        <v>127210</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -11277,7 +11404,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>89926</v>
+        <v>156652</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -11295,7 +11422,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>126370</v>
+        <v>108457</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -11313,7 +11440,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>197235</v>
+        <v>51182</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -11331,7 +11458,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>122102</v>
+        <v>204985</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -11349,7 +11476,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>177763</v>
+        <v>148784</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -11367,7 +11494,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>174816</v>
+        <v>199797</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -11385,7 +11512,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>81388</v>
+        <v>208716</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -11403,7 +11530,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>211885</v>
+        <v>176661</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -11421,7 +11548,7 @@
       </c>
       <c r="E33" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>243388</v>
+        <v>121516</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -11486,49 +11613,49 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364511B7-3F85-F540-BA5C-9DA3347FB2A8}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AZ54"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="61"/>
-    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="61"/>
+    <col min="1" max="1" width="16.5" style="61"/>
+    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="61"/>
     <col min="4" max="4" width="8" style="61" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="24"/>
-    <col min="6" max="6" width="16.42578125" style="61"/>
+    <col min="5" max="5" width="16.5" style="24"/>
+    <col min="6" max="6" width="16.5" style="61"/>
     <col min="7" max="7" width="10" style="4" customWidth="1"/>
     <col min="8" max="8" width="9" style="61" customWidth="1"/>
     <col min="9" max="9" width="11" style="5" customWidth="1"/>
-    <col min="10" max="13" width="16.42578125" style="61"/>
+    <col min="10" max="13" width="16.5" style="61"/>
     <col min="14" max="14" width="17" style="61" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" style="61" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="61" customWidth="1"/>
+    <col min="15" max="15" width="15.5" style="61" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" style="61" customWidth="1"/>
     <col min="17" max="19" width="0" style="61" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="16.42578125" style="61"/>
+    <col min="20" max="21" width="16.5" style="61"/>
     <col min="22" max="22" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="0" style="36" hidden="1" customWidth="1"/>
     <col min="24" max="29" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="0" style="36" hidden="1" customWidth="1"/>
     <col min="31" max="33" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="34" max="36" width="16.42578125" style="2"/>
+    <col min="34" max="36" width="16.5" style="2"/>
     <col min="37" max="44" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="45" max="47" width="16.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="48" max="49" width="16.85546875" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.42578125" style="2"/>
+    <col min="45" max="47" width="16.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="48" max="49" width="16.83203125" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="30">
+    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -16113,27 +16240,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B625E0-7A95-AB40-9EC5-2C6C2025FC51}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="61" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="61"/>
-    <col min="4" max="4" width="8.85546875" style="26"/>
-    <col min="5" max="5" width="17.42578125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" style="61" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="61"/>
+    <col min="4" max="4" width="8.83203125" style="26"/>
+    <col min="5" max="5" width="17.5" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="61" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" style="61" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="20" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" style="61" customWidth="1"/>
     <col min="10" max="10" width="24" style="61" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="61" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" style="61" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="61"/>
+    <col min="11" max="11" width="19.33203125" style="61" customWidth="1"/>
+    <col min="12" max="12" width="21.5" style="61" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="61"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -16674,12 +16801,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -16896,6 +17017,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
   <ds:schemaRefs>
@@ -16905,23 +17032,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16938,4 +17048,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set warning to error and fix failing test - target year in template test data > 2022
Signed-off-by: David Kroon <35101727+dp90@users.noreply.github.com>
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ITR\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3F899F-8718-48EB-A7CA-6B2C002E3766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CE6FE6-0FE7-4356-8CFA-87584D6179F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -3912,7 +3912,7 @@
   </sheetPr>
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="AS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8891,11 +8891,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -9839,7 +9839,7 @@
         <v>319</v>
       </c>
       <c r="K26" s="61">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="L26" s="75">
         <v>0.15</v>
@@ -12183,7 +12183,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>75147</v>
+        <v>197443</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="E3" s="61">
         <f t="shared" ref="E3:E44" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>113777</v>
+        <v>135419</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -12219,7 +12219,7 @@
       </c>
       <c r="E4" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>151524</v>
+        <v>190524</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -12237,7 +12237,7 @@
       </c>
       <c r="E5" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>50348</v>
+        <v>69089</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -12255,7 +12255,7 @@
       </c>
       <c r="E6" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>141603</v>
+        <v>168497</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -12273,7 +12273,7 @@
       </c>
       <c r="E7" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>101890</v>
+        <v>183442</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -12291,7 +12291,7 @@
       </c>
       <c r="E8" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>176248</v>
+        <v>217978</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -12309,7 +12309,7 @@
       </c>
       <c r="E9" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>212108</v>
+        <v>96395</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -12327,7 +12327,7 @@
       </c>
       <c r="E10" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>59504</v>
+        <v>40122</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -12345,7 +12345,7 @@
       </c>
       <c r="E11" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>163701</v>
+        <v>190155</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -12363,7 +12363,7 @@
       </c>
       <c r="E12" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>117268</v>
+        <v>243328</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -12381,7 +12381,7 @@
       </c>
       <c r="E13" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>124600</v>
+        <v>92902</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -12399,7 +12399,7 @@
       </c>
       <c r="E14" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>109132</v>
+        <v>206259</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -12417,7 +12417,7 @@
       </c>
       <c r="E15" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>109787</v>
+        <v>48177</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -12435,7 +12435,7 @@
       </c>
       <c r="E16" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>208759</v>
+        <v>48940</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -12453,7 +12453,7 @@
       </c>
       <c r="E17" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>152288</v>
+        <v>152227</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -12471,7 +12471,7 @@
       </c>
       <c r="E18" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>191643</v>
+        <v>127333</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -12489,7 +12489,7 @@
       </c>
       <c r="E19" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>239209</v>
+        <v>191008</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -12507,7 +12507,7 @@
       </c>
       <c r="E20" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>111937</v>
+        <v>79518</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -12525,7 +12525,7 @@
       </c>
       <c r="E21" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>230786</v>
+        <v>64229</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -12543,7 +12543,7 @@
       </c>
       <c r="E22" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>215941</v>
+        <v>52110</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -12561,7 +12561,7 @@
       </c>
       <c r="E23" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>143300</v>
+        <v>180936</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -12579,7 +12579,7 @@
       </c>
       <c r="E24" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>63685</v>
+        <v>224286</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -12597,7 +12597,7 @@
       </c>
       <c r="E25" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>86096</v>
+        <v>222779</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -12615,7 +12615,7 @@
       </c>
       <c r="E26" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>212955</v>
+        <v>61566</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -12633,7 +12633,7 @@
       </c>
       <c r="E27" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>206411</v>
+        <v>164816</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -12651,7 +12651,7 @@
       </c>
       <c r="E28" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>57887</v>
+        <v>203846</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -12669,7 +12669,7 @@
       </c>
       <c r="E29" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>35972</v>
+        <v>231416</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -12687,7 +12687,7 @@
       </c>
       <c r="E30" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>117570</v>
+        <v>236214</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -12705,7 +12705,7 @@
       </c>
       <c r="E31" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>89312</v>
+        <v>128776</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -12723,7 +12723,7 @@
       </c>
       <c r="E32" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>153872</v>
+        <v>206639</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -12741,7 +12741,7 @@
       </c>
       <c r="E33" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>126631</v>
+        <v>89800</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -12759,7 +12759,7 @@
       </c>
       <c r="E34" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>236355</v>
+        <v>212068</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -12777,7 +12777,7 @@
       </c>
       <c r="E35" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>93507</v>
+        <v>229757</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -12795,7 +12795,7 @@
       </c>
       <c r="E36" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>68182</v>
+        <v>249147</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -12813,7 +12813,7 @@
       </c>
       <c r="E37" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>140564</v>
+        <v>175467</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -12831,7 +12831,7 @@
       </c>
       <c r="E38" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>221642</v>
+        <v>196711</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -12849,7 +12849,7 @@
       </c>
       <c r="E39" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>152407</v>
+        <v>71302</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -12867,7 +12867,7 @@
       </c>
       <c r="E40" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>105912</v>
+        <v>98446</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -12885,7 +12885,7 @@
       </c>
       <c r="E41" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>230178</v>
+        <v>116572</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -12903,7 +12903,7 @@
       </c>
       <c r="E42" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>75278</v>
+        <v>158196</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -12921,7 +12921,7 @@
       </c>
       <c r="E43" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>152703</v>
+        <v>109327</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -12939,7 +12939,7 @@
       </c>
       <c r="E44" s="61">
         <f t="shared" ca="1" si="0"/>
-        <v>242146</v>
+        <v>129499</v>
       </c>
     </row>
   </sheetData>
@@ -18127,9 +18127,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18350,27 +18353,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18395,9 +18386,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update comments and spreadsheets
General source consistency update.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test/inputs/20220215 ITR Tool Sample Data.xlsx
+++ b/test/inputs/20220215 ITR Tool Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Dropbox/My Mac (MacBook-Pro.local)/Documents/GitHub/MichaelTiemannOSC/ITR/test/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C43370-4987-5B48-82A3-DC48CC060B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975E99C9-6F57-CC41-BE90-CC4D2875F80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33820" windowHeight="12580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33820" windowHeight="12580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -3132,7 +3132,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3420,7 +3420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3863,11 +3863,11 @@
   </sheetPr>
   <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V2" sqref="V2"/>
+      <selection pane="bottomRight" activeCell="AT3" sqref="AT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -4339,11 +4339,11 @@
         <v>12628488</v>
       </c>
       <c r="AJ4" s="54" t="str">
-        <f t="shared" ref="AJ2:AJ4" si="4">IF(ISBLANK(V4),IF(ISBLANK(AC4),"",AC4),V4+AC4)</f>
+        <f t="shared" ref="AJ4" si="4">IF(ISBLANK(V4),IF(ISBLANK(AC4),"",AC4),V4+AC4)</f>
         <v/>
       </c>
       <c r="AK4" s="54" t="str">
-        <f t="shared" ref="AK2:AK4" si="5">IF(ISBLANK(W4),IF(ISBLANK(AD4),"",AD4),W4+AD4)</f>
+        <f t="shared" ref="AK4" si="5">IF(ISBLANK(W4),IF(ISBLANK(AD4),"",AD4),W4+AD4)</f>
         <v/>
       </c>
       <c r="AS4" s="61">
@@ -8553,11 +8553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AEF12C-8FCA-4C98-A7E3-A92507F3829D}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11843,7 +11843,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>144449</v>
+        <v>129467</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11861,7 +11861,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E44" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>149527</v>
+        <v>132919</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -11879,7 +11879,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>197376</v>
+        <v>219084</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -11897,7 +11897,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>164289</v>
+        <v>223566</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11915,7 +11915,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>62950</v>
+        <v>213533</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -11933,7 +11933,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>53183</v>
+        <v>218910</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -11951,7 +11951,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>39489</v>
+        <v>61753</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11969,7 +11969,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>58323</v>
+        <v>189276</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11987,7 +11987,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>99701</v>
+        <v>220403</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -12005,7 +12005,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>232092</v>
+        <v>96653</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -12023,7 +12023,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>248623</v>
+        <v>146800</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -12041,7 +12041,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>137717</v>
+        <v>240404</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -12059,7 +12059,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>180832</v>
+        <v>144957</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -12077,7 +12077,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>217286</v>
+        <v>178950</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -12095,7 +12095,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>185549</v>
+        <v>200921</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -12113,7 +12113,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>183871</v>
+        <v>152253</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -12131,7 +12131,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>232952</v>
+        <v>172788</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -12149,7 +12149,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>49766</v>
+        <v>147038</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -12167,7 +12167,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>131979</v>
+        <v>205914</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -12185,7 +12185,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>69334</v>
+        <v>128524</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -12203,7 +12203,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>119132</v>
+        <v>48379</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -12221,7 +12221,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>188797</v>
+        <v>142573</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -12239,7 +12239,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>137873</v>
+        <v>83484</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -12257,7 +12257,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>222382</v>
+        <v>172156</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -12275,7 +12275,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>104078</v>
+        <v>196603</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -12293,7 +12293,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>159774</v>
+        <v>95442</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -12311,7 +12311,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>133969</v>
+        <v>225084</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -12329,7 +12329,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>73356</v>
+        <v>224769</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -12347,7 +12347,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>226321</v>
+        <v>53877</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -12365,7 +12365,7 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>180827</v>
+        <v>179303</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -12383,7 +12383,7 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>91319</v>
+        <v>185926</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -12401,7 +12401,7 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>103160</v>
+        <v>134708</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -12419,7 +12419,7 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>175865</v>
+        <v>110019</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -12437,7 +12437,7 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>217546</v>
+        <v>169662</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -12455,7 +12455,7 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="0"/>
-        <v>249882</v>
+        <v>145590</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -12473,7 +12473,7 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="0"/>
-        <v>35643</v>
+        <v>36223</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -12491,7 +12491,7 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="0"/>
-        <v>94788</v>
+        <v>195150</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -12509,7 +12509,7 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="0"/>
-        <v>67847</v>
+        <v>56981</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -12527,7 +12527,7 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="0"/>
-        <v>94930</v>
+        <v>105345</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -12545,7 +12545,7 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="0"/>
-        <v>110222</v>
+        <v>73269</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -12563,7 +12563,7 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="0"/>
-        <v>118747</v>
+        <v>91032</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -12581,7 +12581,7 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="0"/>
-        <v>209709</v>
+        <v>169555</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -12599,7 +12599,7 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="0"/>
-        <v>83863</v>
+        <v>195150</v>
       </c>
     </row>
   </sheetData>
@@ -17521,12 +17521,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -17743,6 +17737,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
   <ds:schemaRefs>
@@ -17752,23 +17752,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17785,4 +17768,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>